<commit_message>
Move bytecode analysis to the Tvl.Java.DebugInterface.Types project Add BytecodeDisassembler as a reusable way to disassemble method bodies
git-svn-id: https://terabyte:8443/svn/LanguageServices/trunk@495 58fa913a-3432-0140-a220-d8bfcf8ade31
</commit_message>
<xml_diff>
--- a/Reference/JavaOpCodes.xlsx
+++ b/Reference/JavaOpCodes.xlsx
@@ -734,9 +734,6 @@
     <t>Var_I1</t>
   </si>
   <si>
-    <t>Method_I1_0</t>
-  </si>
-  <si>
     <t>Method</t>
   </si>
   <si>
@@ -749,9 +746,6 @@
     <t>TableSwitch</t>
   </si>
   <si>
-    <t>Switch</t>
-  </si>
-  <si>
     <t>ShortConst</t>
   </si>
   <si>
@@ -764,7 +758,13 @@
     <t>Code Name</t>
   </si>
   <si>
-    <t>Type_I1</t>
+    <t>Method_U1_0</t>
+  </si>
+  <si>
+    <t>Type_U1</t>
+  </si>
+  <si>
+    <t>LookupSwitch</t>
   </si>
 </sst>
 </file>
@@ -818,9 +818,6 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -845,6 +842,9 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -861,23 +861,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="OpCodes" displayName="OpCodes" ref="A1:L206" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="OpCodes" displayName="OpCodes" ref="A1:L206" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:L206"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Name"/>
-    <tableColumn id="12" name="Code Name" dataDxfId="0">
+    <tableColumn id="12" name="Code Name" dataDxfId="8">
       <calculatedColumnFormula>CONCATENATE(UPPER(LEFT(OpCodes[[#This Row],[Name]],1)),RIGHT(OpCodes[[#This Row],[Name]],LEN(OpCodes[[#This Row],[Name]])-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Value" dataDxfId="10"/>
+    <tableColumn id="2" name="Value" dataDxfId="7"/>
     <tableColumn id="3" name="Operands"/>
-    <tableColumn id="4" name="Size" dataDxfId="9"/>
+    <tableColumn id="4" name="Size" dataDxfId="6"/>
     <tableColumn id="5" name="Flow"/>
-    <tableColumn id="6" name="Pop 1" dataDxfId="8"/>
-    <tableColumn id="7" name="Pop 2" dataDxfId="7"/>
-    <tableColumn id="8" name="Pop 3" dataDxfId="6"/>
-    <tableColumn id="9" name="Push 1" dataDxfId="5"/>
-    <tableColumn id="10" name="Push 2" dataDxfId="4"/>
-    <tableColumn id="11" name="Description" dataDxfId="1"/>
+    <tableColumn id="6" name="Pop 1" dataDxfId="5"/>
+    <tableColumn id="7" name="Pop 2" dataDxfId="4"/>
+    <tableColumn id="8" name="Pop 3" dataDxfId="3"/>
+    <tableColumn id="9" name="Push 1" dataDxfId="2"/>
+    <tableColumn id="10" name="Push 2" dataDxfId="1"/>
+    <tableColumn id="11" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1172,9 +1172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="D191" sqref="D191"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1195,7 +1193,7 @@
         <v>205</v>
       </c>
       <c r="B1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>206</v>
@@ -1225,7 +1223,7 @@
         <v>228</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -5089,7 +5087,7 @@
         <v>185</v>
       </c>
       <c r="D134" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="E134" s="1">
         <v>5</v>
@@ -5117,7 +5115,7 @@
         <v>183</v>
       </c>
       <c r="D135" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E135" s="1">
         <v>3</v>
@@ -5145,7 +5143,7 @@
         <v>184</v>
       </c>
       <c r="D136" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E136" s="1">
         <v>3</v>
@@ -5173,7 +5171,7 @@
         <v>182</v>
       </c>
       <c r="D137" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E137" s="1">
         <v>3</v>
@@ -5940,7 +5938,7 @@
         <v>18</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E163" s="1">
         <v>2</v>
@@ -5968,7 +5966,7 @@
         <v>19</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E164" s="1">
         <v>3</v>
@@ -5996,7 +5994,7 @@
         <v>20</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E165" s="1">
         <v>3</v>
@@ -6254,13 +6252,13 @@
         <v>171</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="E174" s="1">
         <v>0</v>
       </c>
       <c r="F174" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="G174" s="1" t="s">
         <v>221</v>
@@ -6723,7 +6721,7 @@
         <v>197</v>
       </c>
       <c r="D190" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E190" s="1">
         <v>4</v>
@@ -6757,7 +6755,7 @@
         <v>3</v>
       </c>
       <c r="F191" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="G191" s="1">
         <v>0</v>
@@ -6779,7 +6777,7 @@
         <v>188</v>
       </c>
       <c r="D192" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E192" s="1">
         <v>2</v>
@@ -7071,7 +7069,7 @@
         <v>17</v>
       </c>
       <c r="D202" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E202" s="1">
         <v>3</v>
@@ -7130,13 +7128,13 @@
         <v>170</v>
       </c>
       <c r="D204" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E204" s="1">
         <v>0</v>
       </c>
       <c r="F204" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="G204" s="1" t="s">
         <v>221</v>
@@ -7217,9 +7215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A205"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A205"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7228,1437 +7224,1437 @@
   <sheetData>
     <row r="1" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L2,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B2,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Aaload;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L2,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B2,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Aaload;</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L3,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B3,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Aastore;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L3,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B3,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Aastore;</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L4,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B4,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Aconst_null;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L4,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B4,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Aconst_null;</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L5,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B5,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Aload;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L5,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B5,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Aload;</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L6,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B6,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Aload_0;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L6,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B6,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Aload_0;</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L7,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B7,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Aload_1;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L7,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B7,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Aload_1;</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L8,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B8,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Aload_2;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L8,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B8,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Aload_2;</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L9,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B9,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Aload_3;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L9,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B9,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Aload_3;</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L10,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B10,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Anewarray;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L10,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B10,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Anewarray;</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L11,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B11,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Areturn;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L11,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B11,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Areturn;</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L12,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B12,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Arraylength;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L12,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B12,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Arraylength;</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L13,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B13,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Astore;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L13,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B13,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Astore;</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L14,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B14,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Astore_0;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L14,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B14,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Astore_0;</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L15,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B15,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Astore_1;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L15,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B15,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Astore_1;</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L16,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B16,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Astore_2;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L16,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B16,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Astore_2;</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L17,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B17,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Astore_3;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L17,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B17,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Astore_3;</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L18,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B18,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Athrow;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L18,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B18,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Athrow;</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L19,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B19,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Baload;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L19,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B19,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Baload;</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L20,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B20,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Bastore;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L20,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B20,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Bastore;</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L21,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B21,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Bipush;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L21,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B21,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Bipush;</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L22,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B22,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Breakpoint;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L22,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B22,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Breakpoint;</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L23,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B23,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Caload;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L23,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B23,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Caload;</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L24,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B24,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Castore;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L24,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B24,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Castore;</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L25,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B25,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Checkcast;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L25,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B25,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Checkcast;</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L26,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B26,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction D2f;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L26,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B26,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode D2f;</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L27,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B27,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction D2i;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L27,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B27,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode D2i;</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L28,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B28,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction D2l;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L28,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B28,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode D2l;</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L29,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B29,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Dadd;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L29,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B29,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Dadd;</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L30,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B30,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Daload;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L30,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B30,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Daload;</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L31,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B31,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Dastore;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L31,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B31,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Dastore;</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L32,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B32,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Dcmpg;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L32,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B32,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Dcmpg;</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L33,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B33,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Dcmpl;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L33,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B33,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Dcmpl;</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L34,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B34,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Dconst_0;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L34,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B34,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Dconst_0;</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L35,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B35,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Dconst_1;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L35,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B35,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Dconst_1;</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L36,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B36,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Ddiv;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L36,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B36,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Ddiv;</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L37,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B37,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Dload;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L37,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B37,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Dload;</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L38,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B38,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Dload_0;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L38,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B38,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Dload_0;</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L39,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B39,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Dload_1;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L39,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B39,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Dload_1;</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L40,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B40,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Dload_2;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L40,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B40,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Dload_2;</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L41,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B41,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Dload_3;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L41,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B41,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Dload_3;</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L42,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B42,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Dmul;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L42,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B42,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Dmul;</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L43,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B43,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Dneg;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L43,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B43,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Dneg;</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L44,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B44,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Drem;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L44,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B44,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Drem;</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L45,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B45,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Dreturn;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L45,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B45,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Dreturn;</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L46,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B46,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Dstore;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L46,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B46,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Dstore;</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L47,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B47,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Dstore_0;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L47,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B47,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Dstore_0;</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L48,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B48,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Dstore_1;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L48,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B48,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Dstore_1;</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L49,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B49,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Dstore_2;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L49,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B49,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Dstore_2;</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L50,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B50,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Dstore_3;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L50,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B50,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Dstore_3;</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L51,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B51,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Dsub;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L51,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B51,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Dsub;</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L52,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B52,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Dup;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L52,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B52,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Dup;</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L53,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B53,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Dup_x1;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L53,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B53,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Dup_x1;</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L54,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B54,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Dup_x2;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L54,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B54,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Dup_x2;</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L55,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B55,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Dup2;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L55,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B55,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Dup2;</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L56,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B56,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Dup2_x1;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L56,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B56,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Dup2_x1;</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L57,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B57,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Dup2_x2;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L57,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B57,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Dup2_x2;</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L58,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B58,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction F2d;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L58,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B58,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode F2d;</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L59,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B59,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction F2i;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L59,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B59,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode F2i;</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L60,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B60,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction F2l;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L60,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B60,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode F2l;</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L61,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B61,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Fadd;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L61,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B61,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Fadd;</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L62,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B62,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Faload;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L62,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B62,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Faload;</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L63,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B63,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Fastore;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L63,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B63,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Fastore;</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L64,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B64,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Fcmpg;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L64,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B64,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Fcmpg;</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L65,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B65,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Fcmpl;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L65,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B65,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Fcmpl;</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L66,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B66,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Fconst_0;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L66,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B66,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Fconst_0;</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L67,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B67,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Fconst_1;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L67,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B67,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Fconst_1;</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L68,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B68,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Fconst_2;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L68,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B68,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Fconst_2;</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L69,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B69,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Fdiv;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L69,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B69,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Fdiv;</v>
       </c>
     </row>
     <row r="69" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L70,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B70,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Fload;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L70,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B70,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Fload;</v>
       </c>
     </row>
     <row r="70" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L71,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B71,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Fload_0;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L71,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B71,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Fload_0;</v>
       </c>
     </row>
     <row r="71" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L72,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B72,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Fload_1;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L72,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B72,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Fload_1;</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L73,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B73,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Fload_2;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L73,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B73,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Fload_2;</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L74,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B74,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Fload_3;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L74,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B74,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Fload_3;</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L75,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B75,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Fmul;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L75,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B75,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Fmul;</v>
       </c>
     </row>
     <row r="75" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L76,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B76,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Fneg;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L76,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B76,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Fneg;</v>
       </c>
     </row>
     <row r="76" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L77,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B77,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Frem;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L77,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B77,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Frem;</v>
       </c>
     </row>
     <row r="77" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L78,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B78,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Freturn;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L78,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B78,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Freturn;</v>
       </c>
     </row>
     <row r="78" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L79,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B79,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Fstore;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L79,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B79,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Fstore;</v>
       </c>
     </row>
     <row r="79" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L80,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B80,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Fstore_0;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L80,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B80,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Fstore_0;</v>
       </c>
     </row>
     <row r="80" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L81,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B81,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Fstore_1;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L81,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B81,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Fstore_1;</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L82,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B82,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Fstore_2;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L82,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B82,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Fstore_2;</v>
       </c>
     </row>
     <row r="82" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L83,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B83,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Fstore_3;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L83,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B83,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Fstore_3;</v>
       </c>
     </row>
     <row r="83" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L84,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B84,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Fsub;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L84,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B84,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Fsub;</v>
       </c>
     </row>
     <row r="84" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L85,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B85,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Getfield;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L85,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B85,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Getfield;</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L86,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B86,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Getstatic;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L86,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B86,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Getstatic;</v>
       </c>
     </row>
     <row r="86" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L87,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B87,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Goto;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L87,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B87,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Goto;</v>
       </c>
     </row>
     <row r="87" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L88,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B88,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Goto_w;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L88,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B88,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Goto_w;</v>
       </c>
     </row>
     <row r="88" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L89,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B89,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction I2b;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L89,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B89,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode I2b;</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L90,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B90,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction I2c;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L90,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B90,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode I2c;</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L91,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B91,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction I2d;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L91,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B91,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode I2d;</v>
       </c>
     </row>
     <row r="91" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L92,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B92,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction I2f;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L92,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B92,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode I2f;</v>
       </c>
     </row>
     <row r="92" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L93,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B93,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction I2l;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L93,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B93,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode I2l;</v>
       </c>
     </row>
     <row r="93" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L94,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B94,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction I2s;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L94,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B94,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode I2s;</v>
       </c>
     </row>
     <row r="94" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L95,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B95,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Iadd;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L95,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B95,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Iadd;</v>
       </c>
     </row>
     <row r="95" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L96,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B96,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Iaload;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L96,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B96,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Iaload;</v>
       </c>
     </row>
     <row r="96" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L97,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B97,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Iand;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L97,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B97,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Iand;</v>
       </c>
     </row>
     <row r="97" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L98,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B98,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Iastore;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L98,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B98,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Iastore;</v>
       </c>
     </row>
     <row r="98" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L99,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B99,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Iconst_0;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L99,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B99,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Iconst_0;</v>
       </c>
     </row>
     <row r="99" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L100,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B100,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Iconst_1;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L100,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B100,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Iconst_1;</v>
       </c>
     </row>
     <row r="100" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L101,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B101,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Iconst_2;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L101,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B101,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Iconst_2;</v>
       </c>
     </row>
     <row r="101" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L102,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B102,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Iconst_3;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L102,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B102,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Iconst_3;</v>
       </c>
     </row>
     <row r="102" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L103,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B103,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Iconst_4;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L103,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B103,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Iconst_4;</v>
       </c>
     </row>
     <row r="103" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L104,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B104,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Iconst_5;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L104,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B104,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Iconst_5;</v>
       </c>
     </row>
     <row r="104" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L105,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B105,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Iconst_m1;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L105,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B105,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Iconst_m1;</v>
       </c>
     </row>
     <row r="105" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L106,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B106,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Idiv;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L106,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B106,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Idiv;</v>
       </c>
     </row>
     <row r="106" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L107,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B107,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction If_acmpeq;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L107,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B107,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode If_acmpeq;</v>
       </c>
     </row>
     <row r="107" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L108,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B108,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction If_acmpne;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L108,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B108,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode If_acmpne;</v>
       </c>
     </row>
     <row r="108" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L109,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B109,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction If_icmpeq;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L109,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B109,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode If_icmpeq;</v>
       </c>
     </row>
     <row r="109" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L110,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B110,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction If_icmpge;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L110,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B110,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode If_icmpge;</v>
       </c>
     </row>
     <row r="110" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L111,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B111,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction If_icmpgt;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L111,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B111,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode If_icmpgt;</v>
       </c>
     </row>
     <row r="111" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L112,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B112,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction If_icmple;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L112,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B112,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode If_icmple;</v>
       </c>
     </row>
     <row r="112" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L113,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B113,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction If_icmplt;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L113,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B113,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode If_icmplt;</v>
       </c>
     </row>
     <row r="113" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L114,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B114,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction If_icmpne;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L114,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B114,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode If_icmpne;</v>
       </c>
     </row>
     <row r="114" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L115,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B115,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Ifeq;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L115,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B115,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Ifeq;</v>
       </c>
     </row>
     <row r="115" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L116,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B116,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Ifge;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L116,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B116,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Ifge;</v>
       </c>
     </row>
     <row r="116" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L117,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B117,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Ifgt;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L117,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B117,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Ifgt;</v>
       </c>
     </row>
     <row r="117" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L118,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B118,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Ifle;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L118,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B118,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Ifle;</v>
       </c>
     </row>
     <row r="118" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L119,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B119,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Iflt;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L119,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B119,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Iflt;</v>
       </c>
     </row>
     <row r="119" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L120,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B120,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Ifne;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L120,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B120,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Ifne;</v>
       </c>
     </row>
     <row r="120" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L121,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B121,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Ifnonnull;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L121,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B121,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Ifnonnull;</v>
       </c>
     </row>
     <row r="121" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L122,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B122,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Ifnull;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L122,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B122,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Ifnull;</v>
       </c>
     </row>
     <row r="122" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L123,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B123,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Iinc;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L123,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B123,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Iinc;</v>
       </c>
     </row>
     <row r="123" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L124,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B124,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Iload;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L124,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B124,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Iload;</v>
       </c>
     </row>
     <row r="124" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L125,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B125,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Iload_0;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L125,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B125,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Iload_0;</v>
       </c>
     </row>
     <row r="125" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L126,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B126,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Iload_1;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L126,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B126,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Iload_1;</v>
       </c>
     </row>
     <row r="126" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L127,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B127,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Iload_2;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L127,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B127,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Iload_2;</v>
       </c>
     </row>
     <row r="127" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L128,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B128,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Iload_3;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L128,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B128,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Iload_3;</v>
       </c>
     </row>
     <row r="128" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L129,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B129,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Impdep1;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L129,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B129,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Impdep1;</v>
       </c>
     </row>
     <row r="129" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L130,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B130,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Impdep2;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L130,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B130,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Impdep2;</v>
       </c>
     </row>
     <row r="130" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L131,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B131,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Imul;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L131,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B131,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Imul;</v>
       </c>
     </row>
     <row r="131" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L132,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B132,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Ineg;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L132,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B132,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Ineg;</v>
       </c>
     </row>
     <row r="132" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L133,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B133,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Instanceof;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L133,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B133,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Instanceof;</v>
       </c>
     </row>
     <row r="133" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L134,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B134,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Invokeinterface;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L134,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B134,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Invokeinterface;</v>
       </c>
     </row>
     <row r="134" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L135,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B135,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Invokespecial;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L135,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B135,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Invokespecial;</v>
       </c>
     </row>
     <row r="135" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L136,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B136,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Invokestatic;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L136,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B136,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Invokestatic;</v>
       </c>
     </row>
     <row r="136" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L137,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B137,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Invokevirtual;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L137,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B137,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Invokevirtual;</v>
       </c>
     </row>
     <row r="137" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L138,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B138,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Ior;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L138,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B138,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Ior;</v>
       </c>
     </row>
     <row r="138" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L139,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B139,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Irem;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L139,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B139,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Irem;</v>
       </c>
     </row>
     <row r="139" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L140,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B140,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Ireturn;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L140,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B140,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Ireturn;</v>
       </c>
     </row>
     <row r="140" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L141,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B141,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Ishl;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L141,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B141,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Ishl;</v>
       </c>
     </row>
     <row r="141" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L142,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B142,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Ishr;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L142,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B142,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Ishr;</v>
       </c>
     </row>
     <row r="142" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L143,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B143,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Istore;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L143,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B143,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Istore;</v>
       </c>
     </row>
     <row r="143" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L144,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B144,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Istore_0;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L144,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B144,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Istore_0;</v>
       </c>
     </row>
     <row r="144" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L145,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B145,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Istore_1;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L145,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B145,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Istore_1;</v>
       </c>
     </row>
     <row r="145" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L146,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B146,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Istore_2;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L146,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B146,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Istore_2;</v>
       </c>
     </row>
     <row r="146" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L147,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B147,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Istore_3;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L147,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B147,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Istore_3;</v>
       </c>
     </row>
     <row r="147" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L148,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B148,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Isub;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L148,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B148,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Isub;</v>
       </c>
     </row>
     <row r="148" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L149,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B149,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Iushr;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L149,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B149,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Iushr;</v>
       </c>
     </row>
     <row r="149" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L150,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B150,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Ixor;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L150,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B150,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Ixor;</v>
       </c>
     </row>
     <row r="150" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L151,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B151,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Jsr;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L151,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B151,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Jsr;</v>
       </c>
     </row>
     <row r="151" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L152,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B152,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Jsr_w;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L152,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B152,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Jsr_w;</v>
       </c>
     </row>
     <row r="152" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L153,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B153,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction L2d;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L153,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B153,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode L2d;</v>
       </c>
     </row>
     <row r="153" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L154,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B154,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction L2f;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L154,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B154,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode L2f;</v>
       </c>
     </row>
     <row r="154" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L155,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B155,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction L2i;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L155,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B155,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode L2i;</v>
       </c>
     </row>
     <row r="155" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L156,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B156,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Ladd;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L156,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B156,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Ladd;</v>
       </c>
     </row>
     <row r="156" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L157,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B157,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Laload;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L157,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B157,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Laload;</v>
       </c>
     </row>
     <row r="157" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L158,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B158,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Land;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L158,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B158,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Land;</v>
       </c>
     </row>
     <row r="158" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L159,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B159,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Lastore;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L159,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B159,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Lastore;</v>
       </c>
     </row>
     <row r="159" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L160,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B160,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Lcmp;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L160,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B160,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Lcmp;</v>
       </c>
     </row>
     <row r="160" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L161,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B161,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Lconst_0;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L161,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B161,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Lconst_0;</v>
       </c>
     </row>
     <row r="161" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L162,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B162,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Lconst_1;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L162,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B162,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Lconst_1;</v>
       </c>
     </row>
     <row r="162" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L163,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B163,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Ldc;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L163,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B163,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Ldc;</v>
       </c>
     </row>
     <row r="163" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L164,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B164,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Ldc_w;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L164,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B164,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Ldc_w;</v>
       </c>
     </row>
     <row r="164" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L165,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B165,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Ldc2_w;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L165,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B165,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Ldc2_w;</v>
       </c>
     </row>
     <row r="165" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L166,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B166,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Ldiv;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L166,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B166,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Ldiv;</v>
       </c>
     </row>
     <row r="166" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L167,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B167,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Lload;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L167,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B167,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Lload;</v>
       </c>
     </row>
     <row r="167" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L168,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B168,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Lload_0;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L168,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B168,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Lload_0;</v>
       </c>
     </row>
     <row r="168" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L169,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B169,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Lload_1;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L169,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B169,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Lload_1;</v>
       </c>
     </row>
     <row r="169" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L170,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B170,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Lload_2;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L170,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B170,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Lload_2;</v>
       </c>
     </row>
     <row r="170" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L171,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B171,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Lload_3;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L171,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B171,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Lload_3;</v>
       </c>
     </row>
     <row r="171" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L172,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B172,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Lmul;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L172,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B172,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Lmul;</v>
       </c>
     </row>
     <row r="172" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L173,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B173,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Lneg;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L173,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B173,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Lneg;</v>
       </c>
     </row>
     <row r="173" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A173" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L174,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B174,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Lookupswitch;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L174,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B174,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Lookupswitch;</v>
       </c>
     </row>
     <row r="174" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A174" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L175,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B175,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Lor;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L175,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B175,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Lor;</v>
       </c>
     </row>
     <row r="175" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A175" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L176,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B176,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Lrem;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L176,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B176,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Lrem;</v>
       </c>
     </row>
     <row r="176" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A176" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L177,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B177,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Lreturn;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L177,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B177,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Lreturn;</v>
       </c>
     </row>
     <row r="177" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L178,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B178,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Lshl;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L178,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B178,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Lshl;</v>
       </c>
     </row>
     <row r="178" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A178" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L179,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B179,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Lshr;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L179,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B179,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Lshr;</v>
       </c>
     </row>
     <row r="179" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L180,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B180,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Lstore;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L180,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B180,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Lstore;</v>
       </c>
     </row>
     <row r="180" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A180" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L181,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B181,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Lstore_0;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L181,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B181,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Lstore_0;</v>
       </c>
     </row>
     <row r="181" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A181" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L182,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B182,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Lstore_1;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L182,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B182,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Lstore_1;</v>
       </c>
     </row>
     <row r="182" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A182" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L183,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B183,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Lstore_2;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L183,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B183,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Lstore_2;</v>
       </c>
     </row>
     <row r="183" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A183" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L184,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B184,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Lstore_3;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L184,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B184,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Lstore_3;</v>
       </c>
     </row>
     <row r="184" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A184" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L185,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B185,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Lsub;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L185,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B185,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Lsub;</v>
       </c>
     </row>
     <row r="185" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A185" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L186,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B186,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Lushr;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L186,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B186,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Lushr;</v>
       </c>
     </row>
     <row r="186" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A186" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L187,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B187,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Lxor;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L187,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B187,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Lxor;</v>
       </c>
     </row>
     <row r="187" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A187" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L188,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B188,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Monitorenter;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L188,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B188,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Monitorenter;</v>
       </c>
     </row>
     <row r="188" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A188" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L189,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B189,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Monitorexit;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L189,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B189,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Monitorexit;</v>
       </c>
     </row>
     <row r="189" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A189" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L190,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B190,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Multianewarray;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L190,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B190,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Multianewarray;</v>
       </c>
     </row>
     <row r="190" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A190" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L191,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B191,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction New;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L191,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B191,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode New;</v>
       </c>
     </row>
     <row r="191" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A191" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L192,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B192,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Newarray;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L192,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B192,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Newarray;</v>
       </c>
     </row>
     <row r="192" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A192" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L193,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B193,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Nop;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L193,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B193,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Nop;</v>
       </c>
     </row>
     <row r="193" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A193" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L194,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B194,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Pop;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L194,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B194,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Pop;</v>
       </c>
     </row>
     <row r="194" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A194" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L195,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B195,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Pop2;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L195,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B195,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Pop2;</v>
       </c>
     </row>
     <row r="195" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A195" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L196,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B196,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Putfield;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L196,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B196,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Putfield;</v>
       </c>
     </row>
     <row r="196" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A196" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L197,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B197,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Putstatic;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L197,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B197,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Putstatic;</v>
       </c>
     </row>
     <row r="197" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A197" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L198,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B198,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Ret;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L198,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B198,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Ret;</v>
       </c>
     </row>
     <row r="198" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A198" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L199,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B199,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Return;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L199,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B199,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Return;</v>
       </c>
     </row>
     <row r="199" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A199" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L200,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B200,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Saload;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L200,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B200,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Saload;</v>
       </c>
     </row>
     <row r="200" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A200" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L201,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B201,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Sastore;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L201,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B201,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Sastore;</v>
       </c>
     </row>
     <row r="201" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A201" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L202,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B202,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Sipush;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L202,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B202,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Sipush;</v>
       </c>
     </row>
     <row r="202" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A202" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L203,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B203,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Swap;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L203,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B203,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Swap;</v>
       </c>
     </row>
     <row r="203" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A203" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L204,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B204,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Tableswitch;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L204,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B204,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Tableswitch;</v>
       </c>
     </row>
     <row r="204" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A204" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L205,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B205,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Wide;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L205,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B205,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Wide;</v>
       </c>
     </row>
     <row r="205" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A205" s="4" t="str">
-        <f>CONCATENATE("/// &lt;summary&gt;",Table!L206,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaInstruction ",Table!B206,";")</f>
-        <v>/// &lt;summary&gt;&lt;/summary&gt;
-public static readonly JavaInstruction Xxxunusedxxx1;</v>
+        <f>CONCATENATE("/// &lt;summary&gt;",Table!L206,"&lt;/summary&gt;",CHAR(10),"public static readonly JavaOpCode ",Table!B206,";")</f>
+        <v>/// &lt;summary&gt;&lt;/summary&gt;
+public static readonly JavaOpCode Xxxunusedxxx1;</v>
       </c>
     </row>
   </sheetData>
@@ -8678,6 +8674,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="0" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="199.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -8690,8 +8687,8 @@
         <v>PushRef</v>
       </c>
       <c r="C1" s="1" t="str">
-        <f>CONCATENATE(Table!B2," = new JavaInstruction(JavaOpCode.",Table!B2,", """,Table!A2,""", JavaOperandType.Inline",Table!D2,", JavaFlowControl.",Table!F2,", ",Table!E2,", JavaStackBehavior.",A1,", JavaStackBehavior.",B1,");")</f>
-        <v>Aaload = new JavaInstruction(JavaOpCode.Aaload, "aaload", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI, JavaStackBehavior.PushRef);</v>
+        <f>CONCATENATE(Table!B2," = new JavaOpCode(JavaOpCodeTag.",Table!B2,", """,Table!A2,""", JavaOperandType.Inline",Table!D2,", JavaFlowControl.",Table!F2,", ",Table!E2,", JavaStackBehavior.",A1,", JavaStackBehavior.",B1,");")</f>
+        <v>Aaload = new JavaOpCode(JavaOpCodeTag.Aaload, "aaload", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI, JavaStackBehavior.PushRef);</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -8704,8 +8701,8 @@
         <v>Push0</v>
       </c>
       <c r="C2" s="1" t="str">
-        <f>CONCATENATE(Table!B3," = new JavaInstruction(JavaOpCode.",Table!B3,", """,Table!A3,""", JavaOperandType.Inline",Table!D3,", JavaFlowControl.",Table!F3,", ",Table!E3,", JavaStackBehavior.",A2,", JavaStackBehavior.",B2,");")</f>
-        <v>Aastore = new JavaInstruction(JavaOpCode.Aastore, "aastore", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI_PopRef, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B3," = new JavaOpCode(JavaOpCodeTag.",Table!B3,", """,Table!A3,""", JavaOperandType.Inline",Table!D3,", JavaFlowControl.",Table!F3,", ",Table!E3,", JavaStackBehavior.",A2,", JavaStackBehavior.",B2,");")</f>
+        <v>Aastore = new JavaOpCode(JavaOpCodeTag.Aastore, "aastore", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI_PopRef, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -8718,8 +8715,8 @@
         <v>PushRef</v>
       </c>
       <c r="C3" s="1" t="str">
-        <f>CONCATENATE(Table!B4," = new JavaInstruction(JavaOpCode.",Table!B4,", """,Table!A4,""", JavaOperandType.Inline",Table!D4,", JavaFlowControl.",Table!F4,", ",Table!E4,", JavaStackBehavior.",A3,", JavaStackBehavior.",B3,");")</f>
-        <v>Aconst_null = new JavaInstruction(JavaOpCode.Aconst_null, "aconst_null", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushRef);</v>
+        <f>CONCATENATE(Table!B4," = new JavaOpCode(JavaOpCodeTag.",Table!B4,", """,Table!A4,""", JavaOperandType.Inline",Table!D4,", JavaFlowControl.",Table!F4,", ",Table!E4,", JavaStackBehavior.",A3,", JavaStackBehavior.",B3,");")</f>
+        <v>Aconst_null = new JavaOpCode(JavaOpCodeTag.Aconst_null, "aconst_null", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushRef);</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -8732,8 +8729,8 @@
         <v>PushRef</v>
       </c>
       <c r="C4" s="1" t="str">
-        <f>CONCATENATE(Table!B5," = new JavaInstruction(JavaOpCode.",Table!B5,", """,Table!A5,""", JavaOperandType.Inline",Table!D5,", JavaFlowControl.",Table!F5,", ",Table!E5,", JavaStackBehavior.",A4,", JavaStackBehavior.",B4,");")</f>
-        <v>Aload = new JavaInstruction(JavaOpCode.Aload, "aload", JavaOperandType.InlineVar, JavaFlowControl.Next, 2, JavaStackBehavior.Pop0, JavaStackBehavior.PushRef);</v>
+        <f>CONCATENATE(Table!B5," = new JavaOpCode(JavaOpCodeTag.",Table!B5,", """,Table!A5,""", JavaOperandType.Inline",Table!D5,", JavaFlowControl.",Table!F5,", ",Table!E5,", JavaStackBehavior.",A4,", JavaStackBehavior.",B4,");")</f>
+        <v>Aload = new JavaOpCode(JavaOpCodeTag.Aload, "aload", JavaOperandType.InlineVar, JavaFlowControl.Next, 2, JavaStackBehavior.Pop0, JavaStackBehavior.PushRef);</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -8746,8 +8743,8 @@
         <v>PushRef</v>
       </c>
       <c r="C5" s="1" t="str">
-        <f>CONCATENATE(Table!B6," = new JavaInstruction(JavaOpCode.",Table!B6,", """,Table!A6,""", JavaOperandType.Inline",Table!D6,", JavaFlowControl.",Table!F6,", ",Table!E6,", JavaStackBehavior.",A5,", JavaStackBehavior.",B5,");")</f>
-        <v>Aload_0 = new JavaInstruction(JavaOpCode.Aload_0, "aload_0", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushRef);</v>
+        <f>CONCATENATE(Table!B6," = new JavaOpCode(JavaOpCodeTag.",Table!B6,", """,Table!A6,""", JavaOperandType.Inline",Table!D6,", JavaFlowControl.",Table!F6,", ",Table!E6,", JavaStackBehavior.",A5,", JavaStackBehavior.",B5,");")</f>
+        <v>Aload_0 = new JavaOpCode(JavaOpCodeTag.Aload_0, "aload_0", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushRef);</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -8760,8 +8757,8 @@
         <v>PushRef</v>
       </c>
       <c r="C6" s="1" t="str">
-        <f>CONCATENATE(Table!B7," = new JavaInstruction(JavaOpCode.",Table!B7,", """,Table!A7,""", JavaOperandType.Inline",Table!D7,", JavaFlowControl.",Table!F7,", ",Table!E7,", JavaStackBehavior.",A6,", JavaStackBehavior.",B6,");")</f>
-        <v>Aload_1 = new JavaInstruction(JavaOpCode.Aload_1, "aload_1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushRef);</v>
+        <f>CONCATENATE(Table!B7," = new JavaOpCode(JavaOpCodeTag.",Table!B7,", """,Table!A7,""", JavaOperandType.Inline",Table!D7,", JavaFlowControl.",Table!F7,", ",Table!E7,", JavaStackBehavior.",A6,", JavaStackBehavior.",B6,");")</f>
+        <v>Aload_1 = new JavaOpCode(JavaOpCodeTag.Aload_1, "aload_1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushRef);</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -8774,8 +8771,8 @@
         <v>PushRef</v>
       </c>
       <c r="C7" s="1" t="str">
-        <f>CONCATENATE(Table!B8," = new JavaInstruction(JavaOpCode.",Table!B8,", """,Table!A8,""", JavaOperandType.Inline",Table!D8,", JavaFlowControl.",Table!F8,", ",Table!E8,", JavaStackBehavior.",A7,", JavaStackBehavior.",B7,");")</f>
-        <v>Aload_2 = new JavaInstruction(JavaOpCode.Aload_2, "aload_2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushRef);</v>
+        <f>CONCATENATE(Table!B8," = new JavaOpCode(JavaOpCodeTag.",Table!B8,", """,Table!A8,""", JavaOperandType.Inline",Table!D8,", JavaFlowControl.",Table!F8,", ",Table!E8,", JavaStackBehavior.",A7,", JavaStackBehavior.",B7,");")</f>
+        <v>Aload_2 = new JavaOpCode(JavaOpCodeTag.Aload_2, "aload_2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushRef);</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -8788,8 +8785,8 @@
         <v>PushRef</v>
       </c>
       <c r="C8" s="1" t="str">
-        <f>CONCATENATE(Table!B9," = new JavaInstruction(JavaOpCode.",Table!B9,", """,Table!A9,""", JavaOperandType.Inline",Table!D9,", JavaFlowControl.",Table!F9,", ",Table!E9,", JavaStackBehavior.",A8,", JavaStackBehavior.",B8,");")</f>
-        <v>Aload_3 = new JavaInstruction(JavaOpCode.Aload_3, "aload_3", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushRef);</v>
+        <f>CONCATENATE(Table!B9," = new JavaOpCode(JavaOpCodeTag.",Table!B9,", """,Table!A9,""", JavaOperandType.Inline",Table!D9,", JavaFlowControl.",Table!F9,", ",Table!E9,", JavaStackBehavior.",A8,", JavaStackBehavior.",B8,");")</f>
+        <v>Aload_3 = new JavaOpCode(JavaOpCodeTag.Aload_3, "aload_3", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushRef);</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -8802,8 +8799,8 @@
         <v>PushRef</v>
       </c>
       <c r="C9" s="1" t="str">
-        <f>CONCATENATE(Table!B10," = new JavaInstruction(JavaOpCode.",Table!B10,", """,Table!A10,""", JavaOperandType.Inline",Table!D10,", JavaFlowControl.",Table!F10,", ",Table!E10,", JavaStackBehavior.",A9,", JavaStackBehavior.",B9,");")</f>
-        <v>Anewarray = new JavaInstruction(JavaOpCode.Anewarray, "anewarray", JavaOperandType.InlineType, JavaFlowControl.Next, 3, JavaStackBehavior.PopI, JavaStackBehavior.PushRef);</v>
+        <f>CONCATENATE(Table!B10," = new JavaOpCode(JavaOpCodeTag.",Table!B10,", """,Table!A10,""", JavaOperandType.Inline",Table!D10,", JavaFlowControl.",Table!F10,", ",Table!E10,", JavaStackBehavior.",A9,", JavaStackBehavior.",B9,");")</f>
+        <v>Anewarray = new JavaOpCode(JavaOpCodeTag.Anewarray, "anewarray", JavaOperandType.InlineType, JavaFlowControl.Next, 3, JavaStackBehavior.PopI, JavaStackBehavior.PushRef);</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -8816,8 +8813,8 @@
         <v>Push0</v>
       </c>
       <c r="C10" s="1" t="str">
-        <f>CONCATENATE(Table!B11," = new JavaInstruction(JavaOpCode.",Table!B11,", """,Table!A11,""", JavaOperandType.Inline",Table!D11,", JavaFlowControl.",Table!F11,", ",Table!E11,", JavaStackBehavior.",A10,", JavaStackBehavior.",B10,");")</f>
-        <v>Areturn = new JavaInstruction(JavaOpCode.Areturn, "areturn", JavaOperandType.InlineNone, JavaFlowControl.Return, 1, JavaStackBehavior.PopRef, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B11," = new JavaOpCode(JavaOpCodeTag.",Table!B11,", """,Table!A11,""", JavaOperandType.Inline",Table!D11,", JavaFlowControl.",Table!F11,", ",Table!E11,", JavaStackBehavior.",A10,", JavaStackBehavior.",B10,");")</f>
+        <v>Areturn = new JavaOpCode(JavaOpCodeTag.Areturn, "areturn", JavaOperandType.InlineNone, JavaFlowControl.Return, 1, JavaStackBehavior.PopRef, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -8830,8 +8827,8 @@
         <v>PushI</v>
       </c>
       <c r="C11" s="1" t="str">
-        <f>CONCATENATE(Table!B12," = new JavaInstruction(JavaOpCode.",Table!B12,", """,Table!A12,""", JavaOperandType.Inline",Table!D12,", JavaFlowControl.",Table!F12,", ",Table!E12,", JavaStackBehavior.",A11,", JavaStackBehavior.",B11,");")</f>
-        <v>Arraylength = new JavaInstruction(JavaOpCode.Arraylength, "arraylength", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B12," = new JavaOpCode(JavaOpCodeTag.",Table!B12,", """,Table!A12,""", JavaOperandType.Inline",Table!D12,", JavaFlowControl.",Table!F12,", ",Table!E12,", JavaStackBehavior.",A11,", JavaStackBehavior.",B11,");")</f>
+        <v>Arraylength = new JavaOpCode(JavaOpCodeTag.Arraylength, "arraylength", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -8844,8 +8841,8 @@
         <v>Push0</v>
       </c>
       <c r="C12" s="1" t="str">
-        <f>CONCATENATE(Table!B13," = new JavaInstruction(JavaOpCode.",Table!B13,", """,Table!A13,""", JavaOperandType.Inline",Table!D13,", JavaFlowControl.",Table!F13,", ",Table!E13,", JavaStackBehavior.",A12,", JavaStackBehavior.",B12,");")</f>
-        <v>Astore = new JavaInstruction(JavaOpCode.Astore, "astore", JavaOperandType.InlineVar, JavaFlowControl.Next, 2, JavaStackBehavior.PopRef, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B13," = new JavaOpCode(JavaOpCodeTag.",Table!B13,", """,Table!A13,""", JavaOperandType.Inline",Table!D13,", JavaFlowControl.",Table!F13,", ",Table!E13,", JavaStackBehavior.",A12,", JavaStackBehavior.",B12,");")</f>
+        <v>Astore = new JavaOpCode(JavaOpCodeTag.Astore, "astore", JavaOperandType.InlineVar, JavaFlowControl.Next, 2, JavaStackBehavior.PopRef, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -8858,8 +8855,8 @@
         <v>Push0</v>
       </c>
       <c r="C13" s="1" t="str">
-        <f>CONCATENATE(Table!B14," = new JavaInstruction(JavaOpCode.",Table!B14,", """,Table!A14,""", JavaOperandType.Inline",Table!D14,", JavaFlowControl.",Table!F14,", ",Table!E14,", JavaStackBehavior.",A13,", JavaStackBehavior.",B13,");")</f>
-        <v>Astore_0 = new JavaInstruction(JavaOpCode.Astore_0, "astore_0", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B14," = new JavaOpCode(JavaOpCodeTag.",Table!B14,", """,Table!A14,""", JavaOperandType.Inline",Table!D14,", JavaFlowControl.",Table!F14,", ",Table!E14,", JavaStackBehavior.",A13,", JavaStackBehavior.",B13,");")</f>
+        <v>Astore_0 = new JavaOpCode(JavaOpCodeTag.Astore_0, "astore_0", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -8872,8 +8869,8 @@
         <v>Push0</v>
       </c>
       <c r="C14" s="1" t="str">
-        <f>CONCATENATE(Table!B15," = new JavaInstruction(JavaOpCode.",Table!B15,", """,Table!A15,""", JavaOperandType.Inline",Table!D15,", JavaFlowControl.",Table!F15,", ",Table!E15,", JavaStackBehavior.",A14,", JavaStackBehavior.",B14,");")</f>
-        <v>Astore_1 = new JavaInstruction(JavaOpCode.Astore_1, "astore_1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B15," = new JavaOpCode(JavaOpCodeTag.",Table!B15,", """,Table!A15,""", JavaOperandType.Inline",Table!D15,", JavaFlowControl.",Table!F15,", ",Table!E15,", JavaStackBehavior.",A14,", JavaStackBehavior.",B14,");")</f>
+        <v>Astore_1 = new JavaOpCode(JavaOpCodeTag.Astore_1, "astore_1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -8886,8 +8883,8 @@
         <v>Push0</v>
       </c>
       <c r="C15" s="1" t="str">
-        <f>CONCATENATE(Table!B16," = new JavaInstruction(JavaOpCode.",Table!B16,", """,Table!A16,""", JavaOperandType.Inline",Table!D16,", JavaFlowControl.",Table!F16,", ",Table!E16,", JavaStackBehavior.",A15,", JavaStackBehavior.",B15,");")</f>
-        <v>Astore_2 = new JavaInstruction(JavaOpCode.Astore_2, "astore_2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B16," = new JavaOpCode(JavaOpCodeTag.",Table!B16,", """,Table!A16,""", JavaOperandType.Inline",Table!D16,", JavaFlowControl.",Table!F16,", ",Table!E16,", JavaStackBehavior.",A15,", JavaStackBehavior.",B15,");")</f>
+        <v>Astore_2 = new JavaOpCode(JavaOpCodeTag.Astore_2, "astore_2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -8900,8 +8897,8 @@
         <v>Push0</v>
       </c>
       <c r="C16" s="1" t="str">
-        <f>CONCATENATE(Table!B17," = new JavaInstruction(JavaOpCode.",Table!B17,", """,Table!A17,""", JavaOperandType.Inline",Table!D17,", JavaFlowControl.",Table!F17,", ",Table!E17,", JavaStackBehavior.",A16,", JavaStackBehavior.",B16,");")</f>
-        <v>Astore_3 = new JavaInstruction(JavaOpCode.Astore_3, "astore_3", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B17," = new JavaOpCode(JavaOpCodeTag.",Table!B17,", """,Table!A17,""", JavaOperandType.Inline",Table!D17,", JavaFlowControl.",Table!F17,", ",Table!E17,", JavaStackBehavior.",A16,", JavaStackBehavior.",B16,");")</f>
+        <v>Astore_3 = new JavaOpCode(JavaOpCodeTag.Astore_3, "astore_3", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -8914,8 +8911,8 @@
         <v>PushRef</v>
       </c>
       <c r="C17" s="1" t="str">
-        <f>CONCATENATE(Table!B18," = new JavaInstruction(JavaOpCode.",Table!B18,", """,Table!A18,""", JavaOperandType.Inline",Table!D18,", JavaFlowControl.",Table!F18,", ",Table!E18,", JavaStackBehavior.",A17,", JavaStackBehavior.",B17,");")</f>
-        <v>Athrow = new JavaInstruction(JavaOpCode.Athrow, "athrow", JavaOperandType.InlineNone, JavaFlowControl.Throw, 1, JavaStackBehavior.PopRef, JavaStackBehavior.PushRef);</v>
+        <f>CONCATENATE(Table!B18," = new JavaOpCode(JavaOpCodeTag.",Table!B18,", """,Table!A18,""", JavaOperandType.Inline",Table!D18,", JavaFlowControl.",Table!F18,", ",Table!E18,", JavaStackBehavior.",A17,", JavaStackBehavior.",B17,");")</f>
+        <v>Athrow = new JavaOpCode(JavaOpCodeTag.Athrow, "athrow", JavaOperandType.InlineNone, JavaFlowControl.Throw, 1, JavaStackBehavior.PopRef, JavaStackBehavior.PushRef);</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -8928,8 +8925,8 @@
         <v>PushI</v>
       </c>
       <c r="C18" s="1" t="str">
-        <f>CONCATENATE(Table!B19," = new JavaInstruction(JavaOpCode.",Table!B19,", """,Table!A19,""", JavaOperandType.Inline",Table!D19,", JavaFlowControl.",Table!F19,", ",Table!E19,", JavaStackBehavior.",A18,", JavaStackBehavior.",B18,");")</f>
-        <v>Baload = new JavaInstruction(JavaOpCode.Baload, "baload", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B19," = new JavaOpCode(JavaOpCodeTag.",Table!B19,", """,Table!A19,""", JavaOperandType.Inline",Table!D19,", JavaFlowControl.",Table!F19,", ",Table!E19,", JavaStackBehavior.",A18,", JavaStackBehavior.",B18,");")</f>
+        <v>Baload = new JavaOpCode(JavaOpCodeTag.Baload, "baload", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -8942,8 +8939,8 @@
         <v>Push0</v>
       </c>
       <c r="C19" s="1" t="str">
-        <f>CONCATENATE(Table!B20," = new JavaInstruction(JavaOpCode.",Table!B20,", """,Table!A20,""", JavaOperandType.Inline",Table!D20,", JavaFlowControl.",Table!F20,", ",Table!E20,", JavaStackBehavior.",A19,", JavaStackBehavior.",B19,");")</f>
-        <v>Bastore = new JavaInstruction(JavaOpCode.Bastore, "bastore", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI_PopI, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B20," = new JavaOpCode(JavaOpCodeTag.",Table!B20,", """,Table!A20,""", JavaOperandType.Inline",Table!D20,", JavaFlowControl.",Table!F20,", ",Table!E20,", JavaStackBehavior.",A19,", JavaStackBehavior.",B19,");")</f>
+        <v>Bastore = new JavaOpCode(JavaOpCodeTag.Bastore, "bastore", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI_PopI, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -8956,8 +8953,8 @@
         <v>PushI</v>
       </c>
       <c r="C20" s="1" t="str">
-        <f>CONCATENATE(Table!B21," = new JavaInstruction(JavaOpCode.",Table!B21,", """,Table!A21,""", JavaOperandType.Inline",Table!D21,", JavaFlowControl.",Table!F21,", ",Table!E21,", JavaStackBehavior.",A20,", JavaStackBehavior.",B20,");")</f>
-        <v>Bipush = new JavaInstruction(JavaOpCode.Bipush, "bipush", JavaOperandType.InlineI1, JavaFlowControl.Next, 2, JavaStackBehavior.Pop0, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B21," = new JavaOpCode(JavaOpCodeTag.",Table!B21,", """,Table!A21,""", JavaOperandType.Inline",Table!D21,", JavaFlowControl.",Table!F21,", ",Table!E21,", JavaStackBehavior.",A20,", JavaStackBehavior.",B20,");")</f>
+        <v>Bipush = new JavaOpCode(JavaOpCodeTag.Bipush, "bipush", JavaOperandType.InlineI1, JavaFlowControl.Next, 2, JavaStackBehavior.Pop0, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -8970,8 +8967,8 @@
         <v>Push0</v>
       </c>
       <c r="C21" s="1" t="str">
-        <f>CONCATENATE(Table!B22," = new JavaInstruction(JavaOpCode.",Table!B22,", """,Table!A22,""", JavaOperandType.Inline",Table!D22,", JavaFlowControl.",Table!F22,", ",Table!E22,", JavaStackBehavior.",A21,", JavaStackBehavior.",B21,");")</f>
-        <v>Breakpoint = new JavaInstruction(JavaOpCode.Breakpoint, "breakpoint", JavaOperandType.InlineNone, JavaFlowControl.Break, 1, JavaStackBehavior.Pop0, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B22," = new JavaOpCode(JavaOpCodeTag.",Table!B22,", """,Table!A22,""", JavaOperandType.Inline",Table!D22,", JavaFlowControl.",Table!F22,", ",Table!E22,", JavaStackBehavior.",A21,", JavaStackBehavior.",B21,");")</f>
+        <v>Breakpoint = new JavaOpCode(JavaOpCodeTag.Breakpoint, "breakpoint", JavaOperandType.InlineNone, JavaFlowControl.Break, 1, JavaStackBehavior.Pop0, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -8984,8 +8981,8 @@
         <v>PushI</v>
       </c>
       <c r="C22" s="1" t="str">
-        <f>CONCATENATE(Table!B23," = new JavaInstruction(JavaOpCode.",Table!B23,", """,Table!A23,""", JavaOperandType.Inline",Table!D23,", JavaFlowControl.",Table!F23,", ",Table!E23,", JavaStackBehavior.",A22,", JavaStackBehavior.",B22,");")</f>
-        <v>Caload = new JavaInstruction(JavaOpCode.Caload, "caload", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B23," = new JavaOpCode(JavaOpCodeTag.",Table!B23,", """,Table!A23,""", JavaOperandType.Inline",Table!D23,", JavaFlowControl.",Table!F23,", ",Table!E23,", JavaStackBehavior.",A22,", JavaStackBehavior.",B22,");")</f>
+        <v>Caload = new JavaOpCode(JavaOpCodeTag.Caload, "caload", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -8998,8 +8995,8 @@
         <v>Push0</v>
       </c>
       <c r="C23" s="1" t="str">
-        <f>CONCATENATE(Table!B24," = new JavaInstruction(JavaOpCode.",Table!B24,", """,Table!A24,""", JavaOperandType.Inline",Table!D24,", JavaFlowControl.",Table!F24,", ",Table!E24,", JavaStackBehavior.",A23,", JavaStackBehavior.",B23,");")</f>
-        <v>Castore = new JavaInstruction(JavaOpCode.Castore, "castore", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI_PopI, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B24," = new JavaOpCode(JavaOpCodeTag.",Table!B24,", """,Table!A24,""", JavaOperandType.Inline",Table!D24,", JavaFlowControl.",Table!F24,", ",Table!E24,", JavaStackBehavior.",A23,", JavaStackBehavior.",B23,");")</f>
+        <v>Castore = new JavaOpCode(JavaOpCodeTag.Castore, "castore", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI_PopI, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -9012,8 +9009,8 @@
         <v>PushRef</v>
       </c>
       <c r="C24" s="1" t="str">
-        <f>CONCATENATE(Table!B25," = new JavaInstruction(JavaOpCode.",Table!B25,", """,Table!A25,""", JavaOperandType.Inline",Table!D25,", JavaFlowControl.",Table!F25,", ",Table!E25,", JavaStackBehavior.",A24,", JavaStackBehavior.",B24,");")</f>
-        <v>Checkcast = new JavaInstruction(JavaOpCode.Checkcast, "checkcast", JavaOperandType.InlineType, JavaFlowControl.Next, 3, JavaStackBehavior.PopRef, JavaStackBehavior.PushRef);</v>
+        <f>CONCATENATE(Table!B25," = new JavaOpCode(JavaOpCodeTag.",Table!B25,", """,Table!A25,""", JavaOperandType.Inline",Table!D25,", JavaFlowControl.",Table!F25,", ",Table!E25,", JavaStackBehavior.",A24,", JavaStackBehavior.",B24,");")</f>
+        <v>Checkcast = new JavaOpCode(JavaOpCodeTag.Checkcast, "checkcast", JavaOperandType.InlineType, JavaFlowControl.Next, 3, JavaStackBehavior.PopRef, JavaStackBehavior.PushRef);</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -9026,8 +9023,8 @@
         <v>PushR4</v>
       </c>
       <c r="C25" s="1" t="str">
-        <f>CONCATENATE(Table!B26," = new JavaInstruction(JavaOpCode.",Table!B26,", """,Table!A26,""", JavaOperandType.Inline",Table!D26,", JavaFlowControl.",Table!F26,", ",Table!E26,", JavaStackBehavior.",A25,", JavaStackBehavior.",B25,");")</f>
-        <v>D2f = new JavaInstruction(JavaOpCode.D2f, "d2f", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8, JavaStackBehavior.PushR4);</v>
+        <f>CONCATENATE(Table!B26," = new JavaOpCode(JavaOpCodeTag.",Table!B26,", """,Table!A26,""", JavaOperandType.Inline",Table!D26,", JavaFlowControl.",Table!F26,", ",Table!E26,", JavaStackBehavior.",A25,", JavaStackBehavior.",B25,");")</f>
+        <v>D2f = new JavaOpCode(JavaOpCodeTag.D2f, "d2f", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8, JavaStackBehavior.PushR4);</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -9040,8 +9037,8 @@
         <v>PushI</v>
       </c>
       <c r="C26" s="1" t="str">
-        <f>CONCATENATE(Table!B27," = new JavaInstruction(JavaOpCode.",Table!B27,", """,Table!A27,""", JavaOperandType.Inline",Table!D27,", JavaFlowControl.",Table!F27,", ",Table!E27,", JavaStackBehavior.",A26,", JavaStackBehavior.",B26,");")</f>
-        <v>D2i = new JavaInstruction(JavaOpCode.D2i, "d2i", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B27," = new JavaOpCode(JavaOpCodeTag.",Table!B27,", """,Table!A27,""", JavaOperandType.Inline",Table!D27,", JavaFlowControl.",Table!F27,", ",Table!E27,", JavaStackBehavior.",A26,", JavaStackBehavior.",B26,");")</f>
+        <v>D2i = new JavaOpCode(JavaOpCodeTag.D2i, "d2i", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -9054,8 +9051,8 @@
         <v>PushI8</v>
       </c>
       <c r="C27" s="1" t="str">
-        <f>CONCATENATE(Table!B28," = new JavaInstruction(JavaOpCode.",Table!B28,", """,Table!A28,""", JavaOperandType.Inline",Table!D28,", JavaFlowControl.",Table!F28,", ",Table!E28,", JavaStackBehavior.",A27,", JavaStackBehavior.",B27,");")</f>
-        <v>D2l = new JavaInstruction(JavaOpCode.D2l, "d2l", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8, JavaStackBehavior.PushI8);</v>
+        <f>CONCATENATE(Table!B28," = new JavaOpCode(JavaOpCodeTag.",Table!B28,", """,Table!A28,""", JavaOperandType.Inline",Table!D28,", JavaFlowControl.",Table!F28,", ",Table!E28,", JavaStackBehavior.",A27,", JavaStackBehavior.",B27,");")</f>
+        <v>D2l = new JavaOpCode(JavaOpCodeTag.D2l, "d2l", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8, JavaStackBehavior.PushI8);</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -9068,8 +9065,8 @@
         <v>PushR8</v>
       </c>
       <c r="C28" s="1" t="str">
-        <f>CONCATENATE(Table!B29," = new JavaInstruction(JavaOpCode.",Table!B29,", """,Table!A29,""", JavaOperandType.Inline",Table!D29,", JavaFlowControl.",Table!F29,", ",Table!E29,", JavaStackBehavior.",A28,", JavaStackBehavior.",B28,");")</f>
-        <v>Dadd = new JavaInstruction(JavaOpCode.Dadd, "dadd", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8_PopR8, JavaStackBehavior.PushR8);</v>
+        <f>CONCATENATE(Table!B29," = new JavaOpCode(JavaOpCodeTag.",Table!B29,", """,Table!A29,""", JavaOperandType.Inline",Table!D29,", JavaFlowControl.",Table!F29,", ",Table!E29,", JavaStackBehavior.",A28,", JavaStackBehavior.",B28,");")</f>
+        <v>Dadd = new JavaOpCode(JavaOpCodeTag.Dadd, "dadd", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8_PopR8, JavaStackBehavior.PushR8);</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -9082,8 +9079,8 @@
         <v>PushR8</v>
       </c>
       <c r="C29" s="1" t="str">
-        <f>CONCATENATE(Table!B30," = new JavaInstruction(JavaOpCode.",Table!B30,", """,Table!A30,""", JavaOperandType.Inline",Table!D30,", JavaFlowControl.",Table!F30,", ",Table!E30,", JavaStackBehavior.",A29,", JavaStackBehavior.",B29,");")</f>
-        <v>Daload = new JavaInstruction(JavaOpCode.Daload, "daload", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI, JavaStackBehavior.PushR8);</v>
+        <f>CONCATENATE(Table!B30," = new JavaOpCode(JavaOpCodeTag.",Table!B30,", """,Table!A30,""", JavaOperandType.Inline",Table!D30,", JavaFlowControl.",Table!F30,", ",Table!E30,", JavaStackBehavior.",A29,", JavaStackBehavior.",B29,");")</f>
+        <v>Daload = new JavaOpCode(JavaOpCodeTag.Daload, "daload", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI, JavaStackBehavior.PushR8);</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -9096,8 +9093,8 @@
         <v>Push0</v>
       </c>
       <c r="C30" s="1" t="str">
-        <f>CONCATENATE(Table!B31," = new JavaInstruction(JavaOpCode.",Table!B31,", """,Table!A31,""", JavaOperandType.Inline",Table!D31,", JavaFlowControl.",Table!F31,", ",Table!E31,", JavaStackBehavior.",A30,", JavaStackBehavior.",B30,");")</f>
-        <v>Dastore = new JavaInstruction(JavaOpCode.Dastore, "dastore", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI_PopR8, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B31," = new JavaOpCode(JavaOpCodeTag.",Table!B31,", """,Table!A31,""", JavaOperandType.Inline",Table!D31,", JavaFlowControl.",Table!F31,", ",Table!E31,", JavaStackBehavior.",A30,", JavaStackBehavior.",B30,");")</f>
+        <v>Dastore = new JavaOpCode(JavaOpCodeTag.Dastore, "dastore", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI_PopR8, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -9110,8 +9107,8 @@
         <v>PushI</v>
       </c>
       <c r="C31" s="1" t="str">
-        <f>CONCATENATE(Table!B32," = new JavaInstruction(JavaOpCode.",Table!B32,", """,Table!A32,""", JavaOperandType.Inline",Table!D32,", JavaFlowControl.",Table!F32,", ",Table!E32,", JavaStackBehavior.",A31,", JavaStackBehavior.",B31,");")</f>
-        <v>Dcmpg = new JavaInstruction(JavaOpCode.Dcmpg, "dcmpg", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8_PopR8, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B32," = new JavaOpCode(JavaOpCodeTag.",Table!B32,", """,Table!A32,""", JavaOperandType.Inline",Table!D32,", JavaFlowControl.",Table!F32,", ",Table!E32,", JavaStackBehavior.",A31,", JavaStackBehavior.",B31,");")</f>
+        <v>Dcmpg = new JavaOpCode(JavaOpCodeTag.Dcmpg, "dcmpg", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8_PopR8, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -9124,8 +9121,8 @@
         <v>PushI</v>
       </c>
       <c r="C32" s="1" t="str">
-        <f>CONCATENATE(Table!B33," = new JavaInstruction(JavaOpCode.",Table!B33,", """,Table!A33,""", JavaOperandType.Inline",Table!D33,", JavaFlowControl.",Table!F33,", ",Table!E33,", JavaStackBehavior.",A32,", JavaStackBehavior.",B32,");")</f>
-        <v>Dcmpl = new JavaInstruction(JavaOpCode.Dcmpl, "dcmpl", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8_PopR8, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B33," = new JavaOpCode(JavaOpCodeTag.",Table!B33,", """,Table!A33,""", JavaOperandType.Inline",Table!D33,", JavaFlowControl.",Table!F33,", ",Table!E33,", JavaStackBehavior.",A32,", JavaStackBehavior.",B32,");")</f>
+        <v>Dcmpl = new JavaOpCode(JavaOpCodeTag.Dcmpl, "dcmpl", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8_PopR8, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -9138,8 +9135,8 @@
         <v>PushR8</v>
       </c>
       <c r="C33" s="1" t="str">
-        <f>CONCATENATE(Table!B34," = new JavaInstruction(JavaOpCode.",Table!B34,", """,Table!A34,""", JavaOperandType.Inline",Table!D34,", JavaFlowControl.",Table!F34,", ",Table!E34,", JavaStackBehavior.",A33,", JavaStackBehavior.",B33,");")</f>
-        <v>Dconst_0 = new JavaInstruction(JavaOpCode.Dconst_0, "dconst_0", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushR8);</v>
+        <f>CONCATENATE(Table!B34," = new JavaOpCode(JavaOpCodeTag.",Table!B34,", """,Table!A34,""", JavaOperandType.Inline",Table!D34,", JavaFlowControl.",Table!F34,", ",Table!E34,", JavaStackBehavior.",A33,", JavaStackBehavior.",B33,");")</f>
+        <v>Dconst_0 = new JavaOpCode(JavaOpCodeTag.Dconst_0, "dconst_0", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushR8);</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -9152,8 +9149,8 @@
         <v>PushR8</v>
       </c>
       <c r="C34" s="1" t="str">
-        <f>CONCATENATE(Table!B35," = new JavaInstruction(JavaOpCode.",Table!B35,", """,Table!A35,""", JavaOperandType.Inline",Table!D35,", JavaFlowControl.",Table!F35,", ",Table!E35,", JavaStackBehavior.",A34,", JavaStackBehavior.",B34,");")</f>
-        <v>Dconst_1 = new JavaInstruction(JavaOpCode.Dconst_1, "dconst_1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushR8);</v>
+        <f>CONCATENATE(Table!B35," = new JavaOpCode(JavaOpCodeTag.",Table!B35,", """,Table!A35,""", JavaOperandType.Inline",Table!D35,", JavaFlowControl.",Table!F35,", ",Table!E35,", JavaStackBehavior.",A34,", JavaStackBehavior.",B34,");")</f>
+        <v>Dconst_1 = new JavaOpCode(JavaOpCodeTag.Dconst_1, "dconst_1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushR8);</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -9166,8 +9163,8 @@
         <v>PushR8</v>
       </c>
       <c r="C35" s="1" t="str">
-        <f>CONCATENATE(Table!B36," = new JavaInstruction(JavaOpCode.",Table!B36,", """,Table!A36,""", JavaOperandType.Inline",Table!D36,", JavaFlowControl.",Table!F36,", ",Table!E36,", JavaStackBehavior.",A35,", JavaStackBehavior.",B35,");")</f>
-        <v>Ddiv = new JavaInstruction(JavaOpCode.Ddiv, "ddiv", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8_PopR8, JavaStackBehavior.PushR8);</v>
+        <f>CONCATENATE(Table!B36," = new JavaOpCode(JavaOpCodeTag.",Table!B36,", """,Table!A36,""", JavaOperandType.Inline",Table!D36,", JavaFlowControl.",Table!F36,", ",Table!E36,", JavaStackBehavior.",A35,", JavaStackBehavior.",B35,");")</f>
+        <v>Ddiv = new JavaOpCode(JavaOpCodeTag.Ddiv, "ddiv", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8_PopR8, JavaStackBehavior.PushR8);</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -9180,8 +9177,8 @@
         <v>PushR8</v>
       </c>
       <c r="C36" s="1" t="str">
-        <f>CONCATENATE(Table!B37," = new JavaInstruction(JavaOpCode.",Table!B37,", """,Table!A37,""", JavaOperandType.Inline",Table!D37,", JavaFlowControl.",Table!F37,", ",Table!E37,", JavaStackBehavior.",A36,", JavaStackBehavior.",B36,");")</f>
-        <v>Dload = new JavaInstruction(JavaOpCode.Dload, "dload", JavaOperandType.InlineVar, JavaFlowControl.Next, 2, JavaStackBehavior.Pop0, JavaStackBehavior.PushR8);</v>
+        <f>CONCATENATE(Table!B37," = new JavaOpCode(JavaOpCodeTag.",Table!B37,", """,Table!A37,""", JavaOperandType.Inline",Table!D37,", JavaFlowControl.",Table!F37,", ",Table!E37,", JavaStackBehavior.",A36,", JavaStackBehavior.",B36,");")</f>
+        <v>Dload = new JavaOpCode(JavaOpCodeTag.Dload, "dload", JavaOperandType.InlineVar, JavaFlowControl.Next, 2, JavaStackBehavior.Pop0, JavaStackBehavior.PushR8);</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -9194,8 +9191,8 @@
         <v>PushR8</v>
       </c>
       <c r="C37" s="1" t="str">
-        <f>CONCATENATE(Table!B38," = new JavaInstruction(JavaOpCode.",Table!B38,", """,Table!A38,""", JavaOperandType.Inline",Table!D38,", JavaFlowControl.",Table!F38,", ",Table!E38,", JavaStackBehavior.",A37,", JavaStackBehavior.",B37,");")</f>
-        <v>Dload_0 = new JavaInstruction(JavaOpCode.Dload_0, "dload_0", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushR8);</v>
+        <f>CONCATENATE(Table!B38," = new JavaOpCode(JavaOpCodeTag.",Table!B38,", """,Table!A38,""", JavaOperandType.Inline",Table!D38,", JavaFlowControl.",Table!F38,", ",Table!E38,", JavaStackBehavior.",A37,", JavaStackBehavior.",B37,");")</f>
+        <v>Dload_0 = new JavaOpCode(JavaOpCodeTag.Dload_0, "dload_0", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushR8);</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -9208,8 +9205,8 @@
         <v>PushR8</v>
       </c>
       <c r="C38" s="1" t="str">
-        <f>CONCATENATE(Table!B39," = new JavaInstruction(JavaOpCode.",Table!B39,", """,Table!A39,""", JavaOperandType.Inline",Table!D39,", JavaFlowControl.",Table!F39,", ",Table!E39,", JavaStackBehavior.",A38,", JavaStackBehavior.",B38,");")</f>
-        <v>Dload_1 = new JavaInstruction(JavaOpCode.Dload_1, "dload_1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushR8);</v>
+        <f>CONCATENATE(Table!B39," = new JavaOpCode(JavaOpCodeTag.",Table!B39,", """,Table!A39,""", JavaOperandType.Inline",Table!D39,", JavaFlowControl.",Table!F39,", ",Table!E39,", JavaStackBehavior.",A38,", JavaStackBehavior.",B38,");")</f>
+        <v>Dload_1 = new JavaOpCode(JavaOpCodeTag.Dload_1, "dload_1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushR8);</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -9222,8 +9219,8 @@
         <v>PushR8</v>
       </c>
       <c r="C39" s="1" t="str">
-        <f>CONCATENATE(Table!B40," = new JavaInstruction(JavaOpCode.",Table!B40,", """,Table!A40,""", JavaOperandType.Inline",Table!D40,", JavaFlowControl.",Table!F40,", ",Table!E40,", JavaStackBehavior.",A39,", JavaStackBehavior.",B39,");")</f>
-        <v>Dload_2 = new JavaInstruction(JavaOpCode.Dload_2, "dload_2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushR8);</v>
+        <f>CONCATENATE(Table!B40," = new JavaOpCode(JavaOpCodeTag.",Table!B40,", """,Table!A40,""", JavaOperandType.Inline",Table!D40,", JavaFlowControl.",Table!F40,", ",Table!E40,", JavaStackBehavior.",A39,", JavaStackBehavior.",B39,");")</f>
+        <v>Dload_2 = new JavaOpCode(JavaOpCodeTag.Dload_2, "dload_2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushR8);</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -9236,8 +9233,8 @@
         <v>PushR8</v>
       </c>
       <c r="C40" s="1" t="str">
-        <f>CONCATENATE(Table!B41," = new JavaInstruction(JavaOpCode.",Table!B41,", """,Table!A41,""", JavaOperandType.Inline",Table!D41,", JavaFlowControl.",Table!F41,", ",Table!E41,", JavaStackBehavior.",A40,", JavaStackBehavior.",B40,");")</f>
-        <v>Dload_3 = new JavaInstruction(JavaOpCode.Dload_3, "dload_3", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushR8);</v>
+        <f>CONCATENATE(Table!B41," = new JavaOpCode(JavaOpCodeTag.",Table!B41,", """,Table!A41,""", JavaOperandType.Inline",Table!D41,", JavaFlowControl.",Table!F41,", ",Table!E41,", JavaStackBehavior.",A40,", JavaStackBehavior.",B40,");")</f>
+        <v>Dload_3 = new JavaOpCode(JavaOpCodeTag.Dload_3, "dload_3", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushR8);</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -9250,8 +9247,8 @@
         <v>PushR8</v>
       </c>
       <c r="C41" s="1" t="str">
-        <f>CONCATENATE(Table!B42," = new JavaInstruction(JavaOpCode.",Table!B42,", """,Table!A42,""", JavaOperandType.Inline",Table!D42,", JavaFlowControl.",Table!F42,", ",Table!E42,", JavaStackBehavior.",A41,", JavaStackBehavior.",B41,");")</f>
-        <v>Dmul = new JavaInstruction(JavaOpCode.Dmul, "dmul", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8_PopR8, JavaStackBehavior.PushR8);</v>
+        <f>CONCATENATE(Table!B42," = new JavaOpCode(JavaOpCodeTag.",Table!B42,", """,Table!A42,""", JavaOperandType.Inline",Table!D42,", JavaFlowControl.",Table!F42,", ",Table!E42,", JavaStackBehavior.",A41,", JavaStackBehavior.",B41,");")</f>
+        <v>Dmul = new JavaOpCode(JavaOpCodeTag.Dmul, "dmul", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8_PopR8, JavaStackBehavior.PushR8);</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -9264,8 +9261,8 @@
         <v>PushR8</v>
       </c>
       <c r="C42" s="1" t="str">
-        <f>CONCATENATE(Table!B43," = new JavaInstruction(JavaOpCode.",Table!B43,", """,Table!A43,""", JavaOperandType.Inline",Table!D43,", JavaFlowControl.",Table!F43,", ",Table!E43,", JavaStackBehavior.",A42,", JavaStackBehavior.",B42,");")</f>
-        <v>Dneg = new JavaInstruction(JavaOpCode.Dneg, "dneg", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8, JavaStackBehavior.PushR8);</v>
+        <f>CONCATENATE(Table!B43," = new JavaOpCode(JavaOpCodeTag.",Table!B43,", """,Table!A43,""", JavaOperandType.Inline",Table!D43,", JavaFlowControl.",Table!F43,", ",Table!E43,", JavaStackBehavior.",A42,", JavaStackBehavior.",B42,");")</f>
+        <v>Dneg = new JavaOpCode(JavaOpCodeTag.Dneg, "dneg", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8, JavaStackBehavior.PushR8);</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -9278,8 +9275,8 @@
         <v>PushR8</v>
       </c>
       <c r="C43" s="1" t="str">
-        <f>CONCATENATE(Table!B44," = new JavaInstruction(JavaOpCode.",Table!B44,", """,Table!A44,""", JavaOperandType.Inline",Table!D44,", JavaFlowControl.",Table!F44,", ",Table!E44,", JavaStackBehavior.",A43,", JavaStackBehavior.",B43,");")</f>
-        <v>Drem = new JavaInstruction(JavaOpCode.Drem, "drem", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8_PopR8, JavaStackBehavior.PushR8);</v>
+        <f>CONCATENATE(Table!B44," = new JavaOpCode(JavaOpCodeTag.",Table!B44,", """,Table!A44,""", JavaOperandType.Inline",Table!D44,", JavaFlowControl.",Table!F44,", ",Table!E44,", JavaStackBehavior.",A43,", JavaStackBehavior.",B43,");")</f>
+        <v>Drem = new JavaOpCode(JavaOpCodeTag.Drem, "drem", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8_PopR8, JavaStackBehavior.PushR8);</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -9292,8 +9289,8 @@
         <v>Push0</v>
       </c>
       <c r="C44" s="1" t="str">
-        <f>CONCATENATE(Table!B45," = new JavaInstruction(JavaOpCode.",Table!B45,", """,Table!A45,""", JavaOperandType.Inline",Table!D45,", JavaFlowControl.",Table!F45,", ",Table!E45,", JavaStackBehavior.",A44,", JavaStackBehavior.",B44,");")</f>
-        <v>Dreturn = new JavaInstruction(JavaOpCode.Dreturn, "dreturn", JavaOperandType.InlineNone, JavaFlowControl.Return, 1, JavaStackBehavior.PopR8, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B45," = new JavaOpCode(JavaOpCodeTag.",Table!B45,", """,Table!A45,""", JavaOperandType.Inline",Table!D45,", JavaFlowControl.",Table!F45,", ",Table!E45,", JavaStackBehavior.",A44,", JavaStackBehavior.",B44,");")</f>
+        <v>Dreturn = new JavaOpCode(JavaOpCodeTag.Dreturn, "dreturn", JavaOperandType.InlineNone, JavaFlowControl.Return, 1, JavaStackBehavior.PopR8, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -9306,8 +9303,8 @@
         <v>Push0</v>
       </c>
       <c r="C45" s="1" t="str">
-        <f>CONCATENATE(Table!B46," = new JavaInstruction(JavaOpCode.",Table!B46,", """,Table!A46,""", JavaOperandType.Inline",Table!D46,", JavaFlowControl.",Table!F46,", ",Table!E46,", JavaStackBehavior.",A45,", JavaStackBehavior.",B45,");")</f>
-        <v>Dstore = new JavaInstruction(JavaOpCode.Dstore, "dstore", JavaOperandType.InlineVar, JavaFlowControl.Next, 2, JavaStackBehavior.PopR8, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B46," = new JavaOpCode(JavaOpCodeTag.",Table!B46,", """,Table!A46,""", JavaOperandType.Inline",Table!D46,", JavaFlowControl.",Table!F46,", ",Table!E46,", JavaStackBehavior.",A45,", JavaStackBehavior.",B45,");")</f>
+        <v>Dstore = new JavaOpCode(JavaOpCodeTag.Dstore, "dstore", JavaOperandType.InlineVar, JavaFlowControl.Next, 2, JavaStackBehavior.PopR8, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -9320,8 +9317,8 @@
         <v>Push0</v>
       </c>
       <c r="C46" s="1" t="str">
-        <f>CONCATENATE(Table!B47," = new JavaInstruction(JavaOpCode.",Table!B47,", """,Table!A47,""", JavaOperandType.Inline",Table!D47,", JavaFlowControl.",Table!F47,", ",Table!E47,", JavaStackBehavior.",A46,", JavaStackBehavior.",B46,");")</f>
-        <v>Dstore_0 = new JavaInstruction(JavaOpCode.Dstore_0, "dstore_0", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B47," = new JavaOpCode(JavaOpCodeTag.",Table!B47,", """,Table!A47,""", JavaOperandType.Inline",Table!D47,", JavaFlowControl.",Table!F47,", ",Table!E47,", JavaStackBehavior.",A46,", JavaStackBehavior.",B46,");")</f>
+        <v>Dstore_0 = new JavaOpCode(JavaOpCodeTag.Dstore_0, "dstore_0", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -9334,8 +9331,8 @@
         <v>Push0</v>
       </c>
       <c r="C47" s="1" t="str">
-        <f>CONCATENATE(Table!B48," = new JavaInstruction(JavaOpCode.",Table!B48,", """,Table!A48,""", JavaOperandType.Inline",Table!D48,", JavaFlowControl.",Table!F48,", ",Table!E48,", JavaStackBehavior.",A47,", JavaStackBehavior.",B47,");")</f>
-        <v>Dstore_1 = new JavaInstruction(JavaOpCode.Dstore_1, "dstore_1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B48," = new JavaOpCode(JavaOpCodeTag.",Table!B48,", """,Table!A48,""", JavaOperandType.Inline",Table!D48,", JavaFlowControl.",Table!F48,", ",Table!E48,", JavaStackBehavior.",A47,", JavaStackBehavior.",B47,");")</f>
+        <v>Dstore_1 = new JavaOpCode(JavaOpCodeTag.Dstore_1, "dstore_1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -9348,8 +9345,8 @@
         <v>Push0</v>
       </c>
       <c r="C48" s="1" t="str">
-        <f>CONCATENATE(Table!B49," = new JavaInstruction(JavaOpCode.",Table!B49,", """,Table!A49,""", JavaOperandType.Inline",Table!D49,", JavaFlowControl.",Table!F49,", ",Table!E49,", JavaStackBehavior.",A48,", JavaStackBehavior.",B48,");")</f>
-        <v>Dstore_2 = new JavaInstruction(JavaOpCode.Dstore_2, "dstore_2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B49," = new JavaOpCode(JavaOpCodeTag.",Table!B49,", """,Table!A49,""", JavaOperandType.Inline",Table!D49,", JavaFlowControl.",Table!F49,", ",Table!E49,", JavaStackBehavior.",A48,", JavaStackBehavior.",B48,");")</f>
+        <v>Dstore_2 = new JavaOpCode(JavaOpCodeTag.Dstore_2, "dstore_2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -9362,8 +9359,8 @@
         <v>Push0</v>
       </c>
       <c r="C49" s="1" t="str">
-        <f>CONCATENATE(Table!B50," = new JavaInstruction(JavaOpCode.",Table!B50,", """,Table!A50,""", JavaOperandType.Inline",Table!D50,", JavaFlowControl.",Table!F50,", ",Table!E50,", JavaStackBehavior.",A49,", JavaStackBehavior.",B49,");")</f>
-        <v>Dstore_3 = new JavaInstruction(JavaOpCode.Dstore_3, "dstore_3", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B50," = new JavaOpCode(JavaOpCodeTag.",Table!B50,", """,Table!A50,""", JavaOperandType.Inline",Table!D50,", JavaFlowControl.",Table!F50,", ",Table!E50,", JavaStackBehavior.",A49,", JavaStackBehavior.",B49,");")</f>
+        <v>Dstore_3 = new JavaOpCode(JavaOpCodeTag.Dstore_3, "dstore_3", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -9376,8 +9373,8 @@
         <v>PushR8</v>
       </c>
       <c r="C50" s="1" t="str">
-        <f>CONCATENATE(Table!B51," = new JavaInstruction(JavaOpCode.",Table!B51,", """,Table!A51,""", JavaOperandType.Inline",Table!D51,", JavaFlowControl.",Table!F51,", ",Table!E51,", JavaStackBehavior.",A50,", JavaStackBehavior.",B50,");")</f>
-        <v>Dsub = new JavaInstruction(JavaOpCode.Dsub, "dsub", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8, JavaStackBehavior.PushR8);</v>
+        <f>CONCATENATE(Table!B51," = new JavaOpCode(JavaOpCodeTag.",Table!B51,", """,Table!A51,""", JavaOperandType.Inline",Table!D51,", JavaFlowControl.",Table!F51,", ",Table!E51,", JavaStackBehavior.",A50,", JavaStackBehavior.",B50,");")</f>
+        <v>Dsub = new JavaOpCode(JavaOpCodeTag.Dsub, "dsub", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR8, JavaStackBehavior.PushR8);</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -9390,8 +9387,8 @@
         <v>Push1_Push1</v>
       </c>
       <c r="C51" s="1" t="str">
-        <f>CONCATENATE(Table!B52," = new JavaInstruction(JavaOpCode.",Table!B52,", """,Table!A52,""", JavaOperandType.Inline",Table!D52,", JavaFlowControl.",Table!F52,", ",Table!E52,", JavaStackBehavior.",A51,", JavaStackBehavior.",B51,");")</f>
-        <v>Dup = new JavaInstruction(JavaOpCode.Dup, "dup", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop1, JavaStackBehavior.Push1_Push1);</v>
+        <f>CONCATENATE(Table!B52," = new JavaOpCode(JavaOpCodeTag.",Table!B52,", """,Table!A52,""", JavaOperandType.Inline",Table!D52,", JavaFlowControl.",Table!F52,", ",Table!E52,", JavaStackBehavior.",A51,", JavaStackBehavior.",B51,");")</f>
+        <v>Dup = new JavaOpCode(JavaOpCodeTag.Dup, "dup", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop1, JavaStackBehavior.Push1_Push1);</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -9404,8 +9401,8 @@
         <v>Push1_Push1</v>
       </c>
       <c r="C52" s="1" t="str">
-        <f>CONCATENATE(Table!B53," = new JavaInstruction(JavaOpCode.",Table!B53,", """,Table!A53,""", JavaOperandType.Inline",Table!D53,", JavaFlowControl.",Table!F53,", ",Table!E53,", JavaStackBehavior.",A52,", JavaStackBehavior.",B52,");")</f>
-        <v>Dup_x1 = new JavaInstruction(JavaOpCode.Dup_x1, "dup_x1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop1_Pop1, JavaStackBehavior.Push1_Push1);</v>
+        <f>CONCATENATE(Table!B53," = new JavaOpCode(JavaOpCodeTag.",Table!B53,", """,Table!A53,""", JavaOperandType.Inline",Table!D53,", JavaFlowControl.",Table!F53,", ",Table!E53,", JavaStackBehavior.",A52,", JavaStackBehavior.",B52,");")</f>
+        <v>Dup_x1 = new JavaOpCode(JavaOpCodeTag.Dup_x1, "dup_x1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop1_Pop1, JavaStackBehavior.Push1_Push1);</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -9418,8 +9415,8 @@
         <v>PushVar</v>
       </c>
       <c r="C53" s="1" t="str">
-        <f>CONCATENATE(Table!B54," = new JavaInstruction(JavaOpCode.",Table!B54,", """,Table!A54,""", JavaOperandType.Inline",Table!D54,", JavaFlowControl.",Table!F54,", ",Table!E54,", JavaStackBehavior.",A53,", JavaStackBehavior.",B53,");")</f>
-        <v>Dup_x2 = new JavaInstruction(JavaOpCode.Dup_x2, "dup_x2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopVar, JavaStackBehavior.PushVar);</v>
+        <f>CONCATENATE(Table!B54," = new JavaOpCode(JavaOpCodeTag.",Table!B54,", """,Table!A54,""", JavaOperandType.Inline",Table!D54,", JavaFlowControl.",Table!F54,", ",Table!E54,", JavaStackBehavior.",A53,", JavaStackBehavior.",B53,");")</f>
+        <v>Dup_x2 = new JavaOpCode(JavaOpCodeTag.Dup_x2, "dup_x2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopVar, JavaStackBehavior.PushVar);</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -9432,8 +9429,8 @@
         <v>PushVar</v>
       </c>
       <c r="C54" s="1" t="str">
-        <f>CONCATENATE(Table!B55," = new JavaInstruction(JavaOpCode.",Table!B55,", """,Table!A55,""", JavaOperandType.Inline",Table!D55,", JavaFlowControl.",Table!F55,", ",Table!E55,", JavaStackBehavior.",A54,", JavaStackBehavior.",B54,");")</f>
-        <v>Dup2 = new JavaInstruction(JavaOpCode.Dup2, "dup2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopVar, JavaStackBehavior.PushVar);</v>
+        <f>CONCATENATE(Table!B55," = new JavaOpCode(JavaOpCodeTag.",Table!B55,", """,Table!A55,""", JavaOperandType.Inline",Table!D55,", JavaFlowControl.",Table!F55,", ",Table!E55,", JavaStackBehavior.",A54,", JavaStackBehavior.",B54,");")</f>
+        <v>Dup2 = new JavaOpCode(JavaOpCodeTag.Dup2, "dup2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopVar, JavaStackBehavior.PushVar);</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -9446,8 +9443,8 @@
         <v>PushVar</v>
       </c>
       <c r="C55" s="1" t="str">
-        <f>CONCATENATE(Table!B56," = new JavaInstruction(JavaOpCode.",Table!B56,", """,Table!A56,""", JavaOperandType.Inline",Table!D56,", JavaFlowControl.",Table!F56,", ",Table!E56,", JavaStackBehavior.",A55,", JavaStackBehavior.",B55,");")</f>
-        <v>Dup2_x1 = new JavaInstruction(JavaOpCode.Dup2_x1, "dup2_x1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopVar, JavaStackBehavior.PushVar);</v>
+        <f>CONCATENATE(Table!B56," = new JavaOpCode(JavaOpCodeTag.",Table!B56,", """,Table!A56,""", JavaOperandType.Inline",Table!D56,", JavaFlowControl.",Table!F56,", ",Table!E56,", JavaStackBehavior.",A55,", JavaStackBehavior.",B55,");")</f>
+        <v>Dup2_x1 = new JavaOpCode(JavaOpCodeTag.Dup2_x1, "dup2_x1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopVar, JavaStackBehavior.PushVar);</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -9460,8 +9457,8 @@
         <v>PushVar</v>
       </c>
       <c r="C56" s="1" t="str">
-        <f>CONCATENATE(Table!B57," = new JavaInstruction(JavaOpCode.",Table!B57,", """,Table!A57,""", JavaOperandType.Inline",Table!D57,", JavaFlowControl.",Table!F57,", ",Table!E57,", JavaStackBehavior.",A56,", JavaStackBehavior.",B56,");")</f>
-        <v>Dup2_x2 = new JavaInstruction(JavaOpCode.Dup2_x2, "dup2_x2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopVar, JavaStackBehavior.PushVar);</v>
+        <f>CONCATENATE(Table!B57," = new JavaOpCode(JavaOpCodeTag.",Table!B57,", """,Table!A57,""", JavaOperandType.Inline",Table!D57,", JavaFlowControl.",Table!F57,", ",Table!E57,", JavaStackBehavior.",A56,", JavaStackBehavior.",B56,");")</f>
+        <v>Dup2_x2 = new JavaOpCode(JavaOpCodeTag.Dup2_x2, "dup2_x2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopVar, JavaStackBehavior.PushVar);</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -9474,8 +9471,8 @@
         <v>PushR8</v>
       </c>
       <c r="C57" s="1" t="str">
-        <f>CONCATENATE(Table!B58," = new JavaInstruction(JavaOpCode.",Table!B58,", """,Table!A58,""", JavaOperandType.Inline",Table!D58,", JavaFlowControl.",Table!F58,", ",Table!E58,", JavaStackBehavior.",A57,", JavaStackBehavior.",B57,");")</f>
-        <v>F2d = new JavaInstruction(JavaOpCode.F2d, "f2d", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4, JavaStackBehavior.PushR8);</v>
+        <f>CONCATENATE(Table!B58," = new JavaOpCode(JavaOpCodeTag.",Table!B58,", """,Table!A58,""", JavaOperandType.Inline",Table!D58,", JavaFlowControl.",Table!F58,", ",Table!E58,", JavaStackBehavior.",A57,", JavaStackBehavior.",B57,");")</f>
+        <v>F2d = new JavaOpCode(JavaOpCodeTag.F2d, "f2d", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4, JavaStackBehavior.PushR8);</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -9488,8 +9485,8 @@
         <v>PushI</v>
       </c>
       <c r="C58" s="1" t="str">
-        <f>CONCATENATE(Table!B59," = new JavaInstruction(JavaOpCode.",Table!B59,", """,Table!A59,""", JavaOperandType.Inline",Table!D59,", JavaFlowControl.",Table!F59,", ",Table!E59,", JavaStackBehavior.",A58,", JavaStackBehavior.",B58,");")</f>
-        <v>F2i = new JavaInstruction(JavaOpCode.F2i, "f2i", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B59," = new JavaOpCode(JavaOpCodeTag.",Table!B59,", """,Table!A59,""", JavaOperandType.Inline",Table!D59,", JavaFlowControl.",Table!F59,", ",Table!E59,", JavaStackBehavior.",A58,", JavaStackBehavior.",B58,");")</f>
+        <v>F2i = new JavaOpCode(JavaOpCodeTag.F2i, "f2i", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -9502,8 +9499,8 @@
         <v>PushI8</v>
       </c>
       <c r="C59" s="1" t="str">
-        <f>CONCATENATE(Table!B60," = new JavaInstruction(JavaOpCode.",Table!B60,", """,Table!A60,""", JavaOperandType.Inline",Table!D60,", JavaFlowControl.",Table!F60,", ",Table!E60,", JavaStackBehavior.",A59,", JavaStackBehavior.",B59,");")</f>
-        <v>F2l = new JavaInstruction(JavaOpCode.F2l, "f2l", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4, JavaStackBehavior.PushI8);</v>
+        <f>CONCATENATE(Table!B60," = new JavaOpCode(JavaOpCodeTag.",Table!B60,", """,Table!A60,""", JavaOperandType.Inline",Table!D60,", JavaFlowControl.",Table!F60,", ",Table!E60,", JavaStackBehavior.",A59,", JavaStackBehavior.",B59,");")</f>
+        <v>F2l = new JavaOpCode(JavaOpCodeTag.F2l, "f2l", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4, JavaStackBehavior.PushI8);</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -9516,8 +9513,8 @@
         <v>PushR4</v>
       </c>
       <c r="C60" s="1" t="str">
-        <f>CONCATENATE(Table!B61," = new JavaInstruction(JavaOpCode.",Table!B61,", """,Table!A61,""", JavaOperandType.Inline",Table!D61,", JavaFlowControl.",Table!F61,", ",Table!E61,", JavaStackBehavior.",A60,", JavaStackBehavior.",B60,");")</f>
-        <v>Fadd = new JavaInstruction(JavaOpCode.Fadd, "fadd", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4_PopR4, JavaStackBehavior.PushR4);</v>
+        <f>CONCATENATE(Table!B61," = new JavaOpCode(JavaOpCodeTag.",Table!B61,", """,Table!A61,""", JavaOperandType.Inline",Table!D61,", JavaFlowControl.",Table!F61,", ",Table!E61,", JavaStackBehavior.",A60,", JavaStackBehavior.",B60,");")</f>
+        <v>Fadd = new JavaOpCode(JavaOpCodeTag.Fadd, "fadd", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4_PopR4, JavaStackBehavior.PushR4);</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -9530,8 +9527,8 @@
         <v>PushR4</v>
       </c>
       <c r="C61" s="1" t="str">
-        <f>CONCATENATE(Table!B62," = new JavaInstruction(JavaOpCode.",Table!B62,", """,Table!A62,""", JavaOperandType.Inline",Table!D62,", JavaFlowControl.",Table!F62,", ",Table!E62,", JavaStackBehavior.",A61,", JavaStackBehavior.",B61,");")</f>
-        <v>Faload = new JavaInstruction(JavaOpCode.Faload, "faload", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI, JavaStackBehavior.PushR4);</v>
+        <f>CONCATENATE(Table!B62," = new JavaOpCode(JavaOpCodeTag.",Table!B62,", """,Table!A62,""", JavaOperandType.Inline",Table!D62,", JavaFlowControl.",Table!F62,", ",Table!E62,", JavaStackBehavior.",A61,", JavaStackBehavior.",B61,");")</f>
+        <v>Faload = new JavaOpCode(JavaOpCodeTag.Faload, "faload", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI, JavaStackBehavior.PushR4);</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -9544,8 +9541,8 @@
         <v>Push0</v>
       </c>
       <c r="C62" s="1" t="str">
-        <f>CONCATENATE(Table!B63," = new JavaInstruction(JavaOpCode.",Table!B63,", """,Table!A63,""", JavaOperandType.Inline",Table!D63,", JavaFlowControl.",Table!F63,", ",Table!E63,", JavaStackBehavior.",A62,", JavaStackBehavior.",B62,");")</f>
-        <v>Fastore = new JavaInstruction(JavaOpCode.Fastore, "fastore", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI_PopR4, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B63," = new JavaOpCode(JavaOpCodeTag.",Table!B63,", """,Table!A63,""", JavaOperandType.Inline",Table!D63,", JavaFlowControl.",Table!F63,", ",Table!E63,", JavaStackBehavior.",A62,", JavaStackBehavior.",B62,");")</f>
+        <v>Fastore = new JavaOpCode(JavaOpCodeTag.Fastore, "fastore", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI_PopR4, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -9558,8 +9555,8 @@
         <v>PushI</v>
       </c>
       <c r="C63" s="1" t="str">
-        <f>CONCATENATE(Table!B64," = new JavaInstruction(JavaOpCode.",Table!B64,", """,Table!A64,""", JavaOperandType.Inline",Table!D64,", JavaFlowControl.",Table!F64,", ",Table!E64,", JavaStackBehavior.",A63,", JavaStackBehavior.",B63,");")</f>
-        <v>Fcmpg = new JavaInstruction(JavaOpCode.Fcmpg, "fcmpg", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4_PopR4, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B64," = new JavaOpCode(JavaOpCodeTag.",Table!B64,", """,Table!A64,""", JavaOperandType.Inline",Table!D64,", JavaFlowControl.",Table!F64,", ",Table!E64,", JavaStackBehavior.",A63,", JavaStackBehavior.",B63,");")</f>
+        <v>Fcmpg = new JavaOpCode(JavaOpCodeTag.Fcmpg, "fcmpg", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4_PopR4, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -9572,8 +9569,8 @@
         <v>PushI</v>
       </c>
       <c r="C64" s="1" t="str">
-        <f>CONCATENATE(Table!B65," = new JavaInstruction(JavaOpCode.",Table!B65,", """,Table!A65,""", JavaOperandType.Inline",Table!D65,", JavaFlowControl.",Table!F65,", ",Table!E65,", JavaStackBehavior.",A64,", JavaStackBehavior.",B64,");")</f>
-        <v>Fcmpl = new JavaInstruction(JavaOpCode.Fcmpl, "fcmpl", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4_PopR4, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B65," = new JavaOpCode(JavaOpCodeTag.",Table!B65,", """,Table!A65,""", JavaOperandType.Inline",Table!D65,", JavaFlowControl.",Table!F65,", ",Table!E65,", JavaStackBehavior.",A64,", JavaStackBehavior.",B64,");")</f>
+        <v>Fcmpl = new JavaOpCode(JavaOpCodeTag.Fcmpl, "fcmpl", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4_PopR4, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -9586,8 +9583,8 @@
         <v>PushR4</v>
       </c>
       <c r="C65" s="1" t="str">
-        <f>CONCATENATE(Table!B66," = new JavaInstruction(JavaOpCode.",Table!B66,", """,Table!A66,""", JavaOperandType.Inline",Table!D66,", JavaFlowControl.",Table!F66,", ",Table!E66,", JavaStackBehavior.",A65,", JavaStackBehavior.",B65,");")</f>
-        <v>Fconst_0 = new JavaInstruction(JavaOpCode.Fconst_0, "fconst_0", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushR4);</v>
+        <f>CONCATENATE(Table!B66," = new JavaOpCode(JavaOpCodeTag.",Table!B66,", """,Table!A66,""", JavaOperandType.Inline",Table!D66,", JavaFlowControl.",Table!F66,", ",Table!E66,", JavaStackBehavior.",A65,", JavaStackBehavior.",B65,");")</f>
+        <v>Fconst_0 = new JavaOpCode(JavaOpCodeTag.Fconst_0, "fconst_0", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushR4);</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -9600,8 +9597,8 @@
         <v>PushR4</v>
       </c>
       <c r="C66" s="1" t="str">
-        <f>CONCATENATE(Table!B67," = new JavaInstruction(JavaOpCode.",Table!B67,", """,Table!A67,""", JavaOperandType.Inline",Table!D67,", JavaFlowControl.",Table!F67,", ",Table!E67,", JavaStackBehavior.",A66,", JavaStackBehavior.",B66,");")</f>
-        <v>Fconst_1 = new JavaInstruction(JavaOpCode.Fconst_1, "fconst_1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushR4);</v>
+        <f>CONCATENATE(Table!B67," = new JavaOpCode(JavaOpCodeTag.",Table!B67,", """,Table!A67,""", JavaOperandType.Inline",Table!D67,", JavaFlowControl.",Table!F67,", ",Table!E67,", JavaStackBehavior.",A66,", JavaStackBehavior.",B66,");")</f>
+        <v>Fconst_1 = new JavaOpCode(JavaOpCodeTag.Fconst_1, "fconst_1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushR4);</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -9614,8 +9611,8 @@
         <v>PushR4</v>
       </c>
       <c r="C67" s="1" t="str">
-        <f>CONCATENATE(Table!B68," = new JavaInstruction(JavaOpCode.",Table!B68,", """,Table!A68,""", JavaOperandType.Inline",Table!D68,", JavaFlowControl.",Table!F68,", ",Table!E68,", JavaStackBehavior.",A67,", JavaStackBehavior.",B67,");")</f>
-        <v>Fconst_2 = new JavaInstruction(JavaOpCode.Fconst_2, "fconst_2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushR4);</v>
+        <f>CONCATENATE(Table!B68," = new JavaOpCode(JavaOpCodeTag.",Table!B68,", """,Table!A68,""", JavaOperandType.Inline",Table!D68,", JavaFlowControl.",Table!F68,", ",Table!E68,", JavaStackBehavior.",A67,", JavaStackBehavior.",B67,");")</f>
+        <v>Fconst_2 = new JavaOpCode(JavaOpCodeTag.Fconst_2, "fconst_2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushR4);</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -9628,8 +9625,8 @@
         <v>PushR4</v>
       </c>
       <c r="C68" s="1" t="str">
-        <f>CONCATENATE(Table!B69," = new JavaInstruction(JavaOpCode.",Table!B69,", """,Table!A69,""", JavaOperandType.Inline",Table!D69,", JavaFlowControl.",Table!F69,", ",Table!E69,", JavaStackBehavior.",A68,", JavaStackBehavior.",B68,");")</f>
-        <v>Fdiv = new JavaInstruction(JavaOpCode.Fdiv, "fdiv", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4_PopR4, JavaStackBehavior.PushR4);</v>
+        <f>CONCATENATE(Table!B69," = new JavaOpCode(JavaOpCodeTag.",Table!B69,", """,Table!A69,""", JavaOperandType.Inline",Table!D69,", JavaFlowControl.",Table!F69,", ",Table!E69,", JavaStackBehavior.",A68,", JavaStackBehavior.",B68,");")</f>
+        <v>Fdiv = new JavaOpCode(JavaOpCodeTag.Fdiv, "fdiv", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4_PopR4, JavaStackBehavior.PushR4);</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -9642,8 +9639,8 @@
         <v>PushR4</v>
       </c>
       <c r="C69" s="1" t="str">
-        <f>CONCATENATE(Table!B70," = new JavaInstruction(JavaOpCode.",Table!B70,", """,Table!A70,""", JavaOperandType.Inline",Table!D70,", JavaFlowControl.",Table!F70,", ",Table!E70,", JavaStackBehavior.",A69,", JavaStackBehavior.",B69,");")</f>
-        <v>Fload = new JavaInstruction(JavaOpCode.Fload, "fload", JavaOperandType.InlineVar, JavaFlowControl.Next, 2, JavaStackBehavior.Pop0, JavaStackBehavior.PushR4);</v>
+        <f>CONCATENATE(Table!B70," = new JavaOpCode(JavaOpCodeTag.",Table!B70,", """,Table!A70,""", JavaOperandType.Inline",Table!D70,", JavaFlowControl.",Table!F70,", ",Table!E70,", JavaStackBehavior.",A69,", JavaStackBehavior.",B69,");")</f>
+        <v>Fload = new JavaOpCode(JavaOpCodeTag.Fload, "fload", JavaOperandType.InlineVar, JavaFlowControl.Next, 2, JavaStackBehavior.Pop0, JavaStackBehavior.PushR4);</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -9656,8 +9653,8 @@
         <v>PushR4</v>
       </c>
       <c r="C70" s="1" t="str">
-        <f>CONCATENATE(Table!B71," = new JavaInstruction(JavaOpCode.",Table!B71,", """,Table!A71,""", JavaOperandType.Inline",Table!D71,", JavaFlowControl.",Table!F71,", ",Table!E71,", JavaStackBehavior.",A70,", JavaStackBehavior.",B70,");")</f>
-        <v>Fload_0 = new JavaInstruction(JavaOpCode.Fload_0, "fload_0", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushR4);</v>
+        <f>CONCATENATE(Table!B71," = new JavaOpCode(JavaOpCodeTag.",Table!B71,", """,Table!A71,""", JavaOperandType.Inline",Table!D71,", JavaFlowControl.",Table!F71,", ",Table!E71,", JavaStackBehavior.",A70,", JavaStackBehavior.",B70,");")</f>
+        <v>Fload_0 = new JavaOpCode(JavaOpCodeTag.Fload_0, "fload_0", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushR4);</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -9670,8 +9667,8 @@
         <v>PushR4</v>
       </c>
       <c r="C71" s="1" t="str">
-        <f>CONCATENATE(Table!B72," = new JavaInstruction(JavaOpCode.",Table!B72,", """,Table!A72,""", JavaOperandType.Inline",Table!D72,", JavaFlowControl.",Table!F72,", ",Table!E72,", JavaStackBehavior.",A71,", JavaStackBehavior.",B71,");")</f>
-        <v>Fload_1 = new JavaInstruction(JavaOpCode.Fload_1, "fload_1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushR4);</v>
+        <f>CONCATENATE(Table!B72," = new JavaOpCode(JavaOpCodeTag.",Table!B72,", """,Table!A72,""", JavaOperandType.Inline",Table!D72,", JavaFlowControl.",Table!F72,", ",Table!E72,", JavaStackBehavior.",A71,", JavaStackBehavior.",B71,");")</f>
+        <v>Fload_1 = new JavaOpCode(JavaOpCodeTag.Fload_1, "fload_1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushR4);</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -9684,8 +9681,8 @@
         <v>PushR4</v>
       </c>
       <c r="C72" s="1" t="str">
-        <f>CONCATENATE(Table!B73," = new JavaInstruction(JavaOpCode.",Table!B73,", """,Table!A73,""", JavaOperandType.Inline",Table!D73,", JavaFlowControl.",Table!F73,", ",Table!E73,", JavaStackBehavior.",A72,", JavaStackBehavior.",B72,");")</f>
-        <v>Fload_2 = new JavaInstruction(JavaOpCode.Fload_2, "fload_2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushR4);</v>
+        <f>CONCATENATE(Table!B73," = new JavaOpCode(JavaOpCodeTag.",Table!B73,", """,Table!A73,""", JavaOperandType.Inline",Table!D73,", JavaFlowControl.",Table!F73,", ",Table!E73,", JavaStackBehavior.",A72,", JavaStackBehavior.",B72,");")</f>
+        <v>Fload_2 = new JavaOpCode(JavaOpCodeTag.Fload_2, "fload_2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushR4);</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -9698,8 +9695,8 @@
         <v>PushR4</v>
       </c>
       <c r="C73" s="1" t="str">
-        <f>CONCATENATE(Table!B74," = new JavaInstruction(JavaOpCode.",Table!B74,", """,Table!A74,""", JavaOperandType.Inline",Table!D74,", JavaFlowControl.",Table!F74,", ",Table!E74,", JavaStackBehavior.",A73,", JavaStackBehavior.",B73,");")</f>
-        <v>Fload_3 = new JavaInstruction(JavaOpCode.Fload_3, "fload_3", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushR4);</v>
+        <f>CONCATENATE(Table!B74," = new JavaOpCode(JavaOpCodeTag.",Table!B74,", """,Table!A74,""", JavaOperandType.Inline",Table!D74,", JavaFlowControl.",Table!F74,", ",Table!E74,", JavaStackBehavior.",A73,", JavaStackBehavior.",B73,");")</f>
+        <v>Fload_3 = new JavaOpCode(JavaOpCodeTag.Fload_3, "fload_3", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushR4);</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -9712,8 +9709,8 @@
         <v>PushR4</v>
       </c>
       <c r="C74" s="1" t="str">
-        <f>CONCATENATE(Table!B75," = new JavaInstruction(JavaOpCode.",Table!B75,", """,Table!A75,""", JavaOperandType.Inline",Table!D75,", JavaFlowControl.",Table!F75,", ",Table!E75,", JavaStackBehavior.",A74,", JavaStackBehavior.",B74,");")</f>
-        <v>Fmul = new JavaInstruction(JavaOpCode.Fmul, "fmul", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4_PopR4, JavaStackBehavior.PushR4);</v>
+        <f>CONCATENATE(Table!B75," = new JavaOpCode(JavaOpCodeTag.",Table!B75,", """,Table!A75,""", JavaOperandType.Inline",Table!D75,", JavaFlowControl.",Table!F75,", ",Table!E75,", JavaStackBehavior.",A74,", JavaStackBehavior.",B74,");")</f>
+        <v>Fmul = new JavaOpCode(JavaOpCodeTag.Fmul, "fmul", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4_PopR4, JavaStackBehavior.PushR4);</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -9726,8 +9723,8 @@
         <v>PushR4</v>
       </c>
       <c r="C75" s="1" t="str">
-        <f>CONCATENATE(Table!B76," = new JavaInstruction(JavaOpCode.",Table!B76,", """,Table!A76,""", JavaOperandType.Inline",Table!D76,", JavaFlowControl.",Table!F76,", ",Table!E76,", JavaStackBehavior.",A75,", JavaStackBehavior.",B75,");")</f>
-        <v>Fneg = new JavaInstruction(JavaOpCode.Fneg, "fneg", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4, JavaStackBehavior.PushR4);</v>
+        <f>CONCATENATE(Table!B76," = new JavaOpCode(JavaOpCodeTag.",Table!B76,", """,Table!A76,""", JavaOperandType.Inline",Table!D76,", JavaFlowControl.",Table!F76,", ",Table!E76,", JavaStackBehavior.",A75,", JavaStackBehavior.",B75,");")</f>
+        <v>Fneg = new JavaOpCode(JavaOpCodeTag.Fneg, "fneg", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4, JavaStackBehavior.PushR4);</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -9740,8 +9737,8 @@
         <v>PushR4</v>
       </c>
       <c r="C76" s="1" t="str">
-        <f>CONCATENATE(Table!B77," = new JavaInstruction(JavaOpCode.",Table!B77,", """,Table!A77,""", JavaOperandType.Inline",Table!D77,", JavaFlowControl.",Table!F77,", ",Table!E77,", JavaStackBehavior.",A76,", JavaStackBehavior.",B76,");")</f>
-        <v>Frem = new JavaInstruction(JavaOpCode.Frem, "frem", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4_PopR4, JavaStackBehavior.PushR4);</v>
+        <f>CONCATENATE(Table!B77," = new JavaOpCode(JavaOpCodeTag.",Table!B77,", """,Table!A77,""", JavaOperandType.Inline",Table!D77,", JavaFlowControl.",Table!F77,", ",Table!E77,", JavaStackBehavior.",A76,", JavaStackBehavior.",B76,");")</f>
+        <v>Frem = new JavaOpCode(JavaOpCodeTag.Frem, "frem", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4_PopR4, JavaStackBehavior.PushR4);</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -9754,8 +9751,8 @@
         <v>Push0</v>
       </c>
       <c r="C77" s="1" t="str">
-        <f>CONCATENATE(Table!B78," = new JavaInstruction(JavaOpCode.",Table!B78,", """,Table!A78,""", JavaOperandType.Inline",Table!D78,", JavaFlowControl.",Table!F78,", ",Table!E78,", JavaStackBehavior.",A77,", JavaStackBehavior.",B77,");")</f>
-        <v>Freturn = new JavaInstruction(JavaOpCode.Freturn, "freturn", JavaOperandType.InlineNone, JavaFlowControl.Return, 1, JavaStackBehavior.PopR4, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B78," = new JavaOpCode(JavaOpCodeTag.",Table!B78,", """,Table!A78,""", JavaOperandType.Inline",Table!D78,", JavaFlowControl.",Table!F78,", ",Table!E78,", JavaStackBehavior.",A77,", JavaStackBehavior.",B77,");")</f>
+        <v>Freturn = new JavaOpCode(JavaOpCodeTag.Freturn, "freturn", JavaOperandType.InlineNone, JavaFlowControl.Return, 1, JavaStackBehavior.PopR4, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -9768,8 +9765,8 @@
         <v>Push0</v>
       </c>
       <c r="C78" s="1" t="str">
-        <f>CONCATENATE(Table!B79," = new JavaInstruction(JavaOpCode.",Table!B79,", """,Table!A79,""", JavaOperandType.Inline",Table!D79,", JavaFlowControl.",Table!F79,", ",Table!E79,", JavaStackBehavior.",A78,", JavaStackBehavior.",B78,");")</f>
-        <v>Fstore = new JavaInstruction(JavaOpCode.Fstore, "fstore", JavaOperandType.InlineVar, JavaFlowControl.Next, 2, JavaStackBehavior.PopR4, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B79," = new JavaOpCode(JavaOpCodeTag.",Table!B79,", """,Table!A79,""", JavaOperandType.Inline",Table!D79,", JavaFlowControl.",Table!F79,", ",Table!E79,", JavaStackBehavior.",A78,", JavaStackBehavior.",B78,");")</f>
+        <v>Fstore = new JavaOpCode(JavaOpCodeTag.Fstore, "fstore", JavaOperandType.InlineVar, JavaFlowControl.Next, 2, JavaStackBehavior.PopR4, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -9782,8 +9779,8 @@
         <v>Push0</v>
       </c>
       <c r="C79" s="1" t="str">
-        <f>CONCATENATE(Table!B80," = new JavaInstruction(JavaOpCode.",Table!B80,", """,Table!A80,""", JavaOperandType.Inline",Table!D80,", JavaFlowControl.",Table!F80,", ",Table!E80,", JavaStackBehavior.",A79,", JavaStackBehavior.",B79,");")</f>
-        <v>Fstore_0 = new JavaInstruction(JavaOpCode.Fstore_0, "fstore_0", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B80," = new JavaOpCode(JavaOpCodeTag.",Table!B80,", """,Table!A80,""", JavaOperandType.Inline",Table!D80,", JavaFlowControl.",Table!F80,", ",Table!E80,", JavaStackBehavior.",A79,", JavaStackBehavior.",B79,");")</f>
+        <v>Fstore_0 = new JavaOpCode(JavaOpCodeTag.Fstore_0, "fstore_0", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -9796,8 +9793,8 @@
         <v>Push0</v>
       </c>
       <c r="C80" s="1" t="str">
-        <f>CONCATENATE(Table!B81," = new JavaInstruction(JavaOpCode.",Table!B81,", """,Table!A81,""", JavaOperandType.Inline",Table!D81,", JavaFlowControl.",Table!F81,", ",Table!E81,", JavaStackBehavior.",A80,", JavaStackBehavior.",B80,");")</f>
-        <v>Fstore_1 = new JavaInstruction(JavaOpCode.Fstore_1, "fstore_1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B81," = new JavaOpCode(JavaOpCodeTag.",Table!B81,", """,Table!A81,""", JavaOperandType.Inline",Table!D81,", JavaFlowControl.",Table!F81,", ",Table!E81,", JavaStackBehavior.",A80,", JavaStackBehavior.",B80,");")</f>
+        <v>Fstore_1 = new JavaOpCode(JavaOpCodeTag.Fstore_1, "fstore_1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -9810,8 +9807,8 @@
         <v>Push0</v>
       </c>
       <c r="C81" s="1" t="str">
-        <f>CONCATENATE(Table!B82," = new JavaInstruction(JavaOpCode.",Table!B82,", """,Table!A82,""", JavaOperandType.Inline",Table!D82,", JavaFlowControl.",Table!F82,", ",Table!E82,", JavaStackBehavior.",A81,", JavaStackBehavior.",B81,");")</f>
-        <v>Fstore_2 = new JavaInstruction(JavaOpCode.Fstore_2, "fstore_2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B82," = new JavaOpCode(JavaOpCodeTag.",Table!B82,", """,Table!A82,""", JavaOperandType.Inline",Table!D82,", JavaFlowControl.",Table!F82,", ",Table!E82,", JavaStackBehavior.",A81,", JavaStackBehavior.",B81,");")</f>
+        <v>Fstore_2 = new JavaOpCode(JavaOpCodeTag.Fstore_2, "fstore_2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -9824,8 +9821,8 @@
         <v>Push0</v>
       </c>
       <c r="C82" s="1" t="str">
-        <f>CONCATENATE(Table!B83," = new JavaInstruction(JavaOpCode.",Table!B83,", """,Table!A83,""", JavaOperandType.Inline",Table!D83,", JavaFlowControl.",Table!F83,", ",Table!E83,", JavaStackBehavior.",A82,", JavaStackBehavior.",B82,");")</f>
-        <v>Fstore_3 = new JavaInstruction(JavaOpCode.Fstore_3, "fstore_3", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B83," = new JavaOpCode(JavaOpCodeTag.",Table!B83,", """,Table!A83,""", JavaOperandType.Inline",Table!D83,", JavaFlowControl.",Table!F83,", ",Table!E83,", JavaStackBehavior.",A82,", JavaStackBehavior.",B82,");")</f>
+        <v>Fstore_3 = new JavaOpCode(JavaOpCodeTag.Fstore_3, "fstore_3", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -9838,8 +9835,8 @@
         <v>PushR4</v>
       </c>
       <c r="C83" s="1" t="str">
-        <f>CONCATENATE(Table!B84," = new JavaInstruction(JavaOpCode.",Table!B84,", """,Table!A84,""", JavaOperandType.Inline",Table!D84,", JavaFlowControl.",Table!F84,", ",Table!E84,", JavaStackBehavior.",A83,", JavaStackBehavior.",B83,");")</f>
-        <v>Fsub = new JavaInstruction(JavaOpCode.Fsub, "fsub", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4_PopR4, JavaStackBehavior.PushR4);</v>
+        <f>CONCATENATE(Table!B84," = new JavaOpCode(JavaOpCodeTag.",Table!B84,", """,Table!A84,""", JavaOperandType.Inline",Table!D84,", JavaFlowControl.",Table!F84,", ",Table!E84,", JavaStackBehavior.",A83,", JavaStackBehavior.",B83,");")</f>
+        <v>Fsub = new JavaOpCode(JavaOpCodeTag.Fsub, "fsub", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopR4_PopR4, JavaStackBehavior.PushR4);</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -9852,8 +9849,8 @@
         <v>Push1</v>
       </c>
       <c r="C84" s="1" t="str">
-        <f>CONCATENATE(Table!B85," = new JavaInstruction(JavaOpCode.",Table!B85,", """,Table!A85,""", JavaOperandType.Inline",Table!D85,", JavaFlowControl.",Table!F85,", ",Table!E85,", JavaStackBehavior.",A84,", JavaStackBehavior.",B84,");")</f>
-        <v>Getfield = new JavaInstruction(JavaOpCode.Getfield, "getfield", JavaOperandType.InlineField, JavaFlowControl.Next, 3, JavaStackBehavior.PopRef, JavaStackBehavior.Push1);</v>
+        <f>CONCATENATE(Table!B85," = new JavaOpCode(JavaOpCodeTag.",Table!B85,", """,Table!A85,""", JavaOperandType.Inline",Table!D85,", JavaFlowControl.",Table!F85,", ",Table!E85,", JavaStackBehavior.",A84,", JavaStackBehavior.",B84,");")</f>
+        <v>Getfield = new JavaOpCode(JavaOpCodeTag.Getfield, "getfield", JavaOperandType.InlineField, JavaFlowControl.Next, 3, JavaStackBehavior.PopRef, JavaStackBehavior.Push1);</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -9866,8 +9863,8 @@
         <v>Push1</v>
       </c>
       <c r="C85" s="1" t="str">
-        <f>CONCATENATE(Table!B86," = new JavaInstruction(JavaOpCode.",Table!B86,", """,Table!A86,""", JavaOperandType.Inline",Table!D86,", JavaFlowControl.",Table!F86,", ",Table!E86,", JavaStackBehavior.",A85,", JavaStackBehavior.",B85,");")</f>
-        <v>Getstatic = new JavaInstruction(JavaOpCode.Getstatic, "getstatic", JavaOperandType.InlineField, JavaFlowControl.Next, 3, JavaStackBehavior.Pop0, JavaStackBehavior.Push1);</v>
+        <f>CONCATENATE(Table!B86," = new JavaOpCode(JavaOpCodeTag.",Table!B86,", """,Table!A86,""", JavaOperandType.Inline",Table!D86,", JavaFlowControl.",Table!F86,", ",Table!E86,", JavaStackBehavior.",A85,", JavaStackBehavior.",B85,");")</f>
+        <v>Getstatic = new JavaOpCode(JavaOpCodeTag.Getstatic, "getstatic", JavaOperandType.InlineField, JavaFlowControl.Next, 3, JavaStackBehavior.Pop0, JavaStackBehavior.Push1);</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -9880,8 +9877,8 @@
         <v>Push0</v>
       </c>
       <c r="C86" s="1" t="str">
-        <f>CONCATENATE(Table!B87," = new JavaInstruction(JavaOpCode.",Table!B87,", """,Table!A87,""", JavaOperandType.Inline",Table!D87,", JavaFlowControl.",Table!F87,", ",Table!E87,", JavaStackBehavior.",A86,", JavaStackBehavior.",B86,");")</f>
-        <v>Goto = new JavaInstruction(JavaOpCode.Goto, "goto", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.Branch, 3, JavaStackBehavior.Pop0, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B87," = new JavaOpCode(JavaOpCodeTag.",Table!B87,", """,Table!A87,""", JavaOperandType.Inline",Table!D87,", JavaFlowControl.",Table!F87,", ",Table!E87,", JavaStackBehavior.",A86,", JavaStackBehavior.",B86,");")</f>
+        <v>Goto = new JavaOpCode(JavaOpCodeTag.Goto, "goto", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.Branch, 3, JavaStackBehavior.Pop0, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -9894,8 +9891,8 @@
         <v>Push0</v>
       </c>
       <c r="C87" s="1" t="str">
-        <f>CONCATENATE(Table!B88," = new JavaInstruction(JavaOpCode.",Table!B88,", """,Table!A88,""", JavaOperandType.Inline",Table!D88,", JavaFlowControl.",Table!F88,", ",Table!E88,", JavaStackBehavior.",A87,", JavaStackBehavior.",B87,");")</f>
-        <v>Goto_w = new JavaInstruction(JavaOpCode.Goto_w, "goto_w", JavaOperandType.InlineBranchTarget, JavaFlowControl.Branch, 5, JavaStackBehavior.Pop0, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B88," = new JavaOpCode(JavaOpCodeTag.",Table!B88,", """,Table!A88,""", JavaOperandType.Inline",Table!D88,", JavaFlowControl.",Table!F88,", ",Table!E88,", JavaStackBehavior.",A87,", JavaStackBehavior.",B87,");")</f>
+        <v>Goto_w = new JavaOpCode(JavaOpCodeTag.Goto_w, "goto_w", JavaOperandType.InlineBranchTarget, JavaFlowControl.Branch, 5, JavaStackBehavior.Pop0, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -9908,8 +9905,8 @@
         <v>PushI</v>
       </c>
       <c r="C88" s="1" t="str">
-        <f>CONCATENATE(Table!B89," = new JavaInstruction(JavaOpCode.",Table!B89,", """,Table!A89,""", JavaOperandType.Inline",Table!D89,", JavaFlowControl.",Table!F89,", ",Table!E89,", JavaStackBehavior.",A88,", JavaStackBehavior.",B88,");")</f>
-        <v>I2b = new JavaInstruction(JavaOpCode.I2b, "i2b", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B89," = new JavaOpCode(JavaOpCodeTag.",Table!B89,", """,Table!A89,""", JavaOperandType.Inline",Table!D89,", JavaFlowControl.",Table!F89,", ",Table!E89,", JavaStackBehavior.",A88,", JavaStackBehavior.",B88,");")</f>
+        <v>I2b = new JavaOpCode(JavaOpCodeTag.I2b, "i2b", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -9922,8 +9919,8 @@
         <v>PushI</v>
       </c>
       <c r="C89" s="1" t="str">
-        <f>CONCATENATE(Table!B90," = new JavaInstruction(JavaOpCode.",Table!B90,", """,Table!A90,""", JavaOperandType.Inline",Table!D90,", JavaFlowControl.",Table!F90,", ",Table!E90,", JavaStackBehavior.",A89,", JavaStackBehavior.",B89,");")</f>
-        <v>I2c = new JavaInstruction(JavaOpCode.I2c, "i2c", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B90," = new JavaOpCode(JavaOpCodeTag.",Table!B90,", """,Table!A90,""", JavaOperandType.Inline",Table!D90,", JavaFlowControl.",Table!F90,", ",Table!E90,", JavaStackBehavior.",A89,", JavaStackBehavior.",B89,");")</f>
+        <v>I2c = new JavaOpCode(JavaOpCodeTag.I2c, "i2c", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -9936,8 +9933,8 @@
         <v>PushR8</v>
       </c>
       <c r="C90" s="1" t="str">
-        <f>CONCATENATE(Table!B91," = new JavaInstruction(JavaOpCode.",Table!B91,", """,Table!A91,""", JavaOperandType.Inline",Table!D91,", JavaFlowControl.",Table!F91,", ",Table!E91,", JavaStackBehavior.",A90,", JavaStackBehavior.",B90,");")</f>
-        <v>I2d = new JavaInstruction(JavaOpCode.I2d, "i2d", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI, JavaStackBehavior.PushR8);</v>
+        <f>CONCATENATE(Table!B91," = new JavaOpCode(JavaOpCodeTag.",Table!B91,", """,Table!A91,""", JavaOperandType.Inline",Table!D91,", JavaFlowControl.",Table!F91,", ",Table!E91,", JavaStackBehavior.",A90,", JavaStackBehavior.",B90,");")</f>
+        <v>I2d = new JavaOpCode(JavaOpCodeTag.I2d, "i2d", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI, JavaStackBehavior.PushR8);</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -9950,8 +9947,8 @@
         <v>PushR4</v>
       </c>
       <c r="C91" s="1" t="str">
-        <f>CONCATENATE(Table!B92," = new JavaInstruction(JavaOpCode.",Table!B92,", """,Table!A92,""", JavaOperandType.Inline",Table!D92,", JavaFlowControl.",Table!F92,", ",Table!E92,", JavaStackBehavior.",A91,", JavaStackBehavior.",B91,");")</f>
-        <v>I2f = new JavaInstruction(JavaOpCode.I2f, "i2f", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI, JavaStackBehavior.PushR4);</v>
+        <f>CONCATENATE(Table!B92," = new JavaOpCode(JavaOpCodeTag.",Table!B92,", """,Table!A92,""", JavaOperandType.Inline",Table!D92,", JavaFlowControl.",Table!F92,", ",Table!E92,", JavaStackBehavior.",A91,", JavaStackBehavior.",B91,");")</f>
+        <v>I2f = new JavaOpCode(JavaOpCodeTag.I2f, "i2f", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI, JavaStackBehavior.PushR4);</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -9964,8 +9961,8 @@
         <v>PushI8</v>
       </c>
       <c r="C92" s="1" t="str">
-        <f>CONCATENATE(Table!B93," = new JavaInstruction(JavaOpCode.",Table!B93,", """,Table!A93,""", JavaOperandType.Inline",Table!D93,", JavaFlowControl.",Table!F93,", ",Table!E93,", JavaStackBehavior.",A92,", JavaStackBehavior.",B92,");")</f>
-        <v>I2l = new JavaInstruction(JavaOpCode.I2l, "i2l", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI, JavaStackBehavior.PushI8);</v>
+        <f>CONCATENATE(Table!B93," = new JavaOpCode(JavaOpCodeTag.",Table!B93,", """,Table!A93,""", JavaOperandType.Inline",Table!D93,", JavaFlowControl.",Table!F93,", ",Table!E93,", JavaStackBehavior.",A92,", JavaStackBehavior.",B92,");")</f>
+        <v>I2l = new JavaOpCode(JavaOpCodeTag.I2l, "i2l", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI, JavaStackBehavior.PushI8);</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -9978,8 +9975,8 @@
         <v>PushI</v>
       </c>
       <c r="C93" s="1" t="str">
-        <f>CONCATENATE(Table!B94," = new JavaInstruction(JavaOpCode.",Table!B94,", """,Table!A94,""", JavaOperandType.Inline",Table!D94,", JavaFlowControl.",Table!F94,", ",Table!E94,", JavaStackBehavior.",A93,", JavaStackBehavior.",B93,");")</f>
-        <v>I2s = new JavaInstruction(JavaOpCode.I2s, "i2s", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B94," = new JavaOpCode(JavaOpCodeTag.",Table!B94,", """,Table!A94,""", JavaOperandType.Inline",Table!D94,", JavaFlowControl.",Table!F94,", ",Table!E94,", JavaStackBehavior.",A93,", JavaStackBehavior.",B93,");")</f>
+        <v>I2s = new JavaOpCode(JavaOpCodeTag.I2s, "i2s", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -9992,8 +9989,8 @@
         <v>PushI</v>
       </c>
       <c r="C94" s="1" t="str">
-        <f>CONCATENATE(Table!B95," = new JavaInstruction(JavaOpCode.",Table!B95,", """,Table!A95,""", JavaOperandType.Inline",Table!D95,", JavaFlowControl.",Table!F95,", ",Table!E95,", JavaStackBehavior.",A94,", JavaStackBehavior.",B94,");")</f>
-        <v>Iadd = new JavaInstruction(JavaOpCode.Iadd, "iadd", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI_PopI, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B95," = new JavaOpCode(JavaOpCodeTag.",Table!B95,", """,Table!A95,""", JavaOperandType.Inline",Table!D95,", JavaFlowControl.",Table!F95,", ",Table!E95,", JavaStackBehavior.",A94,", JavaStackBehavior.",B94,");")</f>
+        <v>Iadd = new JavaOpCode(JavaOpCodeTag.Iadd, "iadd", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI_PopI, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -10006,8 +10003,8 @@
         <v>PushI</v>
       </c>
       <c r="C95" s="1" t="str">
-        <f>CONCATENATE(Table!B96," = new JavaInstruction(JavaOpCode.",Table!B96,", """,Table!A96,""", JavaOperandType.Inline",Table!D96,", JavaFlowControl.",Table!F96,", ",Table!E96,", JavaStackBehavior.",A95,", JavaStackBehavior.",B95,");")</f>
-        <v>Iaload = new JavaInstruction(JavaOpCode.Iaload, "iaload", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B96," = new JavaOpCode(JavaOpCodeTag.",Table!B96,", """,Table!A96,""", JavaOperandType.Inline",Table!D96,", JavaFlowControl.",Table!F96,", ",Table!E96,", JavaStackBehavior.",A95,", JavaStackBehavior.",B95,");")</f>
+        <v>Iaload = new JavaOpCode(JavaOpCodeTag.Iaload, "iaload", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -10020,8 +10017,8 @@
         <v>PushI</v>
       </c>
       <c r="C96" s="1" t="str">
-        <f>CONCATENATE(Table!B97," = new JavaInstruction(JavaOpCode.",Table!B97,", """,Table!A97,""", JavaOperandType.Inline",Table!D97,", JavaFlowControl.",Table!F97,", ",Table!E97,", JavaStackBehavior.",A96,", JavaStackBehavior.",B96,");")</f>
-        <v>Iand = new JavaInstruction(JavaOpCode.Iand, "iand", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI_PopI, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B97," = new JavaOpCode(JavaOpCodeTag.",Table!B97,", """,Table!A97,""", JavaOperandType.Inline",Table!D97,", JavaFlowControl.",Table!F97,", ",Table!E97,", JavaStackBehavior.",A96,", JavaStackBehavior.",B96,");")</f>
+        <v>Iand = new JavaOpCode(JavaOpCodeTag.Iand, "iand", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI_PopI, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -10034,8 +10031,8 @@
         <v>Push0</v>
       </c>
       <c r="C97" s="1" t="str">
-        <f>CONCATENATE(Table!B98," = new JavaInstruction(JavaOpCode.",Table!B98,", """,Table!A98,""", JavaOperandType.Inline",Table!D98,", JavaFlowControl.",Table!F98,", ",Table!E98,", JavaStackBehavior.",A97,", JavaStackBehavior.",B97,");")</f>
-        <v>Iastore = new JavaInstruction(JavaOpCode.Iastore, "iastore", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI_PopI, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B98," = new JavaOpCode(JavaOpCodeTag.",Table!B98,", """,Table!A98,""", JavaOperandType.Inline",Table!D98,", JavaFlowControl.",Table!F98,", ",Table!E98,", JavaStackBehavior.",A97,", JavaStackBehavior.",B97,");")</f>
+        <v>Iastore = new JavaOpCode(JavaOpCodeTag.Iastore, "iastore", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI_PopI, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -10048,8 +10045,8 @@
         <v>PushI</v>
       </c>
       <c r="C98" s="1" t="str">
-        <f>CONCATENATE(Table!B99," = new JavaInstruction(JavaOpCode.",Table!B99,", """,Table!A99,""", JavaOperandType.Inline",Table!D99,", JavaFlowControl.",Table!F99,", ",Table!E99,", JavaStackBehavior.",A98,", JavaStackBehavior.",B98,");")</f>
-        <v>Iconst_0 = new JavaInstruction(JavaOpCode.Iconst_0, "iconst_0", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B99," = new JavaOpCode(JavaOpCodeTag.",Table!B99,", """,Table!A99,""", JavaOperandType.Inline",Table!D99,", JavaFlowControl.",Table!F99,", ",Table!E99,", JavaStackBehavior.",A98,", JavaStackBehavior.",B98,");")</f>
+        <v>Iconst_0 = new JavaOpCode(JavaOpCodeTag.Iconst_0, "iconst_0", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -10062,8 +10059,8 @@
         <v>PushI</v>
       </c>
       <c r="C99" s="1" t="str">
-        <f>CONCATENATE(Table!B100," = new JavaInstruction(JavaOpCode.",Table!B100,", """,Table!A100,""", JavaOperandType.Inline",Table!D100,", JavaFlowControl.",Table!F100,", ",Table!E100,", JavaStackBehavior.",A99,", JavaStackBehavior.",B99,");")</f>
-        <v>Iconst_1 = new JavaInstruction(JavaOpCode.Iconst_1, "iconst_1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B100," = new JavaOpCode(JavaOpCodeTag.",Table!B100,", """,Table!A100,""", JavaOperandType.Inline",Table!D100,", JavaFlowControl.",Table!F100,", ",Table!E100,", JavaStackBehavior.",A99,", JavaStackBehavior.",B99,");")</f>
+        <v>Iconst_1 = new JavaOpCode(JavaOpCodeTag.Iconst_1, "iconst_1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -10076,8 +10073,8 @@
         <v>PushI</v>
       </c>
       <c r="C100" s="1" t="str">
-        <f>CONCATENATE(Table!B101," = new JavaInstruction(JavaOpCode.",Table!B101,", """,Table!A101,""", JavaOperandType.Inline",Table!D101,", JavaFlowControl.",Table!F101,", ",Table!E101,", JavaStackBehavior.",A100,", JavaStackBehavior.",B100,");")</f>
-        <v>Iconst_2 = new JavaInstruction(JavaOpCode.Iconst_2, "iconst_2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B101," = new JavaOpCode(JavaOpCodeTag.",Table!B101,", """,Table!A101,""", JavaOperandType.Inline",Table!D101,", JavaFlowControl.",Table!F101,", ",Table!E101,", JavaStackBehavior.",A100,", JavaStackBehavior.",B100,");")</f>
+        <v>Iconst_2 = new JavaOpCode(JavaOpCodeTag.Iconst_2, "iconst_2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -10090,8 +10087,8 @@
         <v>PushI</v>
       </c>
       <c r="C101" s="1" t="str">
-        <f>CONCATENATE(Table!B102," = new JavaInstruction(JavaOpCode.",Table!B102,", """,Table!A102,""", JavaOperandType.Inline",Table!D102,", JavaFlowControl.",Table!F102,", ",Table!E102,", JavaStackBehavior.",A101,", JavaStackBehavior.",B101,");")</f>
-        <v>Iconst_3 = new JavaInstruction(JavaOpCode.Iconst_3, "iconst_3", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B102," = new JavaOpCode(JavaOpCodeTag.",Table!B102,", """,Table!A102,""", JavaOperandType.Inline",Table!D102,", JavaFlowControl.",Table!F102,", ",Table!E102,", JavaStackBehavior.",A101,", JavaStackBehavior.",B101,");")</f>
+        <v>Iconst_3 = new JavaOpCode(JavaOpCodeTag.Iconst_3, "iconst_3", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -10104,8 +10101,8 @@
         <v>PushI</v>
       </c>
       <c r="C102" s="1" t="str">
-        <f>CONCATENATE(Table!B103," = new JavaInstruction(JavaOpCode.",Table!B103,", """,Table!A103,""", JavaOperandType.Inline",Table!D103,", JavaFlowControl.",Table!F103,", ",Table!E103,", JavaStackBehavior.",A102,", JavaStackBehavior.",B102,");")</f>
-        <v>Iconst_4 = new JavaInstruction(JavaOpCode.Iconst_4, "iconst_4", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B103," = new JavaOpCode(JavaOpCodeTag.",Table!B103,", """,Table!A103,""", JavaOperandType.Inline",Table!D103,", JavaFlowControl.",Table!F103,", ",Table!E103,", JavaStackBehavior.",A102,", JavaStackBehavior.",B102,");")</f>
+        <v>Iconst_4 = new JavaOpCode(JavaOpCodeTag.Iconst_4, "iconst_4", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -10118,8 +10115,8 @@
         <v>PushI</v>
       </c>
       <c r="C103" s="1" t="str">
-        <f>CONCATENATE(Table!B104," = new JavaInstruction(JavaOpCode.",Table!B104,", """,Table!A104,""", JavaOperandType.Inline",Table!D104,", JavaFlowControl.",Table!F104,", ",Table!E104,", JavaStackBehavior.",A103,", JavaStackBehavior.",B103,");")</f>
-        <v>Iconst_5 = new JavaInstruction(JavaOpCode.Iconst_5, "iconst_5", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B104," = new JavaOpCode(JavaOpCodeTag.",Table!B104,", """,Table!A104,""", JavaOperandType.Inline",Table!D104,", JavaFlowControl.",Table!F104,", ",Table!E104,", JavaStackBehavior.",A103,", JavaStackBehavior.",B103,");")</f>
+        <v>Iconst_5 = new JavaOpCode(JavaOpCodeTag.Iconst_5, "iconst_5", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -10132,8 +10129,8 @@
         <v>PushI</v>
       </c>
       <c r="C104" s="1" t="str">
-        <f>CONCATENATE(Table!B105," = new JavaInstruction(JavaOpCode.",Table!B105,", """,Table!A105,""", JavaOperandType.Inline",Table!D105,", JavaFlowControl.",Table!F105,", ",Table!E105,", JavaStackBehavior.",A104,", JavaStackBehavior.",B104,");")</f>
-        <v>Iconst_m1 = new JavaInstruction(JavaOpCode.Iconst_m1, "iconst_m1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B105," = new JavaOpCode(JavaOpCodeTag.",Table!B105,", """,Table!A105,""", JavaOperandType.Inline",Table!D105,", JavaFlowControl.",Table!F105,", ",Table!E105,", JavaStackBehavior.",A104,", JavaStackBehavior.",B104,");")</f>
+        <v>Iconst_m1 = new JavaOpCode(JavaOpCodeTag.Iconst_m1, "iconst_m1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -10146,8 +10143,8 @@
         <v>PushI</v>
       </c>
       <c r="C105" s="1" t="str">
-        <f>CONCATENATE(Table!B106," = new JavaInstruction(JavaOpCode.",Table!B106,", """,Table!A106,""", JavaOperandType.Inline",Table!D106,", JavaFlowControl.",Table!F106,", ",Table!E106,", JavaStackBehavior.",A105,", JavaStackBehavior.",B105,");")</f>
-        <v>Idiv = new JavaInstruction(JavaOpCode.Idiv, "idiv", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI_PopI, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B106," = new JavaOpCode(JavaOpCodeTag.",Table!B106,", """,Table!A106,""", JavaOperandType.Inline",Table!D106,", JavaFlowControl.",Table!F106,", ",Table!E106,", JavaStackBehavior.",A105,", JavaStackBehavior.",B105,");")</f>
+        <v>Idiv = new JavaOpCode(JavaOpCodeTag.Idiv, "idiv", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI_PopI, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -10160,8 +10157,8 @@
         <v>Push0</v>
       </c>
       <c r="C106" s="1" t="str">
-        <f>CONCATENATE(Table!B107," = new JavaInstruction(JavaOpCode.",Table!B107,", """,Table!A107,""", JavaOperandType.Inline",Table!D107,", JavaFlowControl.",Table!F107,", ",Table!E107,", JavaStackBehavior.",A106,", JavaStackBehavior.",B106,");")</f>
-        <v>If_acmpeq = new JavaInstruction(JavaOpCode.If_acmpeq, "if_acmpeq", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopRef_PopRef, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B107," = new JavaOpCode(JavaOpCodeTag.",Table!B107,", """,Table!A107,""", JavaOperandType.Inline",Table!D107,", JavaFlowControl.",Table!F107,", ",Table!E107,", JavaStackBehavior.",A106,", JavaStackBehavior.",B106,");")</f>
+        <v>If_acmpeq = new JavaOpCode(JavaOpCodeTag.If_acmpeq, "if_acmpeq", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopRef_PopRef, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -10174,8 +10171,8 @@
         <v>Push0</v>
       </c>
       <c r="C107" s="1" t="str">
-        <f>CONCATENATE(Table!B108," = new JavaInstruction(JavaOpCode.",Table!B108,", """,Table!A108,""", JavaOperandType.Inline",Table!D108,", JavaFlowControl.",Table!F108,", ",Table!E108,", JavaStackBehavior.",A107,", JavaStackBehavior.",B107,");")</f>
-        <v>If_acmpne = new JavaInstruction(JavaOpCode.If_acmpne, "if_acmpne", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopRef_PopRef, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B108," = new JavaOpCode(JavaOpCodeTag.",Table!B108,", """,Table!A108,""", JavaOperandType.Inline",Table!D108,", JavaFlowControl.",Table!F108,", ",Table!E108,", JavaStackBehavior.",A107,", JavaStackBehavior.",B107,");")</f>
+        <v>If_acmpne = new JavaOpCode(JavaOpCodeTag.If_acmpne, "if_acmpne", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopRef_PopRef, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -10188,8 +10185,8 @@
         <v>Push0</v>
       </c>
       <c r="C108" s="1" t="str">
-        <f>CONCATENATE(Table!B109," = new JavaInstruction(JavaOpCode.",Table!B109,", """,Table!A109,""", JavaOperandType.Inline",Table!D109,", JavaFlowControl.",Table!F109,", ",Table!E109,", JavaStackBehavior.",A108,", JavaStackBehavior.",B108,");")</f>
-        <v>If_icmpeq = new JavaInstruction(JavaOpCode.If_icmpeq, "if_icmpeq", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopI_PopI, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B109," = new JavaOpCode(JavaOpCodeTag.",Table!B109,", """,Table!A109,""", JavaOperandType.Inline",Table!D109,", JavaFlowControl.",Table!F109,", ",Table!E109,", JavaStackBehavior.",A108,", JavaStackBehavior.",B108,");")</f>
+        <v>If_icmpeq = new JavaOpCode(JavaOpCodeTag.If_icmpeq, "if_icmpeq", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopI_PopI, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -10202,8 +10199,8 @@
         <v>Push0</v>
       </c>
       <c r="C109" s="1" t="str">
-        <f>CONCATENATE(Table!B110," = new JavaInstruction(JavaOpCode.",Table!B110,", """,Table!A110,""", JavaOperandType.Inline",Table!D110,", JavaFlowControl.",Table!F110,", ",Table!E110,", JavaStackBehavior.",A109,", JavaStackBehavior.",B109,");")</f>
-        <v>If_icmpge = new JavaInstruction(JavaOpCode.If_icmpge, "if_icmpge", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopI_PopI, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B110," = new JavaOpCode(JavaOpCodeTag.",Table!B110,", """,Table!A110,""", JavaOperandType.Inline",Table!D110,", JavaFlowControl.",Table!F110,", ",Table!E110,", JavaStackBehavior.",A109,", JavaStackBehavior.",B109,");")</f>
+        <v>If_icmpge = new JavaOpCode(JavaOpCodeTag.If_icmpge, "if_icmpge", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopI_PopI, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -10216,8 +10213,8 @@
         <v>Push0</v>
       </c>
       <c r="C110" s="1" t="str">
-        <f>CONCATENATE(Table!B111," = new JavaInstruction(JavaOpCode.",Table!B111,", """,Table!A111,""", JavaOperandType.Inline",Table!D111,", JavaFlowControl.",Table!F111,", ",Table!E111,", JavaStackBehavior.",A110,", JavaStackBehavior.",B110,");")</f>
-        <v>If_icmpgt = new JavaInstruction(JavaOpCode.If_icmpgt, "if_icmpgt", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopI_PopI, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B111," = new JavaOpCode(JavaOpCodeTag.",Table!B111,", """,Table!A111,""", JavaOperandType.Inline",Table!D111,", JavaFlowControl.",Table!F111,", ",Table!E111,", JavaStackBehavior.",A110,", JavaStackBehavior.",B110,");")</f>
+        <v>If_icmpgt = new JavaOpCode(JavaOpCodeTag.If_icmpgt, "if_icmpgt", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopI_PopI, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -10230,8 +10227,8 @@
         <v>Push0</v>
       </c>
       <c r="C111" s="1" t="str">
-        <f>CONCATENATE(Table!B112," = new JavaInstruction(JavaOpCode.",Table!B112,", """,Table!A112,""", JavaOperandType.Inline",Table!D112,", JavaFlowControl.",Table!F112,", ",Table!E112,", JavaStackBehavior.",A111,", JavaStackBehavior.",B111,");")</f>
-        <v>If_icmple = new JavaInstruction(JavaOpCode.If_icmple, "if_icmple", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopI_PopI, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B112," = new JavaOpCode(JavaOpCodeTag.",Table!B112,", """,Table!A112,""", JavaOperandType.Inline",Table!D112,", JavaFlowControl.",Table!F112,", ",Table!E112,", JavaStackBehavior.",A111,", JavaStackBehavior.",B111,");")</f>
+        <v>If_icmple = new JavaOpCode(JavaOpCodeTag.If_icmple, "if_icmple", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopI_PopI, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -10244,8 +10241,8 @@
         <v>Push0</v>
       </c>
       <c r="C112" s="1" t="str">
-        <f>CONCATENATE(Table!B113," = new JavaInstruction(JavaOpCode.",Table!B113,", """,Table!A113,""", JavaOperandType.Inline",Table!D113,", JavaFlowControl.",Table!F113,", ",Table!E113,", JavaStackBehavior.",A112,", JavaStackBehavior.",B112,");")</f>
-        <v>If_icmplt = new JavaInstruction(JavaOpCode.If_icmplt, "if_icmplt", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopI_PopI, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B113," = new JavaOpCode(JavaOpCodeTag.",Table!B113,", """,Table!A113,""", JavaOperandType.Inline",Table!D113,", JavaFlowControl.",Table!F113,", ",Table!E113,", JavaStackBehavior.",A112,", JavaStackBehavior.",B112,");")</f>
+        <v>If_icmplt = new JavaOpCode(JavaOpCodeTag.If_icmplt, "if_icmplt", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopI_PopI, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -10258,8 +10255,8 @@
         <v>Push0</v>
       </c>
       <c r="C113" s="1" t="str">
-        <f>CONCATENATE(Table!B114," = new JavaInstruction(JavaOpCode.",Table!B114,", """,Table!A114,""", JavaOperandType.Inline",Table!D114,", JavaFlowControl.",Table!F114,", ",Table!E114,", JavaStackBehavior.",A113,", JavaStackBehavior.",B113,");")</f>
-        <v>If_icmpne = new JavaInstruction(JavaOpCode.If_icmpne, "if_icmpne", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopI_PopI, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B114," = new JavaOpCode(JavaOpCodeTag.",Table!B114,", """,Table!A114,""", JavaOperandType.Inline",Table!D114,", JavaFlowControl.",Table!F114,", ",Table!E114,", JavaStackBehavior.",A113,", JavaStackBehavior.",B113,");")</f>
+        <v>If_icmpne = new JavaOpCode(JavaOpCodeTag.If_icmpne, "if_icmpne", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopI_PopI, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -10272,8 +10269,8 @@
         <v>Push0</v>
       </c>
       <c r="C114" s="1" t="str">
-        <f>CONCATENATE(Table!B115," = new JavaInstruction(JavaOpCode.",Table!B115,", """,Table!A115,""", JavaOperandType.Inline",Table!D115,", JavaFlowControl.",Table!F115,", ",Table!E115,", JavaStackBehavior.",A114,", JavaStackBehavior.",B114,");")</f>
-        <v>Ifeq = new JavaInstruction(JavaOpCode.Ifeq, "ifeq", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopI, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B115," = new JavaOpCode(JavaOpCodeTag.",Table!B115,", """,Table!A115,""", JavaOperandType.Inline",Table!D115,", JavaFlowControl.",Table!F115,", ",Table!E115,", JavaStackBehavior.",A114,", JavaStackBehavior.",B114,");")</f>
+        <v>Ifeq = new JavaOpCode(JavaOpCodeTag.Ifeq, "ifeq", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopI, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -10286,8 +10283,8 @@
         <v>Push0</v>
       </c>
       <c r="C115" s="1" t="str">
-        <f>CONCATENATE(Table!B116," = new JavaInstruction(JavaOpCode.",Table!B116,", """,Table!A116,""", JavaOperandType.Inline",Table!D116,", JavaFlowControl.",Table!F116,", ",Table!E116,", JavaStackBehavior.",A115,", JavaStackBehavior.",B115,");")</f>
-        <v>Ifge = new JavaInstruction(JavaOpCode.Ifge, "ifge", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopI, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B116," = new JavaOpCode(JavaOpCodeTag.",Table!B116,", """,Table!A116,""", JavaOperandType.Inline",Table!D116,", JavaFlowControl.",Table!F116,", ",Table!E116,", JavaStackBehavior.",A115,", JavaStackBehavior.",B115,");")</f>
+        <v>Ifge = new JavaOpCode(JavaOpCodeTag.Ifge, "ifge", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopI, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -10300,8 +10297,8 @@
         <v>Push0</v>
       </c>
       <c r="C116" s="1" t="str">
-        <f>CONCATENATE(Table!B117," = new JavaInstruction(JavaOpCode.",Table!B117,", """,Table!A117,""", JavaOperandType.Inline",Table!D117,", JavaFlowControl.",Table!F117,", ",Table!E117,", JavaStackBehavior.",A116,", JavaStackBehavior.",B116,");")</f>
-        <v>Ifgt = new JavaInstruction(JavaOpCode.Ifgt, "ifgt", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopI, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B117," = new JavaOpCode(JavaOpCodeTag.",Table!B117,", """,Table!A117,""", JavaOperandType.Inline",Table!D117,", JavaFlowControl.",Table!F117,", ",Table!E117,", JavaStackBehavior.",A116,", JavaStackBehavior.",B116,");")</f>
+        <v>Ifgt = new JavaOpCode(JavaOpCodeTag.Ifgt, "ifgt", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopI, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -10314,8 +10311,8 @@
         <v>Push0</v>
       </c>
       <c r="C117" s="1" t="str">
-        <f>CONCATENATE(Table!B118," = new JavaInstruction(JavaOpCode.",Table!B118,", """,Table!A118,""", JavaOperandType.Inline",Table!D118,", JavaFlowControl.",Table!F118,", ",Table!E118,", JavaStackBehavior.",A117,", JavaStackBehavior.",B117,");")</f>
-        <v>Ifle = new JavaInstruction(JavaOpCode.Ifle, "ifle", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopI, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B118," = new JavaOpCode(JavaOpCodeTag.",Table!B118,", """,Table!A118,""", JavaOperandType.Inline",Table!D118,", JavaFlowControl.",Table!F118,", ",Table!E118,", JavaStackBehavior.",A117,", JavaStackBehavior.",B117,");")</f>
+        <v>Ifle = new JavaOpCode(JavaOpCodeTag.Ifle, "ifle", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopI, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -10328,8 +10325,8 @@
         <v>Push0</v>
       </c>
       <c r="C118" s="1" t="str">
-        <f>CONCATENATE(Table!B119," = new JavaInstruction(JavaOpCode.",Table!B119,", """,Table!A119,""", JavaOperandType.Inline",Table!D119,", JavaFlowControl.",Table!F119,", ",Table!E119,", JavaStackBehavior.",A118,", JavaStackBehavior.",B118,");")</f>
-        <v>Iflt = new JavaInstruction(JavaOpCode.Iflt, "iflt", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopI, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B119," = new JavaOpCode(JavaOpCodeTag.",Table!B119,", """,Table!A119,""", JavaOperandType.Inline",Table!D119,", JavaFlowControl.",Table!F119,", ",Table!E119,", JavaStackBehavior.",A118,", JavaStackBehavior.",B118,");")</f>
+        <v>Iflt = new JavaOpCode(JavaOpCodeTag.Iflt, "iflt", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopI, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -10342,8 +10339,8 @@
         <v>Push0</v>
       </c>
       <c r="C119" s="1" t="str">
-        <f>CONCATENATE(Table!B120," = new JavaInstruction(JavaOpCode.",Table!B120,", """,Table!A120,""", JavaOperandType.Inline",Table!D120,", JavaFlowControl.",Table!F120,", ",Table!E120,", JavaStackBehavior.",A119,", JavaStackBehavior.",B119,");")</f>
-        <v>Ifne = new JavaInstruction(JavaOpCode.Ifne, "ifne", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopI, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B120," = new JavaOpCode(JavaOpCodeTag.",Table!B120,", """,Table!A120,""", JavaOperandType.Inline",Table!D120,", JavaFlowControl.",Table!F120,", ",Table!E120,", JavaStackBehavior.",A119,", JavaStackBehavior.",B119,");")</f>
+        <v>Ifne = new JavaOpCode(JavaOpCodeTag.Ifne, "ifne", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopI, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -10356,8 +10353,8 @@
         <v>Push0</v>
       </c>
       <c r="C120" s="1" t="str">
-        <f>CONCATENATE(Table!B121," = new JavaInstruction(JavaOpCode.",Table!B121,", """,Table!A121,""", JavaOperandType.Inline",Table!D121,", JavaFlowControl.",Table!F121,", ",Table!E121,", JavaStackBehavior.",A120,", JavaStackBehavior.",B120,");")</f>
-        <v>Ifnonnull = new JavaInstruction(JavaOpCode.Ifnonnull, "ifnonnull", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopRef, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B121," = new JavaOpCode(JavaOpCodeTag.",Table!B121,", """,Table!A121,""", JavaOperandType.Inline",Table!D121,", JavaFlowControl.",Table!F121,", ",Table!E121,", JavaStackBehavior.",A120,", JavaStackBehavior.",B120,");")</f>
+        <v>Ifnonnull = new JavaOpCode(JavaOpCodeTag.Ifnonnull, "ifnonnull", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopRef, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -10370,8 +10367,8 @@
         <v>Push0</v>
       </c>
       <c r="C121" s="1" t="str">
-        <f>CONCATENATE(Table!B122," = new JavaInstruction(JavaOpCode.",Table!B122,", """,Table!A122,""", JavaOperandType.Inline",Table!D122,", JavaFlowControl.",Table!F122,", ",Table!E122,", JavaStackBehavior.",A121,", JavaStackBehavior.",B121,");")</f>
-        <v>Ifnull = new JavaInstruction(JavaOpCode.Ifnull, "ifnull", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopRef, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B122," = new JavaOpCode(JavaOpCodeTag.",Table!B122,", """,Table!A122,""", JavaOperandType.Inline",Table!D122,", JavaFlowControl.",Table!F122,", ",Table!E122,", JavaStackBehavior.",A121,", JavaStackBehavior.",B121,");")</f>
+        <v>Ifnull = new JavaOpCode(JavaOpCodeTag.Ifnull, "ifnull", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.ConditionalBranch, 3, JavaStackBehavior.PopRef, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -10384,8 +10381,8 @@
         <v>Push0</v>
       </c>
       <c r="C122" s="1" t="str">
-        <f>CONCATENATE(Table!B123," = new JavaInstruction(JavaOpCode.",Table!B123,", """,Table!A123,""", JavaOperandType.Inline",Table!D123,", JavaFlowControl.",Table!F123,", ",Table!E123,", JavaStackBehavior.",A122,", JavaStackBehavior.",B122,");")</f>
-        <v>Iinc = new JavaInstruction(JavaOpCode.Iinc, "iinc", JavaOperandType.InlineVar_I1, JavaFlowControl.Next, 3, JavaStackBehavior.Pop0, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B123," = new JavaOpCode(JavaOpCodeTag.",Table!B123,", """,Table!A123,""", JavaOperandType.Inline",Table!D123,", JavaFlowControl.",Table!F123,", ",Table!E123,", JavaStackBehavior.",A122,", JavaStackBehavior.",B122,");")</f>
+        <v>Iinc = new JavaOpCode(JavaOpCodeTag.Iinc, "iinc", JavaOperandType.InlineVar_I1, JavaFlowControl.Next, 3, JavaStackBehavior.Pop0, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -10398,8 +10395,8 @@
         <v>PushI</v>
       </c>
       <c r="C123" s="1" t="str">
-        <f>CONCATENATE(Table!B124," = new JavaInstruction(JavaOpCode.",Table!B124,", """,Table!A124,""", JavaOperandType.Inline",Table!D124,", JavaFlowControl.",Table!F124,", ",Table!E124,", JavaStackBehavior.",A123,", JavaStackBehavior.",B123,");")</f>
-        <v>Iload = new JavaInstruction(JavaOpCode.Iload, "iload", JavaOperandType.InlineVar, JavaFlowControl.Next, 2, JavaStackBehavior.Pop0, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B124," = new JavaOpCode(JavaOpCodeTag.",Table!B124,", """,Table!A124,""", JavaOperandType.Inline",Table!D124,", JavaFlowControl.",Table!F124,", ",Table!E124,", JavaStackBehavior.",A123,", JavaStackBehavior.",B123,");")</f>
+        <v>Iload = new JavaOpCode(JavaOpCodeTag.Iload, "iload", JavaOperandType.InlineVar, JavaFlowControl.Next, 2, JavaStackBehavior.Pop0, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -10412,8 +10409,8 @@
         <v>PushI</v>
       </c>
       <c r="C124" s="1" t="str">
-        <f>CONCATENATE(Table!B125," = new JavaInstruction(JavaOpCode.",Table!B125,", """,Table!A125,""", JavaOperandType.Inline",Table!D125,", JavaFlowControl.",Table!F125,", ",Table!E125,", JavaStackBehavior.",A124,", JavaStackBehavior.",B124,");")</f>
-        <v>Iload_0 = new JavaInstruction(JavaOpCode.Iload_0, "iload_0", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B125," = new JavaOpCode(JavaOpCodeTag.",Table!B125,", """,Table!A125,""", JavaOperandType.Inline",Table!D125,", JavaFlowControl.",Table!F125,", ",Table!E125,", JavaStackBehavior.",A124,", JavaStackBehavior.",B124,");")</f>
+        <v>Iload_0 = new JavaOpCode(JavaOpCodeTag.Iload_0, "iload_0", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -10426,8 +10423,8 @@
         <v>PushI</v>
       </c>
       <c r="C125" s="1" t="str">
-        <f>CONCATENATE(Table!B126," = new JavaInstruction(JavaOpCode.",Table!B126,", """,Table!A126,""", JavaOperandType.Inline",Table!D126,", JavaFlowControl.",Table!F126,", ",Table!E126,", JavaStackBehavior.",A125,", JavaStackBehavior.",B125,");")</f>
-        <v>Iload_1 = new JavaInstruction(JavaOpCode.Iload_1, "iload_1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B126," = new JavaOpCode(JavaOpCodeTag.",Table!B126,", """,Table!A126,""", JavaOperandType.Inline",Table!D126,", JavaFlowControl.",Table!F126,", ",Table!E126,", JavaStackBehavior.",A125,", JavaStackBehavior.",B125,");")</f>
+        <v>Iload_1 = new JavaOpCode(JavaOpCodeTag.Iload_1, "iload_1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -10440,8 +10437,8 @@
         <v>PushI</v>
       </c>
       <c r="C126" s="1" t="str">
-        <f>CONCATENATE(Table!B127," = new JavaInstruction(JavaOpCode.",Table!B127,", """,Table!A127,""", JavaOperandType.Inline",Table!D127,", JavaFlowControl.",Table!F127,", ",Table!E127,", JavaStackBehavior.",A126,", JavaStackBehavior.",B126,");")</f>
-        <v>Iload_2 = new JavaInstruction(JavaOpCode.Iload_2, "iload_2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B127," = new JavaOpCode(JavaOpCodeTag.",Table!B127,", """,Table!A127,""", JavaOperandType.Inline",Table!D127,", JavaFlowControl.",Table!F127,", ",Table!E127,", JavaStackBehavior.",A126,", JavaStackBehavior.",B126,");")</f>
+        <v>Iload_2 = new JavaOpCode(JavaOpCodeTag.Iload_2, "iload_2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -10454,8 +10451,8 @@
         <v>PushI</v>
       </c>
       <c r="C127" s="1" t="str">
-        <f>CONCATENATE(Table!B128," = new JavaInstruction(JavaOpCode.",Table!B128,", """,Table!A128,""", JavaOperandType.Inline",Table!D128,", JavaFlowControl.",Table!F128,", ",Table!E128,", JavaStackBehavior.",A127,", JavaStackBehavior.",B127,");")</f>
-        <v>Iload_3 = new JavaInstruction(JavaOpCode.Iload_3, "iload_3", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B128," = new JavaOpCode(JavaOpCodeTag.",Table!B128,", """,Table!A128,""", JavaOperandType.Inline",Table!D128,", JavaFlowControl.",Table!F128,", ",Table!E128,", JavaStackBehavior.",A127,", JavaStackBehavior.",B127,");")</f>
+        <v>Iload_3 = new JavaOpCode(JavaOpCodeTag.Iload_3, "iload_3", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -10468,8 +10465,8 @@
         <v>Push0</v>
       </c>
       <c r="C128" s="1" t="str">
-        <f>CONCATENATE(Table!B129," = new JavaInstruction(JavaOpCode.",Table!B129,", """,Table!A129,""", JavaOperandType.Inline",Table!D129,", JavaFlowControl.",Table!F129,", ",Table!E129,", JavaStackBehavior.",A128,", JavaStackBehavior.",B128,");")</f>
-        <v>Impdep1 = new JavaInstruction(JavaOpCode.Impdep1, "impdep1", JavaOperandType.InlineNone, JavaFlowControl.Special, 1, JavaStackBehavior.Pop0, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B129," = new JavaOpCode(JavaOpCodeTag.",Table!B129,", """,Table!A129,""", JavaOperandType.Inline",Table!D129,", JavaFlowControl.",Table!F129,", ",Table!E129,", JavaStackBehavior.",A128,", JavaStackBehavior.",B128,");")</f>
+        <v>Impdep1 = new JavaOpCode(JavaOpCodeTag.Impdep1, "impdep1", JavaOperandType.InlineNone, JavaFlowControl.Special, 1, JavaStackBehavior.Pop0, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -10482,8 +10479,8 @@
         <v>Push0</v>
       </c>
       <c r="C129" s="1" t="str">
-        <f>CONCATENATE(Table!B130," = new JavaInstruction(JavaOpCode.",Table!B130,", """,Table!A130,""", JavaOperandType.Inline",Table!D130,", JavaFlowControl.",Table!F130,", ",Table!E130,", JavaStackBehavior.",A129,", JavaStackBehavior.",B129,");")</f>
-        <v>Impdep2 = new JavaInstruction(JavaOpCode.Impdep2, "impdep2", JavaOperandType.InlineNone, JavaFlowControl.Special, 1, JavaStackBehavior.Pop0, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B130," = new JavaOpCode(JavaOpCodeTag.",Table!B130,", """,Table!A130,""", JavaOperandType.Inline",Table!D130,", JavaFlowControl.",Table!F130,", ",Table!E130,", JavaStackBehavior.",A129,", JavaStackBehavior.",B129,");")</f>
+        <v>Impdep2 = new JavaOpCode(JavaOpCodeTag.Impdep2, "impdep2", JavaOperandType.InlineNone, JavaFlowControl.Special, 1, JavaStackBehavior.Pop0, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -10496,8 +10493,8 @@
         <v>PushI</v>
       </c>
       <c r="C130" s="1" t="str">
-        <f>CONCATENATE(Table!B131," = new JavaInstruction(JavaOpCode.",Table!B131,", """,Table!A131,""", JavaOperandType.Inline",Table!D131,", JavaFlowControl.",Table!F131,", ",Table!E131,", JavaStackBehavior.",A130,", JavaStackBehavior.",B130,");")</f>
-        <v>Imul = new JavaInstruction(JavaOpCode.Imul, "imul", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI_PopI, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B131," = new JavaOpCode(JavaOpCodeTag.",Table!B131,", """,Table!A131,""", JavaOperandType.Inline",Table!D131,", JavaFlowControl.",Table!F131,", ",Table!E131,", JavaStackBehavior.",A130,", JavaStackBehavior.",B130,");")</f>
+        <v>Imul = new JavaOpCode(JavaOpCodeTag.Imul, "imul", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI_PopI, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -10510,8 +10507,8 @@
         <v>PushI</v>
       </c>
       <c r="C131" s="1" t="str">
-        <f>CONCATENATE(Table!B132," = new JavaInstruction(JavaOpCode.",Table!B132,", """,Table!A132,""", JavaOperandType.Inline",Table!D132,", JavaFlowControl.",Table!F132,", ",Table!E132,", JavaStackBehavior.",A131,", JavaStackBehavior.",B131,");")</f>
-        <v>Ineg = new JavaInstruction(JavaOpCode.Ineg, "ineg", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B132," = new JavaOpCode(JavaOpCodeTag.",Table!B132,", """,Table!A132,""", JavaOperandType.Inline",Table!D132,", JavaFlowControl.",Table!F132,", ",Table!E132,", JavaStackBehavior.",A131,", JavaStackBehavior.",B131,");")</f>
+        <v>Ineg = new JavaOpCode(JavaOpCodeTag.Ineg, "ineg", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -10524,8 +10521,8 @@
         <v>PushI</v>
       </c>
       <c r="C132" s="1" t="str">
-        <f>CONCATENATE(Table!B133," = new JavaInstruction(JavaOpCode.",Table!B133,", """,Table!A133,""", JavaOperandType.Inline",Table!D133,", JavaFlowControl.",Table!F133,", ",Table!E133,", JavaStackBehavior.",A132,", JavaStackBehavior.",B132,");")</f>
-        <v>Instanceof = new JavaInstruction(JavaOpCode.Instanceof, "instanceof", JavaOperandType.InlineType, JavaFlowControl.Next, 3, JavaStackBehavior.PopRef, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B133," = new JavaOpCode(JavaOpCodeTag.",Table!B133,", """,Table!A133,""", JavaOperandType.Inline",Table!D133,", JavaFlowControl.",Table!F133,", ",Table!E133,", JavaStackBehavior.",A132,", JavaStackBehavior.",B132,");")</f>
+        <v>Instanceof = new JavaOpCode(JavaOpCodeTag.Instanceof, "instanceof", JavaOperandType.InlineType, JavaFlowControl.Next, 3, JavaStackBehavior.PopRef, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -10538,8 +10535,8 @@
         <v>PushVar</v>
       </c>
       <c r="C133" s="1" t="str">
-        <f>CONCATENATE(Table!B134," = new JavaInstruction(JavaOpCode.",Table!B134,", """,Table!A134,""", JavaOperandType.Inline",Table!D134,", JavaFlowControl.",Table!F134,", ",Table!E134,", JavaStackBehavior.",A133,", JavaStackBehavior.",B133,");")</f>
-        <v>Invokeinterface = new JavaInstruction(JavaOpCode.Invokeinterface, "invokeinterface", JavaOperandType.InlineMethod_I1_0, JavaFlowControl.Call, 5, JavaStackBehavior.PopVar, JavaStackBehavior.PushVar);</v>
+        <f>CONCATENATE(Table!B134," = new JavaOpCode(JavaOpCodeTag.",Table!B134,", """,Table!A134,""", JavaOperandType.Inline",Table!D134,", JavaFlowControl.",Table!F134,", ",Table!E134,", JavaStackBehavior.",A133,", JavaStackBehavior.",B133,");")</f>
+        <v>Invokeinterface = new JavaOpCode(JavaOpCodeTag.Invokeinterface, "invokeinterface", JavaOperandType.InlineMethod_U1_0, JavaFlowControl.Call, 5, JavaStackBehavior.PopVar, JavaStackBehavior.PushVar);</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -10552,8 +10549,8 @@
         <v>PushVar</v>
       </c>
       <c r="C134" s="1" t="str">
-        <f>CONCATENATE(Table!B135," = new JavaInstruction(JavaOpCode.",Table!B135,", """,Table!A135,""", JavaOperandType.Inline",Table!D135,", JavaFlowControl.",Table!F135,", ",Table!E135,", JavaStackBehavior.",A134,", JavaStackBehavior.",B134,");")</f>
-        <v>Invokespecial = new JavaInstruction(JavaOpCode.Invokespecial, "invokespecial", JavaOperandType.InlineMethod, JavaFlowControl.Call, 3, JavaStackBehavior.PopVar, JavaStackBehavior.PushVar);</v>
+        <f>CONCATENATE(Table!B135," = new JavaOpCode(JavaOpCodeTag.",Table!B135,", """,Table!A135,""", JavaOperandType.Inline",Table!D135,", JavaFlowControl.",Table!F135,", ",Table!E135,", JavaStackBehavior.",A134,", JavaStackBehavior.",B134,");")</f>
+        <v>Invokespecial = new JavaOpCode(JavaOpCodeTag.Invokespecial, "invokespecial", JavaOperandType.InlineMethod, JavaFlowControl.Call, 3, JavaStackBehavior.PopVar, JavaStackBehavior.PushVar);</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -10566,8 +10563,8 @@
         <v>PushVar</v>
       </c>
       <c r="C135" s="1" t="str">
-        <f>CONCATENATE(Table!B136," = new JavaInstruction(JavaOpCode.",Table!B136,", """,Table!A136,""", JavaOperandType.Inline",Table!D136,", JavaFlowControl.",Table!F136,", ",Table!E136,", JavaStackBehavior.",A135,", JavaStackBehavior.",B135,");")</f>
-        <v>Invokestatic = new JavaInstruction(JavaOpCode.Invokestatic, "invokestatic", JavaOperandType.InlineMethod, JavaFlowControl.Call, 3, JavaStackBehavior.PopVar, JavaStackBehavior.PushVar);</v>
+        <f>CONCATENATE(Table!B136," = new JavaOpCode(JavaOpCodeTag.",Table!B136,", """,Table!A136,""", JavaOperandType.Inline",Table!D136,", JavaFlowControl.",Table!F136,", ",Table!E136,", JavaStackBehavior.",A135,", JavaStackBehavior.",B135,");")</f>
+        <v>Invokestatic = new JavaOpCode(JavaOpCodeTag.Invokestatic, "invokestatic", JavaOperandType.InlineMethod, JavaFlowControl.Call, 3, JavaStackBehavior.PopVar, JavaStackBehavior.PushVar);</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -10580,8 +10577,8 @@
         <v>PushVar</v>
       </c>
       <c r="C136" s="1" t="str">
-        <f>CONCATENATE(Table!B137," = new JavaInstruction(JavaOpCode.",Table!B137,", """,Table!A137,""", JavaOperandType.Inline",Table!D137,", JavaFlowControl.",Table!F137,", ",Table!E137,", JavaStackBehavior.",A136,", JavaStackBehavior.",B136,");")</f>
-        <v>Invokevirtual = new JavaInstruction(JavaOpCode.Invokevirtual, "invokevirtual", JavaOperandType.InlineMethod, JavaFlowControl.Call, 3, JavaStackBehavior.PopVar, JavaStackBehavior.PushVar);</v>
+        <f>CONCATENATE(Table!B137," = new JavaOpCode(JavaOpCodeTag.",Table!B137,", """,Table!A137,""", JavaOperandType.Inline",Table!D137,", JavaFlowControl.",Table!F137,", ",Table!E137,", JavaStackBehavior.",A136,", JavaStackBehavior.",B136,");")</f>
+        <v>Invokevirtual = new JavaOpCode(JavaOpCodeTag.Invokevirtual, "invokevirtual", JavaOperandType.InlineMethod, JavaFlowControl.Call, 3, JavaStackBehavior.PopVar, JavaStackBehavior.PushVar);</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -10594,8 +10591,8 @@
         <v>PushI</v>
       </c>
       <c r="C137" s="1" t="str">
-        <f>CONCATENATE(Table!B138," = new JavaInstruction(JavaOpCode.",Table!B138,", """,Table!A138,""", JavaOperandType.Inline",Table!D138,", JavaFlowControl.",Table!F138,", ",Table!E138,", JavaStackBehavior.",A137,", JavaStackBehavior.",B137,");")</f>
-        <v>Ior = new JavaInstruction(JavaOpCode.Ior, "ior", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI_PopI, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B138," = new JavaOpCode(JavaOpCodeTag.",Table!B138,", """,Table!A138,""", JavaOperandType.Inline",Table!D138,", JavaFlowControl.",Table!F138,", ",Table!E138,", JavaStackBehavior.",A137,", JavaStackBehavior.",B137,");")</f>
+        <v>Ior = new JavaOpCode(JavaOpCodeTag.Ior, "ior", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI_PopI, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -10608,8 +10605,8 @@
         <v>PushI</v>
       </c>
       <c r="C138" s="1" t="str">
-        <f>CONCATENATE(Table!B139," = new JavaInstruction(JavaOpCode.",Table!B139,", """,Table!A139,""", JavaOperandType.Inline",Table!D139,", JavaFlowControl.",Table!F139,", ",Table!E139,", JavaStackBehavior.",A138,", JavaStackBehavior.",B138,");")</f>
-        <v>Irem = new JavaInstruction(JavaOpCode.Irem, "irem", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI_PopI, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B139," = new JavaOpCode(JavaOpCodeTag.",Table!B139,", """,Table!A139,""", JavaOperandType.Inline",Table!D139,", JavaFlowControl.",Table!F139,", ",Table!E139,", JavaStackBehavior.",A138,", JavaStackBehavior.",B138,");")</f>
+        <v>Irem = new JavaOpCode(JavaOpCodeTag.Irem, "irem", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI_PopI, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -10622,8 +10619,8 @@
         <v>Push0</v>
       </c>
       <c r="C139" s="1" t="str">
-        <f>CONCATENATE(Table!B140," = new JavaInstruction(JavaOpCode.",Table!B140,", """,Table!A140,""", JavaOperandType.Inline",Table!D140,", JavaFlowControl.",Table!F140,", ",Table!E140,", JavaStackBehavior.",A139,", JavaStackBehavior.",B139,");")</f>
-        <v>Ireturn = new JavaInstruction(JavaOpCode.Ireturn, "ireturn", JavaOperandType.InlineNone, JavaFlowControl.Return, 1, JavaStackBehavior.PopI, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B140," = new JavaOpCode(JavaOpCodeTag.",Table!B140,", """,Table!A140,""", JavaOperandType.Inline",Table!D140,", JavaFlowControl.",Table!F140,", ",Table!E140,", JavaStackBehavior.",A139,", JavaStackBehavior.",B139,");")</f>
+        <v>Ireturn = new JavaOpCode(JavaOpCodeTag.Ireturn, "ireturn", JavaOperandType.InlineNone, JavaFlowControl.Return, 1, JavaStackBehavior.PopI, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -10636,8 +10633,8 @@
         <v>PushI</v>
       </c>
       <c r="C140" s="1" t="str">
-        <f>CONCATENATE(Table!B141," = new JavaInstruction(JavaOpCode.",Table!B141,", """,Table!A141,""", JavaOperandType.Inline",Table!D141,", JavaFlowControl.",Table!F141,", ",Table!E141,", JavaStackBehavior.",A140,", JavaStackBehavior.",B140,");")</f>
-        <v>Ishl = new JavaInstruction(JavaOpCode.Ishl, "ishl", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI_PopI, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B141," = new JavaOpCode(JavaOpCodeTag.",Table!B141,", """,Table!A141,""", JavaOperandType.Inline",Table!D141,", JavaFlowControl.",Table!F141,", ",Table!E141,", JavaStackBehavior.",A140,", JavaStackBehavior.",B140,");")</f>
+        <v>Ishl = new JavaOpCode(JavaOpCodeTag.Ishl, "ishl", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI_PopI, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -10650,8 +10647,8 @@
         <v>PushI</v>
       </c>
       <c r="C141" s="1" t="str">
-        <f>CONCATENATE(Table!B142," = new JavaInstruction(JavaOpCode.",Table!B142,", """,Table!A142,""", JavaOperandType.Inline",Table!D142,", JavaFlowControl.",Table!F142,", ",Table!E142,", JavaStackBehavior.",A141,", JavaStackBehavior.",B141,");")</f>
-        <v>Ishr = new JavaInstruction(JavaOpCode.Ishr, "ishr", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI_PopI, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B142," = new JavaOpCode(JavaOpCodeTag.",Table!B142,", """,Table!A142,""", JavaOperandType.Inline",Table!D142,", JavaFlowControl.",Table!F142,", ",Table!E142,", JavaStackBehavior.",A141,", JavaStackBehavior.",B141,");")</f>
+        <v>Ishr = new JavaOpCode(JavaOpCodeTag.Ishr, "ishr", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI_PopI, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -10664,8 +10661,8 @@
         <v>Push0</v>
       </c>
       <c r="C142" s="1" t="str">
-        <f>CONCATENATE(Table!B143," = new JavaInstruction(JavaOpCode.",Table!B143,", """,Table!A143,""", JavaOperandType.Inline",Table!D143,", JavaFlowControl.",Table!F143,", ",Table!E143,", JavaStackBehavior.",A142,", JavaStackBehavior.",B142,");")</f>
-        <v>Istore = new JavaInstruction(JavaOpCode.Istore, "istore", JavaOperandType.InlineVar, JavaFlowControl.Next, 2, JavaStackBehavior.PopI, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B143," = new JavaOpCode(JavaOpCodeTag.",Table!B143,", """,Table!A143,""", JavaOperandType.Inline",Table!D143,", JavaFlowControl.",Table!F143,", ",Table!E143,", JavaStackBehavior.",A142,", JavaStackBehavior.",B142,");")</f>
+        <v>Istore = new JavaOpCode(JavaOpCodeTag.Istore, "istore", JavaOperandType.InlineVar, JavaFlowControl.Next, 2, JavaStackBehavior.PopI, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -10678,8 +10675,8 @@
         <v>Push0</v>
       </c>
       <c r="C143" s="1" t="str">
-        <f>CONCATENATE(Table!B144," = new JavaInstruction(JavaOpCode.",Table!B144,", """,Table!A144,""", JavaOperandType.Inline",Table!D144,", JavaFlowControl.",Table!F144,", ",Table!E144,", JavaStackBehavior.",A143,", JavaStackBehavior.",B143,");")</f>
-        <v>Istore_0 = new JavaInstruction(JavaOpCode.Istore_0, "istore_0", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B144," = new JavaOpCode(JavaOpCodeTag.",Table!B144,", """,Table!A144,""", JavaOperandType.Inline",Table!D144,", JavaFlowControl.",Table!F144,", ",Table!E144,", JavaStackBehavior.",A143,", JavaStackBehavior.",B143,");")</f>
+        <v>Istore_0 = new JavaOpCode(JavaOpCodeTag.Istore_0, "istore_0", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -10692,8 +10689,8 @@
         <v>Push0</v>
       </c>
       <c r="C144" s="1" t="str">
-        <f>CONCATENATE(Table!B145," = new JavaInstruction(JavaOpCode.",Table!B145,", """,Table!A145,""", JavaOperandType.Inline",Table!D145,", JavaFlowControl.",Table!F145,", ",Table!E145,", JavaStackBehavior.",A144,", JavaStackBehavior.",B144,");")</f>
-        <v>Istore_1 = new JavaInstruction(JavaOpCode.Istore_1, "istore_1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B145," = new JavaOpCode(JavaOpCodeTag.",Table!B145,", """,Table!A145,""", JavaOperandType.Inline",Table!D145,", JavaFlowControl.",Table!F145,", ",Table!E145,", JavaStackBehavior.",A144,", JavaStackBehavior.",B144,");")</f>
+        <v>Istore_1 = new JavaOpCode(JavaOpCodeTag.Istore_1, "istore_1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -10706,8 +10703,8 @@
         <v>Push0</v>
       </c>
       <c r="C145" s="1" t="str">
-        <f>CONCATENATE(Table!B146," = new JavaInstruction(JavaOpCode.",Table!B146,", """,Table!A146,""", JavaOperandType.Inline",Table!D146,", JavaFlowControl.",Table!F146,", ",Table!E146,", JavaStackBehavior.",A145,", JavaStackBehavior.",B145,");")</f>
-        <v>Istore_2 = new JavaInstruction(JavaOpCode.Istore_2, "istore_2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B146," = new JavaOpCode(JavaOpCodeTag.",Table!B146,", """,Table!A146,""", JavaOperandType.Inline",Table!D146,", JavaFlowControl.",Table!F146,", ",Table!E146,", JavaStackBehavior.",A145,", JavaStackBehavior.",B145,");")</f>
+        <v>Istore_2 = new JavaOpCode(JavaOpCodeTag.Istore_2, "istore_2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -10720,8 +10717,8 @@
         <v>Push0</v>
       </c>
       <c r="C146" s="1" t="str">
-        <f>CONCATENATE(Table!B147," = new JavaInstruction(JavaOpCode.",Table!B147,", """,Table!A147,""", JavaOperandType.Inline",Table!D147,", JavaFlowControl.",Table!F147,", ",Table!E147,", JavaStackBehavior.",A146,", JavaStackBehavior.",B146,");")</f>
-        <v>Istore_3 = new JavaInstruction(JavaOpCode.Istore_3, "istore_3", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B147," = new JavaOpCode(JavaOpCodeTag.",Table!B147,", """,Table!A147,""", JavaOperandType.Inline",Table!D147,", JavaFlowControl.",Table!F147,", ",Table!E147,", JavaStackBehavior.",A146,", JavaStackBehavior.",B146,");")</f>
+        <v>Istore_3 = new JavaOpCode(JavaOpCodeTag.Istore_3, "istore_3", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -10734,8 +10731,8 @@
         <v>PushI</v>
       </c>
       <c r="C147" s="1" t="str">
-        <f>CONCATENATE(Table!B148," = new JavaInstruction(JavaOpCode.",Table!B148,", """,Table!A148,""", JavaOperandType.Inline",Table!D148,", JavaFlowControl.",Table!F148,", ",Table!E148,", JavaStackBehavior.",A147,", JavaStackBehavior.",B147,");")</f>
-        <v>Isub = new JavaInstruction(JavaOpCode.Isub, "isub", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI_PopI, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B148," = new JavaOpCode(JavaOpCodeTag.",Table!B148,", """,Table!A148,""", JavaOperandType.Inline",Table!D148,", JavaFlowControl.",Table!F148,", ",Table!E148,", JavaStackBehavior.",A147,", JavaStackBehavior.",B147,");")</f>
+        <v>Isub = new JavaOpCode(JavaOpCodeTag.Isub, "isub", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI_PopI, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -10748,8 +10745,8 @@
         <v>PushI</v>
       </c>
       <c r="C148" s="1" t="str">
-        <f>CONCATENATE(Table!B149," = new JavaInstruction(JavaOpCode.",Table!B149,", """,Table!A149,""", JavaOperandType.Inline",Table!D149,", JavaFlowControl.",Table!F149,", ",Table!E149,", JavaStackBehavior.",A148,", JavaStackBehavior.",B148,");")</f>
-        <v>Iushr = new JavaInstruction(JavaOpCode.Iushr, "iushr", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI_PopI, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B149," = new JavaOpCode(JavaOpCodeTag.",Table!B149,", """,Table!A149,""", JavaOperandType.Inline",Table!D149,", JavaFlowControl.",Table!F149,", ",Table!E149,", JavaStackBehavior.",A148,", JavaStackBehavior.",B148,");")</f>
+        <v>Iushr = new JavaOpCode(JavaOpCodeTag.Iushr, "iushr", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI_PopI, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -10762,8 +10759,8 @@
         <v>PushI</v>
       </c>
       <c r="C149" s="1" t="str">
-        <f>CONCATENATE(Table!B150," = new JavaInstruction(JavaOpCode.",Table!B150,", """,Table!A150,""", JavaOperandType.Inline",Table!D150,", JavaFlowControl.",Table!F150,", ",Table!E150,", JavaStackBehavior.",A149,", JavaStackBehavior.",B149,");")</f>
-        <v>Ixor = new JavaInstruction(JavaOpCode.Ixor, "ixor", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI_PopI, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B150," = new JavaOpCode(JavaOpCodeTag.",Table!B150,", """,Table!A150,""", JavaOperandType.Inline",Table!D150,", JavaFlowControl.",Table!F150,", ",Table!E150,", JavaStackBehavior.",A149,", JavaStackBehavior.",B149,");")</f>
+        <v>Ixor = new JavaOpCode(JavaOpCodeTag.Ixor, "ixor", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI_PopI, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -10776,8 +10773,8 @@
         <v>PushRet</v>
       </c>
       <c r="C150" s="1" t="str">
-        <f>CONCATENATE(Table!B151," = new JavaInstruction(JavaOpCode.",Table!B151,", """,Table!A151,""", JavaOperandType.Inline",Table!D151,", JavaFlowControl.",Table!F151,", ",Table!E151,", JavaStackBehavior.",A150,", JavaStackBehavior.",B150,");")</f>
-        <v>Jsr = new JavaInstruction(JavaOpCode.Jsr, "jsr", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.Branch, 3, JavaStackBehavior.Pop0, JavaStackBehavior.PushRet);</v>
+        <f>CONCATENATE(Table!B151," = new JavaOpCode(JavaOpCodeTag.",Table!B151,", """,Table!A151,""", JavaOperandType.Inline",Table!D151,", JavaFlowControl.",Table!F151,", ",Table!E151,", JavaStackBehavior.",A150,", JavaStackBehavior.",B150,");")</f>
+        <v>Jsr = new JavaOpCode(JavaOpCodeTag.Jsr, "jsr", JavaOperandType.InlineShortBranchTarget, JavaFlowControl.Branch, 3, JavaStackBehavior.Pop0, JavaStackBehavior.PushRet);</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -10790,8 +10787,8 @@
         <v>PushRet</v>
       </c>
       <c r="C151" s="1" t="str">
-        <f>CONCATENATE(Table!B152," = new JavaInstruction(JavaOpCode.",Table!B152,", """,Table!A152,""", JavaOperandType.Inline",Table!D152,", JavaFlowControl.",Table!F152,", ",Table!E152,", JavaStackBehavior.",A151,", JavaStackBehavior.",B151,");")</f>
-        <v>Jsr_w = new JavaInstruction(JavaOpCode.Jsr_w, "jsr_w", JavaOperandType.InlineBranchTarget, JavaFlowControl.Branch, 5, JavaStackBehavior.Pop0, JavaStackBehavior.PushRet);</v>
+        <f>CONCATENATE(Table!B152," = new JavaOpCode(JavaOpCodeTag.",Table!B152,", """,Table!A152,""", JavaOperandType.Inline",Table!D152,", JavaFlowControl.",Table!F152,", ",Table!E152,", JavaStackBehavior.",A151,", JavaStackBehavior.",B151,");")</f>
+        <v>Jsr_w = new JavaOpCode(JavaOpCodeTag.Jsr_w, "jsr_w", JavaOperandType.InlineBranchTarget, JavaFlowControl.Branch, 5, JavaStackBehavior.Pop0, JavaStackBehavior.PushRet);</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -10804,8 +10801,8 @@
         <v>PushR8</v>
       </c>
       <c r="C152" s="1" t="str">
-        <f>CONCATENATE(Table!B153," = new JavaInstruction(JavaOpCode.",Table!B153,", """,Table!A153,""", JavaOperandType.Inline",Table!D153,", JavaFlowControl.",Table!F153,", ",Table!E153,", JavaStackBehavior.",A152,", JavaStackBehavior.",B152,");")</f>
-        <v>L2d = new JavaInstruction(JavaOpCode.L2d, "l2d", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8, JavaStackBehavior.PushR8);</v>
+        <f>CONCATENATE(Table!B153," = new JavaOpCode(JavaOpCodeTag.",Table!B153,", """,Table!A153,""", JavaOperandType.Inline",Table!D153,", JavaFlowControl.",Table!F153,", ",Table!E153,", JavaStackBehavior.",A152,", JavaStackBehavior.",B152,");")</f>
+        <v>L2d = new JavaOpCode(JavaOpCodeTag.L2d, "l2d", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8, JavaStackBehavior.PushR8);</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -10818,8 +10815,8 @@
         <v>PushR4</v>
       </c>
       <c r="C153" s="1" t="str">
-        <f>CONCATENATE(Table!B154," = new JavaInstruction(JavaOpCode.",Table!B154,", """,Table!A154,""", JavaOperandType.Inline",Table!D154,", JavaFlowControl.",Table!F154,", ",Table!E154,", JavaStackBehavior.",A153,", JavaStackBehavior.",B153,");")</f>
-        <v>L2f = new JavaInstruction(JavaOpCode.L2f, "l2f", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8, JavaStackBehavior.PushR4);</v>
+        <f>CONCATENATE(Table!B154," = new JavaOpCode(JavaOpCodeTag.",Table!B154,", """,Table!A154,""", JavaOperandType.Inline",Table!D154,", JavaFlowControl.",Table!F154,", ",Table!E154,", JavaStackBehavior.",A153,", JavaStackBehavior.",B153,");")</f>
+        <v>L2f = new JavaOpCode(JavaOpCodeTag.L2f, "l2f", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8, JavaStackBehavior.PushR4);</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -10832,8 +10829,8 @@
         <v>PushI</v>
       </c>
       <c r="C154" s="1" t="str">
-        <f>CONCATENATE(Table!B155," = new JavaInstruction(JavaOpCode.",Table!B155,", """,Table!A155,""", JavaOperandType.Inline",Table!D155,", JavaFlowControl.",Table!F155,", ",Table!E155,", JavaStackBehavior.",A154,", JavaStackBehavior.",B154,");")</f>
-        <v>L2i = new JavaInstruction(JavaOpCode.L2i, "l2i", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B155," = new JavaOpCode(JavaOpCodeTag.",Table!B155,", """,Table!A155,""", JavaOperandType.Inline",Table!D155,", JavaFlowControl.",Table!F155,", ",Table!E155,", JavaStackBehavior.",A154,", JavaStackBehavior.",B154,");")</f>
+        <v>L2i = new JavaOpCode(JavaOpCodeTag.L2i, "l2i", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -10846,8 +10843,8 @@
         <v>PushI8</v>
       </c>
       <c r="C155" s="1" t="str">
-        <f>CONCATENATE(Table!B156," = new JavaInstruction(JavaOpCode.",Table!B156,", """,Table!A156,""", JavaOperandType.Inline",Table!D156,", JavaFlowControl.",Table!F156,", ",Table!E156,", JavaStackBehavior.",A155,", JavaStackBehavior.",B155,");")</f>
-        <v>Ladd = new JavaInstruction(JavaOpCode.Ladd, "ladd", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8_PopI8, JavaStackBehavior.PushI8);</v>
+        <f>CONCATENATE(Table!B156," = new JavaOpCode(JavaOpCodeTag.",Table!B156,", """,Table!A156,""", JavaOperandType.Inline",Table!D156,", JavaFlowControl.",Table!F156,", ",Table!E156,", JavaStackBehavior.",A155,", JavaStackBehavior.",B155,");")</f>
+        <v>Ladd = new JavaOpCode(JavaOpCodeTag.Ladd, "ladd", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8_PopI8, JavaStackBehavior.PushI8);</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -10860,8 +10857,8 @@
         <v>PushI8</v>
       </c>
       <c r="C156" s="1" t="str">
-        <f>CONCATENATE(Table!B157," = new JavaInstruction(JavaOpCode.",Table!B157,", """,Table!A157,""", JavaOperandType.Inline",Table!D157,", JavaFlowControl.",Table!F157,", ",Table!E157,", JavaStackBehavior.",A156,", JavaStackBehavior.",B156,");")</f>
-        <v>Laload = new JavaInstruction(JavaOpCode.Laload, "laload", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI, JavaStackBehavior.PushI8);</v>
+        <f>CONCATENATE(Table!B157," = new JavaOpCode(JavaOpCodeTag.",Table!B157,", """,Table!A157,""", JavaOperandType.Inline",Table!D157,", JavaFlowControl.",Table!F157,", ",Table!E157,", JavaStackBehavior.",A156,", JavaStackBehavior.",B156,");")</f>
+        <v>Laload = new JavaOpCode(JavaOpCodeTag.Laload, "laload", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI, JavaStackBehavior.PushI8);</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -10874,8 +10871,8 @@
         <v>PushI8</v>
       </c>
       <c r="C157" s="1" t="str">
-        <f>CONCATENATE(Table!B158," = new JavaInstruction(JavaOpCode.",Table!B158,", """,Table!A158,""", JavaOperandType.Inline",Table!D158,", JavaFlowControl.",Table!F158,", ",Table!E158,", JavaStackBehavior.",A157,", JavaStackBehavior.",B157,");")</f>
-        <v>Land = new JavaInstruction(JavaOpCode.Land, "land", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8_PopI8, JavaStackBehavior.PushI8);</v>
+        <f>CONCATENATE(Table!B158," = new JavaOpCode(JavaOpCodeTag.",Table!B158,", """,Table!A158,""", JavaOperandType.Inline",Table!D158,", JavaFlowControl.",Table!F158,", ",Table!E158,", JavaStackBehavior.",A157,", JavaStackBehavior.",B157,");")</f>
+        <v>Land = new JavaOpCode(JavaOpCodeTag.Land, "land", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8_PopI8, JavaStackBehavior.PushI8);</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -10888,8 +10885,8 @@
         <v>Push0</v>
       </c>
       <c r="C158" s="1" t="str">
-        <f>CONCATENATE(Table!B159," = new JavaInstruction(JavaOpCode.",Table!B159,", """,Table!A159,""", JavaOperandType.Inline",Table!D159,", JavaFlowControl.",Table!F159,", ",Table!E159,", JavaStackBehavior.",A158,", JavaStackBehavior.",B158,");")</f>
-        <v>Lastore = new JavaInstruction(JavaOpCode.Lastore, "lastore", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI_PopI8, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B159," = new JavaOpCode(JavaOpCodeTag.",Table!B159,", """,Table!A159,""", JavaOperandType.Inline",Table!D159,", JavaFlowControl.",Table!F159,", ",Table!E159,", JavaStackBehavior.",A158,", JavaStackBehavior.",B158,");")</f>
+        <v>Lastore = new JavaOpCode(JavaOpCodeTag.Lastore, "lastore", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI_PopI8, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -10902,8 +10899,8 @@
         <v>PushI</v>
       </c>
       <c r="C159" s="1" t="str">
-        <f>CONCATENATE(Table!B160," = new JavaInstruction(JavaOpCode.",Table!B160,", """,Table!A160,""", JavaOperandType.Inline",Table!D160,", JavaFlowControl.",Table!F160,", ",Table!E160,", JavaStackBehavior.",A159,", JavaStackBehavior.",B159,");")</f>
-        <v>Lcmp = new JavaInstruction(JavaOpCode.Lcmp, "lcmp", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8_PopI8, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B160," = new JavaOpCode(JavaOpCodeTag.",Table!B160,", """,Table!A160,""", JavaOperandType.Inline",Table!D160,", JavaFlowControl.",Table!F160,", ",Table!E160,", JavaStackBehavior.",A159,", JavaStackBehavior.",B159,");")</f>
+        <v>Lcmp = new JavaOpCode(JavaOpCodeTag.Lcmp, "lcmp", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8_PopI8, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -10916,8 +10913,8 @@
         <v>PushI8</v>
       </c>
       <c r="C160" s="1" t="str">
-        <f>CONCATENATE(Table!B161," = new JavaInstruction(JavaOpCode.",Table!B161,", """,Table!A161,""", JavaOperandType.Inline",Table!D161,", JavaFlowControl.",Table!F161,", ",Table!E161,", JavaStackBehavior.",A160,", JavaStackBehavior.",B160,");")</f>
-        <v>Lconst_0 = new JavaInstruction(JavaOpCode.Lconst_0, "lconst_0", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI8);</v>
+        <f>CONCATENATE(Table!B161," = new JavaOpCode(JavaOpCodeTag.",Table!B161,", """,Table!A161,""", JavaOperandType.Inline",Table!D161,", JavaFlowControl.",Table!F161,", ",Table!E161,", JavaStackBehavior.",A160,", JavaStackBehavior.",B160,");")</f>
+        <v>Lconst_0 = new JavaOpCode(JavaOpCodeTag.Lconst_0, "lconst_0", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI8);</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -10930,8 +10927,8 @@
         <v>PushI8</v>
       </c>
       <c r="C161" s="1" t="str">
-        <f>CONCATENATE(Table!B162," = new JavaInstruction(JavaOpCode.",Table!B162,", """,Table!A162,""", JavaOperandType.Inline",Table!D162,", JavaFlowControl.",Table!F162,", ",Table!E162,", JavaStackBehavior.",A161,", JavaStackBehavior.",B161,");")</f>
-        <v>Lconst_1 = new JavaInstruction(JavaOpCode.Lconst_1, "lconst_1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI8);</v>
+        <f>CONCATENATE(Table!B162," = new JavaOpCode(JavaOpCodeTag.",Table!B162,", """,Table!A162,""", JavaOperandType.Inline",Table!D162,", JavaFlowControl.",Table!F162,", ",Table!E162,", JavaStackBehavior.",A161,", JavaStackBehavior.",B161,");")</f>
+        <v>Lconst_1 = new JavaOpCode(JavaOpCodeTag.Lconst_1, "lconst_1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI8);</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -10944,8 +10941,8 @@
         <v>Push1</v>
       </c>
       <c r="C162" s="1" t="str">
-        <f>CONCATENATE(Table!B163," = new JavaInstruction(JavaOpCode.",Table!B163,", """,Table!A163,""", JavaOperandType.Inline",Table!D163,", JavaFlowControl.",Table!F163,", ",Table!E163,", JavaStackBehavior.",A162,", JavaStackBehavior.",B162,");")</f>
-        <v>Ldc = new JavaInstruction(JavaOpCode.Ldc, "ldc", JavaOperandType.InlineShortConst, JavaFlowControl.Next, 2, JavaStackBehavior.Pop0, JavaStackBehavior.Push1);</v>
+        <f>CONCATENATE(Table!B163," = new JavaOpCode(JavaOpCodeTag.",Table!B163,", """,Table!A163,""", JavaOperandType.Inline",Table!D163,", JavaFlowControl.",Table!F163,", ",Table!E163,", JavaStackBehavior.",A162,", JavaStackBehavior.",B162,");")</f>
+        <v>Ldc = new JavaOpCode(JavaOpCodeTag.Ldc, "ldc", JavaOperandType.InlineShortConst, JavaFlowControl.Next, 2, JavaStackBehavior.Pop0, JavaStackBehavior.Push1);</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -10958,8 +10955,8 @@
         <v>Push1</v>
       </c>
       <c r="C163" s="1" t="str">
-        <f>CONCATENATE(Table!B164," = new JavaInstruction(JavaOpCode.",Table!B164,", """,Table!A164,""", JavaOperandType.Inline",Table!D164,", JavaFlowControl.",Table!F164,", ",Table!E164,", JavaStackBehavior.",A163,", JavaStackBehavior.",B163,");")</f>
-        <v>Ldc_w = new JavaInstruction(JavaOpCode.Ldc_w, "ldc_w", JavaOperandType.InlineConst, JavaFlowControl.Next, 3, JavaStackBehavior.Pop0, JavaStackBehavior.Push1);</v>
+        <f>CONCATENATE(Table!B164," = new JavaOpCode(JavaOpCodeTag.",Table!B164,", """,Table!A164,""", JavaOperandType.Inline",Table!D164,", JavaFlowControl.",Table!F164,", ",Table!E164,", JavaStackBehavior.",A163,", JavaStackBehavior.",B163,");")</f>
+        <v>Ldc_w = new JavaOpCode(JavaOpCodeTag.Ldc_w, "ldc_w", JavaOperandType.InlineConst, JavaFlowControl.Next, 3, JavaStackBehavior.Pop0, JavaStackBehavior.Push1);</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -10972,8 +10969,8 @@
         <v>Push1</v>
       </c>
       <c r="C164" s="1" t="str">
-        <f>CONCATENATE(Table!B165," = new JavaInstruction(JavaOpCode.",Table!B165,", """,Table!A165,""", JavaOperandType.Inline",Table!D165,", JavaFlowControl.",Table!F165,", ",Table!E165,", JavaStackBehavior.",A164,", JavaStackBehavior.",B164,");")</f>
-        <v>Ldc2_w = new JavaInstruction(JavaOpCode.Ldc2_w, "ldc2_w", JavaOperandType.InlineConst, JavaFlowControl.Next, 3, JavaStackBehavior.Pop0, JavaStackBehavior.Push1);</v>
+        <f>CONCATENATE(Table!B165," = new JavaOpCode(JavaOpCodeTag.",Table!B165,", """,Table!A165,""", JavaOperandType.Inline",Table!D165,", JavaFlowControl.",Table!F165,", ",Table!E165,", JavaStackBehavior.",A164,", JavaStackBehavior.",B164,");")</f>
+        <v>Ldc2_w = new JavaOpCode(JavaOpCodeTag.Ldc2_w, "ldc2_w", JavaOperandType.InlineConst, JavaFlowControl.Next, 3, JavaStackBehavior.Pop0, JavaStackBehavior.Push1);</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -10986,8 +10983,8 @@
         <v>PushI8</v>
       </c>
       <c r="C165" s="1" t="str">
-        <f>CONCATENATE(Table!B166," = new JavaInstruction(JavaOpCode.",Table!B166,", """,Table!A166,""", JavaOperandType.Inline",Table!D166,", JavaFlowControl.",Table!F166,", ",Table!E166,", JavaStackBehavior.",A165,", JavaStackBehavior.",B165,");")</f>
-        <v>Ldiv = new JavaInstruction(JavaOpCode.Ldiv, "ldiv", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8_PopI8, JavaStackBehavior.PushI8);</v>
+        <f>CONCATENATE(Table!B166," = new JavaOpCode(JavaOpCodeTag.",Table!B166,", """,Table!A166,""", JavaOperandType.Inline",Table!D166,", JavaFlowControl.",Table!F166,", ",Table!E166,", JavaStackBehavior.",A165,", JavaStackBehavior.",B165,");")</f>
+        <v>Ldiv = new JavaOpCode(JavaOpCodeTag.Ldiv, "ldiv", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8_PopI8, JavaStackBehavior.PushI8);</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -11000,8 +10997,8 @@
         <v>PushI8</v>
       </c>
       <c r="C166" s="1" t="str">
-        <f>CONCATENATE(Table!B167," = new JavaInstruction(JavaOpCode.",Table!B167,", """,Table!A167,""", JavaOperandType.Inline",Table!D167,", JavaFlowControl.",Table!F167,", ",Table!E167,", JavaStackBehavior.",A166,", JavaStackBehavior.",B166,");")</f>
-        <v>Lload = new JavaInstruction(JavaOpCode.Lload, "lload", JavaOperandType.InlineVar, JavaFlowControl.Next, 2, JavaStackBehavior.Pop0, JavaStackBehavior.PushI8);</v>
+        <f>CONCATENATE(Table!B167," = new JavaOpCode(JavaOpCodeTag.",Table!B167,", """,Table!A167,""", JavaOperandType.Inline",Table!D167,", JavaFlowControl.",Table!F167,", ",Table!E167,", JavaStackBehavior.",A166,", JavaStackBehavior.",B166,");")</f>
+        <v>Lload = new JavaOpCode(JavaOpCodeTag.Lload, "lload", JavaOperandType.InlineVar, JavaFlowControl.Next, 2, JavaStackBehavior.Pop0, JavaStackBehavior.PushI8);</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -11014,8 +11011,8 @@
         <v>PushI8</v>
       </c>
       <c r="C167" s="1" t="str">
-        <f>CONCATENATE(Table!B168," = new JavaInstruction(JavaOpCode.",Table!B168,", """,Table!A168,""", JavaOperandType.Inline",Table!D168,", JavaFlowControl.",Table!F168,", ",Table!E168,", JavaStackBehavior.",A167,", JavaStackBehavior.",B167,");")</f>
-        <v>Lload_0 = new JavaInstruction(JavaOpCode.Lload_0, "lload_0", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI8);</v>
+        <f>CONCATENATE(Table!B168," = new JavaOpCode(JavaOpCodeTag.",Table!B168,", """,Table!A168,""", JavaOperandType.Inline",Table!D168,", JavaFlowControl.",Table!F168,", ",Table!E168,", JavaStackBehavior.",A167,", JavaStackBehavior.",B167,");")</f>
+        <v>Lload_0 = new JavaOpCode(JavaOpCodeTag.Lload_0, "lload_0", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI8);</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -11028,8 +11025,8 @@
         <v>PushI8</v>
       </c>
       <c r="C168" s="1" t="str">
-        <f>CONCATENATE(Table!B169," = new JavaInstruction(JavaOpCode.",Table!B169,", """,Table!A169,""", JavaOperandType.Inline",Table!D169,", JavaFlowControl.",Table!F169,", ",Table!E169,", JavaStackBehavior.",A168,", JavaStackBehavior.",B168,");")</f>
-        <v>Lload_1 = new JavaInstruction(JavaOpCode.Lload_1, "lload_1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI8);</v>
+        <f>CONCATENATE(Table!B169," = new JavaOpCode(JavaOpCodeTag.",Table!B169,", """,Table!A169,""", JavaOperandType.Inline",Table!D169,", JavaFlowControl.",Table!F169,", ",Table!E169,", JavaStackBehavior.",A168,", JavaStackBehavior.",B168,");")</f>
+        <v>Lload_1 = new JavaOpCode(JavaOpCodeTag.Lload_1, "lload_1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI8);</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -11042,8 +11039,8 @@
         <v>PushI8</v>
       </c>
       <c r="C169" s="1" t="str">
-        <f>CONCATENATE(Table!B170," = new JavaInstruction(JavaOpCode.",Table!B170,", """,Table!A170,""", JavaOperandType.Inline",Table!D170,", JavaFlowControl.",Table!F170,", ",Table!E170,", JavaStackBehavior.",A169,", JavaStackBehavior.",B169,");")</f>
-        <v>Lload_2 = new JavaInstruction(JavaOpCode.Lload_2, "lload_2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI8);</v>
+        <f>CONCATENATE(Table!B170," = new JavaOpCode(JavaOpCodeTag.",Table!B170,", """,Table!A170,""", JavaOperandType.Inline",Table!D170,", JavaFlowControl.",Table!F170,", ",Table!E170,", JavaStackBehavior.",A169,", JavaStackBehavior.",B169,");")</f>
+        <v>Lload_2 = new JavaOpCode(JavaOpCodeTag.Lload_2, "lload_2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI8);</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -11056,8 +11053,8 @@
         <v>PushI8</v>
       </c>
       <c r="C170" s="1" t="str">
-        <f>CONCATENATE(Table!B171," = new JavaInstruction(JavaOpCode.",Table!B171,", """,Table!A171,""", JavaOperandType.Inline",Table!D171,", JavaFlowControl.",Table!F171,", ",Table!E171,", JavaStackBehavior.",A170,", JavaStackBehavior.",B170,");")</f>
-        <v>Lload_3 = new JavaInstruction(JavaOpCode.Lload_3, "lload_3", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI8);</v>
+        <f>CONCATENATE(Table!B171," = new JavaOpCode(JavaOpCodeTag.",Table!B171,", """,Table!A171,""", JavaOperandType.Inline",Table!D171,", JavaFlowControl.",Table!F171,", ",Table!E171,", JavaStackBehavior.",A170,", JavaStackBehavior.",B170,");")</f>
+        <v>Lload_3 = new JavaOpCode(JavaOpCodeTag.Lload_3, "lload_3", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.PushI8);</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -11070,8 +11067,8 @@
         <v>PushI8</v>
       </c>
       <c r="C171" s="1" t="str">
-        <f>CONCATENATE(Table!B172," = new JavaInstruction(JavaOpCode.",Table!B172,", """,Table!A172,""", JavaOperandType.Inline",Table!D172,", JavaFlowControl.",Table!F172,", ",Table!E172,", JavaStackBehavior.",A171,", JavaStackBehavior.",B171,");")</f>
-        <v>Lmul = new JavaInstruction(JavaOpCode.Lmul, "lmul", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8_PopI8, JavaStackBehavior.PushI8);</v>
+        <f>CONCATENATE(Table!B172," = new JavaOpCode(JavaOpCodeTag.",Table!B172,", """,Table!A172,""", JavaOperandType.Inline",Table!D172,", JavaFlowControl.",Table!F172,", ",Table!E172,", JavaStackBehavior.",A171,", JavaStackBehavior.",B171,");")</f>
+        <v>Lmul = new JavaOpCode(JavaOpCodeTag.Lmul, "lmul", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8_PopI8, JavaStackBehavior.PushI8);</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -11084,8 +11081,8 @@
         <v>PushI8</v>
       </c>
       <c r="C172" s="1" t="str">
-        <f>CONCATENATE(Table!B173," = new JavaInstruction(JavaOpCode.",Table!B173,", """,Table!A173,""", JavaOperandType.Inline",Table!D173,", JavaFlowControl.",Table!F173,", ",Table!E173,", JavaStackBehavior.",A172,", JavaStackBehavior.",B172,");")</f>
-        <v>Lneg = new JavaInstruction(JavaOpCode.Lneg, "lneg", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8, JavaStackBehavior.PushI8);</v>
+        <f>CONCATENATE(Table!B173," = new JavaOpCode(JavaOpCodeTag.",Table!B173,", """,Table!A173,""", JavaOperandType.Inline",Table!D173,", JavaFlowControl.",Table!F173,", ",Table!E173,", JavaStackBehavior.",A172,", JavaStackBehavior.",B172,");")</f>
+        <v>Lneg = new JavaOpCode(JavaOpCodeTag.Lneg, "lneg", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8, JavaStackBehavior.PushI8);</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -11098,8 +11095,8 @@
         <v>Push0</v>
       </c>
       <c r="C173" s="1" t="str">
-        <f>CONCATENATE(Table!B174," = new JavaInstruction(JavaOpCode.",Table!B174,", """,Table!A174,""", JavaOperandType.Inline",Table!D174,", JavaFlowControl.",Table!F174,", ",Table!E174,", JavaStackBehavior.",A173,", JavaStackBehavior.",B173,");")</f>
-        <v>Lookupswitch = new JavaInstruction(JavaOpCode.Lookupswitch, "lookupswitch", JavaOperandType.InlineSwitch, JavaFlowControl.Next, 0, JavaStackBehavior.PopI, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B174," = new JavaOpCode(JavaOpCodeTag.",Table!B174,", """,Table!A174,""", JavaOperandType.Inline",Table!D174,", JavaFlowControl.",Table!F174,", ",Table!E174,", JavaStackBehavior.",A173,", JavaStackBehavior.",B173,");")</f>
+        <v>Lookupswitch = new JavaOpCode(JavaOpCodeTag.Lookupswitch, "lookupswitch", JavaOperandType.InlineLookupSwitch, JavaFlowControl.ConditionalBranch, 0, JavaStackBehavior.PopI, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -11112,8 +11109,8 @@
         <v>PushI8</v>
       </c>
       <c r="C174" s="1" t="str">
-        <f>CONCATENATE(Table!B175," = new JavaInstruction(JavaOpCode.",Table!B175,", """,Table!A175,""", JavaOperandType.Inline",Table!D175,", JavaFlowControl.",Table!F175,", ",Table!E175,", JavaStackBehavior.",A174,", JavaStackBehavior.",B174,");")</f>
-        <v>Lor = new JavaInstruction(JavaOpCode.Lor, "lor", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8_PopI8, JavaStackBehavior.PushI8);</v>
+        <f>CONCATENATE(Table!B175," = new JavaOpCode(JavaOpCodeTag.",Table!B175,", """,Table!A175,""", JavaOperandType.Inline",Table!D175,", JavaFlowControl.",Table!F175,", ",Table!E175,", JavaStackBehavior.",A174,", JavaStackBehavior.",B174,");")</f>
+        <v>Lor = new JavaOpCode(JavaOpCodeTag.Lor, "lor", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8_PopI8, JavaStackBehavior.PushI8);</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -11126,8 +11123,8 @@
         <v>PushI8</v>
       </c>
       <c r="C175" s="1" t="str">
-        <f>CONCATENATE(Table!B176," = new JavaInstruction(JavaOpCode.",Table!B176,", """,Table!A176,""", JavaOperandType.Inline",Table!D176,", JavaFlowControl.",Table!F176,", ",Table!E176,", JavaStackBehavior.",A175,", JavaStackBehavior.",B175,");")</f>
-        <v>Lrem = new JavaInstruction(JavaOpCode.Lrem, "lrem", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8_PopI8, JavaStackBehavior.PushI8);</v>
+        <f>CONCATENATE(Table!B176," = new JavaOpCode(JavaOpCodeTag.",Table!B176,", """,Table!A176,""", JavaOperandType.Inline",Table!D176,", JavaFlowControl.",Table!F176,", ",Table!E176,", JavaStackBehavior.",A175,", JavaStackBehavior.",B175,");")</f>
+        <v>Lrem = new JavaOpCode(JavaOpCodeTag.Lrem, "lrem", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8_PopI8, JavaStackBehavior.PushI8);</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -11140,8 +11137,8 @@
         <v>Push0</v>
       </c>
       <c r="C176" s="1" t="str">
-        <f>CONCATENATE(Table!B177," = new JavaInstruction(JavaOpCode.",Table!B177,", """,Table!A177,""", JavaOperandType.Inline",Table!D177,", JavaFlowControl.",Table!F177,", ",Table!E177,", JavaStackBehavior.",A176,", JavaStackBehavior.",B176,");")</f>
-        <v>Lreturn = new JavaInstruction(JavaOpCode.Lreturn, "lreturn", JavaOperandType.InlineNone, JavaFlowControl.Return, 1, JavaStackBehavior.PopI8, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B177," = new JavaOpCode(JavaOpCodeTag.",Table!B177,", """,Table!A177,""", JavaOperandType.Inline",Table!D177,", JavaFlowControl.",Table!F177,", ",Table!E177,", JavaStackBehavior.",A176,", JavaStackBehavior.",B176,");")</f>
+        <v>Lreturn = new JavaOpCode(JavaOpCodeTag.Lreturn, "lreturn", JavaOperandType.InlineNone, JavaFlowControl.Return, 1, JavaStackBehavior.PopI8, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -11154,8 +11151,8 @@
         <v>PushI8</v>
       </c>
       <c r="C177" s="1" t="str">
-        <f>CONCATENATE(Table!B178," = new JavaInstruction(JavaOpCode.",Table!B178,", """,Table!A178,""", JavaOperandType.Inline",Table!D178,", JavaFlowControl.",Table!F178,", ",Table!E178,", JavaStackBehavior.",A177,", JavaStackBehavior.",B177,");")</f>
-        <v>Lshl = new JavaInstruction(JavaOpCode.Lshl, "lshl", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8_PopI, JavaStackBehavior.PushI8);</v>
+        <f>CONCATENATE(Table!B178," = new JavaOpCode(JavaOpCodeTag.",Table!B178,", """,Table!A178,""", JavaOperandType.Inline",Table!D178,", JavaFlowControl.",Table!F178,", ",Table!E178,", JavaStackBehavior.",A177,", JavaStackBehavior.",B177,");")</f>
+        <v>Lshl = new JavaOpCode(JavaOpCodeTag.Lshl, "lshl", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8_PopI, JavaStackBehavior.PushI8);</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
@@ -11168,8 +11165,8 @@
         <v>PushI8</v>
       </c>
       <c r="C178" s="1" t="str">
-        <f>CONCATENATE(Table!B179," = new JavaInstruction(JavaOpCode.",Table!B179,", """,Table!A179,""", JavaOperandType.Inline",Table!D179,", JavaFlowControl.",Table!F179,", ",Table!E179,", JavaStackBehavior.",A178,", JavaStackBehavior.",B178,");")</f>
-        <v>Lshr = new JavaInstruction(JavaOpCode.Lshr, "lshr", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8_PopI, JavaStackBehavior.PushI8);</v>
+        <f>CONCATENATE(Table!B179," = new JavaOpCode(JavaOpCodeTag.",Table!B179,", """,Table!A179,""", JavaOperandType.Inline",Table!D179,", JavaFlowControl.",Table!F179,", ",Table!E179,", JavaStackBehavior.",A178,", JavaStackBehavior.",B178,");")</f>
+        <v>Lshr = new JavaOpCode(JavaOpCodeTag.Lshr, "lshr", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8_PopI, JavaStackBehavior.PushI8);</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -11182,8 +11179,8 @@
         <v>Push0</v>
       </c>
       <c r="C179" s="1" t="str">
-        <f>CONCATENATE(Table!B180," = new JavaInstruction(JavaOpCode.",Table!B180,", """,Table!A180,""", JavaOperandType.Inline",Table!D180,", JavaFlowControl.",Table!F180,", ",Table!E180,", JavaStackBehavior.",A179,", JavaStackBehavior.",B179,");")</f>
-        <v>Lstore = new JavaInstruction(JavaOpCode.Lstore, "lstore", JavaOperandType.InlineVar, JavaFlowControl.Next, 2, JavaStackBehavior.PopI8, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B180," = new JavaOpCode(JavaOpCodeTag.",Table!B180,", """,Table!A180,""", JavaOperandType.Inline",Table!D180,", JavaFlowControl.",Table!F180,", ",Table!E180,", JavaStackBehavior.",A179,", JavaStackBehavior.",B179,");")</f>
+        <v>Lstore = new JavaOpCode(JavaOpCodeTag.Lstore, "lstore", JavaOperandType.InlineVar, JavaFlowControl.Next, 2, JavaStackBehavior.PopI8, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -11196,8 +11193,8 @@
         <v>Push0</v>
       </c>
       <c r="C180" s="1" t="str">
-        <f>CONCATENATE(Table!B181," = new JavaInstruction(JavaOpCode.",Table!B181,", """,Table!A181,""", JavaOperandType.Inline",Table!D181,", JavaFlowControl.",Table!F181,", ",Table!E181,", JavaStackBehavior.",A180,", JavaStackBehavior.",B180,");")</f>
-        <v>Lstore_0 = new JavaInstruction(JavaOpCode.Lstore_0, "lstore_0", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B181," = new JavaOpCode(JavaOpCodeTag.",Table!B181,", """,Table!A181,""", JavaOperandType.Inline",Table!D181,", JavaFlowControl.",Table!F181,", ",Table!E181,", JavaStackBehavior.",A180,", JavaStackBehavior.",B180,");")</f>
+        <v>Lstore_0 = new JavaOpCode(JavaOpCodeTag.Lstore_0, "lstore_0", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -11210,8 +11207,8 @@
         <v>Push0</v>
       </c>
       <c r="C181" s="1" t="str">
-        <f>CONCATENATE(Table!B182," = new JavaInstruction(JavaOpCode.",Table!B182,", """,Table!A182,""", JavaOperandType.Inline",Table!D182,", JavaFlowControl.",Table!F182,", ",Table!E182,", JavaStackBehavior.",A181,", JavaStackBehavior.",B181,");")</f>
-        <v>Lstore_1 = new JavaInstruction(JavaOpCode.Lstore_1, "lstore_1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B182," = new JavaOpCode(JavaOpCodeTag.",Table!B182,", """,Table!A182,""", JavaOperandType.Inline",Table!D182,", JavaFlowControl.",Table!F182,", ",Table!E182,", JavaStackBehavior.",A181,", JavaStackBehavior.",B181,");")</f>
+        <v>Lstore_1 = new JavaOpCode(JavaOpCodeTag.Lstore_1, "lstore_1", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -11224,8 +11221,8 @@
         <v>Push0</v>
       </c>
       <c r="C182" s="1" t="str">
-        <f>CONCATENATE(Table!B183," = new JavaInstruction(JavaOpCode.",Table!B183,", """,Table!A183,""", JavaOperandType.Inline",Table!D183,", JavaFlowControl.",Table!F183,", ",Table!E183,", JavaStackBehavior.",A182,", JavaStackBehavior.",B182,");")</f>
-        <v>Lstore_2 = new JavaInstruction(JavaOpCode.Lstore_2, "lstore_2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B183," = new JavaOpCode(JavaOpCodeTag.",Table!B183,", """,Table!A183,""", JavaOperandType.Inline",Table!D183,", JavaFlowControl.",Table!F183,", ",Table!E183,", JavaStackBehavior.",A182,", JavaStackBehavior.",B182,");")</f>
+        <v>Lstore_2 = new JavaOpCode(JavaOpCodeTag.Lstore_2, "lstore_2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -11238,8 +11235,8 @@
         <v>Push0</v>
       </c>
       <c r="C183" s="1" t="str">
-        <f>CONCATENATE(Table!B184," = new JavaInstruction(JavaOpCode.",Table!B184,", """,Table!A184,""", JavaOperandType.Inline",Table!D184,", JavaFlowControl.",Table!F184,", ",Table!E184,", JavaStackBehavior.",A183,", JavaStackBehavior.",B183,");")</f>
-        <v>Lstore_3 = new JavaInstruction(JavaOpCode.Lstore_3, "lstore_3", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B184," = new JavaOpCode(JavaOpCodeTag.",Table!B184,", """,Table!A184,""", JavaOperandType.Inline",Table!D184,", JavaFlowControl.",Table!F184,", ",Table!E184,", JavaStackBehavior.",A183,", JavaStackBehavior.",B183,");")</f>
+        <v>Lstore_3 = new JavaOpCode(JavaOpCodeTag.Lstore_3, "lstore_3", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -11252,8 +11249,8 @@
         <v>PushI8</v>
       </c>
       <c r="C184" s="1" t="str">
-        <f>CONCATENATE(Table!B185," = new JavaInstruction(JavaOpCode.",Table!B185,", """,Table!A185,""", JavaOperandType.Inline",Table!D185,", JavaFlowControl.",Table!F185,", ",Table!E185,", JavaStackBehavior.",A184,", JavaStackBehavior.",B184,");")</f>
-        <v>Lsub = new JavaInstruction(JavaOpCode.Lsub, "lsub", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8_PopI8, JavaStackBehavior.PushI8);</v>
+        <f>CONCATENATE(Table!B185," = new JavaOpCode(JavaOpCodeTag.",Table!B185,", """,Table!A185,""", JavaOperandType.Inline",Table!D185,", JavaFlowControl.",Table!F185,", ",Table!E185,", JavaStackBehavior.",A184,", JavaStackBehavior.",B184,");")</f>
+        <v>Lsub = new JavaOpCode(JavaOpCodeTag.Lsub, "lsub", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8_PopI8, JavaStackBehavior.PushI8);</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
@@ -11266,8 +11263,8 @@
         <v>PushI8</v>
       </c>
       <c r="C185" s="1" t="str">
-        <f>CONCATENATE(Table!B186," = new JavaInstruction(JavaOpCode.",Table!B186,", """,Table!A186,""", JavaOperandType.Inline",Table!D186,", JavaFlowControl.",Table!F186,", ",Table!E186,", JavaStackBehavior.",A185,", JavaStackBehavior.",B185,");")</f>
-        <v>Lushr = new JavaInstruction(JavaOpCode.Lushr, "lushr", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8_PopI, JavaStackBehavior.PushI8);</v>
+        <f>CONCATENATE(Table!B186," = new JavaOpCode(JavaOpCodeTag.",Table!B186,", """,Table!A186,""", JavaOperandType.Inline",Table!D186,", JavaFlowControl.",Table!F186,", ",Table!E186,", JavaStackBehavior.",A185,", JavaStackBehavior.",B185,");")</f>
+        <v>Lushr = new JavaOpCode(JavaOpCodeTag.Lushr, "lushr", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8_PopI, JavaStackBehavior.PushI8);</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
@@ -11280,8 +11277,8 @@
         <v>PushI8</v>
       </c>
       <c r="C186" s="1" t="str">
-        <f>CONCATENATE(Table!B187," = new JavaInstruction(JavaOpCode.",Table!B187,", """,Table!A187,""", JavaOperandType.Inline",Table!D187,", JavaFlowControl.",Table!F187,", ",Table!E187,", JavaStackBehavior.",A186,", JavaStackBehavior.",B186,");")</f>
-        <v>Lxor = new JavaInstruction(JavaOpCode.Lxor, "lxor", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8_PopI8, JavaStackBehavior.PushI8);</v>
+        <f>CONCATENATE(Table!B187," = new JavaOpCode(JavaOpCodeTag.",Table!B187,", """,Table!A187,""", JavaOperandType.Inline",Table!D187,", JavaFlowControl.",Table!F187,", ",Table!E187,", JavaStackBehavior.",A186,", JavaStackBehavior.",B186,");")</f>
+        <v>Lxor = new JavaOpCode(JavaOpCodeTag.Lxor, "lxor", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopI8_PopI8, JavaStackBehavior.PushI8);</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
@@ -11294,8 +11291,8 @@
         <v>Push0</v>
       </c>
       <c r="C187" s="1" t="str">
-        <f>CONCATENATE(Table!B188," = new JavaInstruction(JavaOpCode.",Table!B188,", """,Table!A188,""", JavaOperandType.Inline",Table!D188,", JavaFlowControl.",Table!F188,", ",Table!E188,", JavaStackBehavior.",A187,", JavaStackBehavior.",B187,");")</f>
-        <v>Monitorenter = new JavaInstruction(JavaOpCode.Monitorenter, "monitorenter", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B188," = new JavaOpCode(JavaOpCodeTag.",Table!B188,", """,Table!A188,""", JavaOperandType.Inline",Table!D188,", JavaFlowControl.",Table!F188,", ",Table!E188,", JavaStackBehavior.",A187,", JavaStackBehavior.",B187,");")</f>
+        <v>Monitorenter = new JavaOpCode(JavaOpCodeTag.Monitorenter, "monitorenter", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -11308,8 +11305,8 @@
         <v>Push0</v>
       </c>
       <c r="C188" s="1" t="str">
-        <f>CONCATENATE(Table!B189," = new JavaInstruction(JavaOpCode.",Table!B189,", """,Table!A189,""", JavaOperandType.Inline",Table!D189,", JavaFlowControl.",Table!F189,", ",Table!E189,", JavaStackBehavior.",A188,", JavaStackBehavior.",B188,");")</f>
-        <v>Monitorexit = new JavaInstruction(JavaOpCode.Monitorexit, "monitorexit", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B189," = new JavaOpCode(JavaOpCodeTag.",Table!B189,", """,Table!A189,""", JavaOperandType.Inline",Table!D189,", JavaFlowControl.",Table!F189,", ",Table!E189,", JavaStackBehavior.",A188,", JavaStackBehavior.",B188,");")</f>
+        <v>Monitorexit = new JavaOpCode(JavaOpCodeTag.Monitorexit, "monitorexit", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
@@ -11322,8 +11319,8 @@
         <v>PushRef</v>
       </c>
       <c r="C189" s="1" t="str">
-        <f>CONCATENATE(Table!B190," = new JavaInstruction(JavaOpCode.",Table!B190,", """,Table!A190,""", JavaOperandType.Inline",Table!D190,", JavaFlowControl.",Table!F190,", ",Table!E190,", JavaStackBehavior.",A189,", JavaStackBehavior.",B189,");")</f>
-        <v>Multianewarray = new JavaInstruction(JavaOpCode.Multianewarray, "multianewarray", JavaOperandType.InlineType_I1, JavaFlowControl.Next, 4, JavaStackBehavior.PopVar, JavaStackBehavior.PushRef);</v>
+        <f>CONCATENATE(Table!B190," = new JavaOpCode(JavaOpCodeTag.",Table!B190,", """,Table!A190,""", JavaOperandType.Inline",Table!D190,", JavaFlowControl.",Table!F190,", ",Table!E190,", JavaStackBehavior.",A189,", JavaStackBehavior.",B189,");")</f>
+        <v>Multianewarray = new JavaOpCode(JavaOpCodeTag.Multianewarray, "multianewarray", JavaOperandType.InlineType_U1, JavaFlowControl.Next, 4, JavaStackBehavior.PopVar, JavaStackBehavior.PushRef);</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
@@ -11336,8 +11333,8 @@
         <v>PushRef</v>
       </c>
       <c r="C190" s="1" t="str">
-        <f>CONCATENATE(Table!B191," = new JavaInstruction(JavaOpCode.",Table!B191,", """,Table!A191,""", JavaOperandType.Inline",Table!D191,", JavaFlowControl.",Table!F191,", ",Table!E191,", JavaStackBehavior.",A190,", JavaStackBehavior.",B190,");")</f>
-        <v>New = new JavaInstruction(JavaOpCode.New, "new", JavaOperandType.InlineType, JavaFlowControl.Call, 3, JavaStackBehavior.Pop0, JavaStackBehavior.PushRef);</v>
+        <f>CONCATENATE(Table!B191," = new JavaOpCode(JavaOpCodeTag.",Table!B191,", """,Table!A191,""", JavaOperandType.Inline",Table!D191,", JavaFlowControl.",Table!F191,", ",Table!E191,", JavaStackBehavior.",A190,", JavaStackBehavior.",B190,");")</f>
+        <v>New = new JavaOpCode(JavaOpCodeTag.New, "new", JavaOperandType.InlineType, JavaFlowControl.Next, 3, JavaStackBehavior.Pop0, JavaStackBehavior.PushRef);</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
@@ -11350,8 +11347,8 @@
         <v>PushRef</v>
       </c>
       <c r="C191" s="1" t="str">
-        <f>CONCATENATE(Table!B192," = new JavaInstruction(JavaOpCode.",Table!B192,", """,Table!A192,""", JavaOperandType.Inline",Table!D192,", JavaFlowControl.",Table!F192,", ",Table!E192,", JavaStackBehavior.",A191,", JavaStackBehavior.",B191,");")</f>
-        <v>Newarray = new JavaInstruction(JavaOpCode.Newarray, "newarray", JavaOperandType.InlineArrayType, JavaFlowControl.Next, 2, JavaStackBehavior.PopI, JavaStackBehavior.PushRef);</v>
+        <f>CONCATENATE(Table!B192," = new JavaOpCode(JavaOpCodeTag.",Table!B192,", """,Table!A192,""", JavaOperandType.Inline",Table!D192,", JavaFlowControl.",Table!F192,", ",Table!E192,", JavaStackBehavior.",A191,", JavaStackBehavior.",B191,");")</f>
+        <v>Newarray = new JavaOpCode(JavaOpCodeTag.Newarray, "newarray", JavaOperandType.InlineArrayType, JavaFlowControl.Next, 2, JavaStackBehavior.PopI, JavaStackBehavior.PushRef);</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
@@ -11364,8 +11361,8 @@
         <v>Push0</v>
       </c>
       <c r="C192" s="1" t="str">
-        <f>CONCATENATE(Table!B193," = new JavaInstruction(JavaOpCode.",Table!B193,", """,Table!A193,""", JavaOperandType.Inline",Table!D193,", JavaFlowControl.",Table!F193,", ",Table!E193,", JavaStackBehavior.",A192,", JavaStackBehavior.",B192,");")</f>
-        <v>Nop = new JavaInstruction(JavaOpCode.Nop, "nop", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B193," = new JavaOpCode(JavaOpCodeTag.",Table!B193,", """,Table!A193,""", JavaOperandType.Inline",Table!D193,", JavaFlowControl.",Table!F193,", ",Table!E193,", JavaStackBehavior.",A192,", JavaStackBehavior.",B192,");")</f>
+        <v>Nop = new JavaOpCode(JavaOpCodeTag.Nop, "nop", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop0, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
@@ -11378,8 +11375,8 @@
         <v>Push0</v>
       </c>
       <c r="C193" s="1" t="str">
-        <f>CONCATENATE(Table!B194," = new JavaInstruction(JavaOpCode.",Table!B194,", """,Table!A194,""", JavaOperandType.Inline",Table!D194,", JavaFlowControl.",Table!F194,", ",Table!E194,", JavaStackBehavior.",A193,", JavaStackBehavior.",B193,");")</f>
-        <v>Pop = new JavaInstruction(JavaOpCode.Pop, "pop", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop1, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B194," = new JavaOpCode(JavaOpCodeTag.",Table!B194,", """,Table!A194,""", JavaOperandType.Inline",Table!D194,", JavaFlowControl.",Table!F194,", ",Table!E194,", JavaStackBehavior.",A193,", JavaStackBehavior.",B193,");")</f>
+        <v>Pop = new JavaOpCode(JavaOpCodeTag.Pop, "pop", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop1, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
@@ -11392,8 +11389,8 @@
         <v>Push0</v>
       </c>
       <c r="C194" s="1" t="str">
-        <f>CONCATENATE(Table!B195," = new JavaInstruction(JavaOpCode.",Table!B195,", """,Table!A195,""", JavaOperandType.Inline",Table!D195,", JavaFlowControl.",Table!F195,", ",Table!E195,", JavaStackBehavior.",A194,", JavaStackBehavior.",B194,");")</f>
-        <v>Pop2 = new JavaInstruction(JavaOpCode.Pop2, "pop2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop1, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B195," = new JavaOpCode(JavaOpCodeTag.",Table!B195,", """,Table!A195,""", JavaOperandType.Inline",Table!D195,", JavaFlowControl.",Table!F195,", ",Table!E195,", JavaStackBehavior.",A194,", JavaStackBehavior.",B194,");")</f>
+        <v>Pop2 = new JavaOpCode(JavaOpCodeTag.Pop2, "pop2", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop1, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -11406,8 +11403,8 @@
         <v>Push0</v>
       </c>
       <c r="C195" s="1" t="str">
-        <f>CONCATENATE(Table!B196," = new JavaInstruction(JavaOpCode.",Table!B196,", """,Table!A196,""", JavaOperandType.Inline",Table!D196,", JavaFlowControl.",Table!F196,", ",Table!E196,", JavaStackBehavior.",A195,", JavaStackBehavior.",B195,");")</f>
-        <v>Putfield = new JavaInstruction(JavaOpCode.Putfield, "putfield", JavaOperandType.InlineField, JavaFlowControl.Next, 3, JavaStackBehavior.PopRef_Pop1, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B196," = new JavaOpCode(JavaOpCodeTag.",Table!B196,", """,Table!A196,""", JavaOperandType.Inline",Table!D196,", JavaFlowControl.",Table!F196,", ",Table!E196,", JavaStackBehavior.",A195,", JavaStackBehavior.",B195,");")</f>
+        <v>Putfield = new JavaOpCode(JavaOpCodeTag.Putfield, "putfield", JavaOperandType.InlineField, JavaFlowControl.Next, 3, JavaStackBehavior.PopRef_Pop1, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -11420,8 +11417,8 @@
         <v>Push0</v>
       </c>
       <c r="C196" s="1" t="str">
-        <f>CONCATENATE(Table!B197," = new JavaInstruction(JavaOpCode.",Table!B197,", """,Table!A197,""", JavaOperandType.Inline",Table!D197,", JavaFlowControl.",Table!F197,", ",Table!E197,", JavaStackBehavior.",A196,", JavaStackBehavior.",B196,");")</f>
-        <v>Putstatic = new JavaInstruction(JavaOpCode.Putstatic, "putstatic", JavaOperandType.InlineField, JavaFlowControl.Next, 3, JavaStackBehavior.Pop1, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B197," = new JavaOpCode(JavaOpCodeTag.",Table!B197,", """,Table!A197,""", JavaOperandType.Inline",Table!D197,", JavaFlowControl.",Table!F197,", ",Table!E197,", JavaStackBehavior.",A196,", JavaStackBehavior.",B196,");")</f>
+        <v>Putstatic = new JavaOpCode(JavaOpCodeTag.Putstatic, "putstatic", JavaOperandType.InlineField, JavaFlowControl.Next, 3, JavaStackBehavior.Pop1, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -11434,8 +11431,8 @@
         <v>Push0</v>
       </c>
       <c r="C197" s="1" t="str">
-        <f>CONCATENATE(Table!B198," = new JavaInstruction(JavaOpCode.",Table!B198,", """,Table!A198,""", JavaOperandType.Inline",Table!D198,", JavaFlowControl.",Table!F198,", ",Table!E198,", JavaStackBehavior.",A197,", JavaStackBehavior.",B197,");")</f>
-        <v>Ret = new JavaInstruction(JavaOpCode.Ret, "ret", JavaOperandType.InlineVar, JavaFlowControl.Return, 2, JavaStackBehavior.Pop0, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B198," = new JavaOpCode(JavaOpCodeTag.",Table!B198,", """,Table!A198,""", JavaOperandType.Inline",Table!D198,", JavaFlowControl.",Table!F198,", ",Table!E198,", JavaStackBehavior.",A197,", JavaStackBehavior.",B197,");")</f>
+        <v>Ret = new JavaOpCode(JavaOpCodeTag.Ret, "ret", JavaOperandType.InlineVar, JavaFlowControl.Return, 2, JavaStackBehavior.Pop0, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -11448,8 +11445,8 @@
         <v>Push0</v>
       </c>
       <c r="C198" s="1" t="str">
-        <f>CONCATENATE(Table!B199," = new JavaInstruction(JavaOpCode.",Table!B199,", """,Table!A199,""", JavaOperandType.Inline",Table!D199,", JavaFlowControl.",Table!F199,", ",Table!E199,", JavaStackBehavior.",A198,", JavaStackBehavior.",B198,");")</f>
-        <v>Return = new JavaInstruction(JavaOpCode.Return, "return", JavaOperandType.InlineNone, JavaFlowControl.Return, 1, JavaStackBehavior.Pop0, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B199," = new JavaOpCode(JavaOpCodeTag.",Table!B199,", """,Table!A199,""", JavaOperandType.Inline",Table!D199,", JavaFlowControl.",Table!F199,", ",Table!E199,", JavaStackBehavior.",A198,", JavaStackBehavior.",B198,");")</f>
+        <v>Return = new JavaOpCode(JavaOpCodeTag.Return, "return", JavaOperandType.InlineNone, JavaFlowControl.Return, 1, JavaStackBehavior.Pop0, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
@@ -11462,8 +11459,8 @@
         <v>PushI</v>
       </c>
       <c r="C199" s="1" t="str">
-        <f>CONCATENATE(Table!B200," = new JavaInstruction(JavaOpCode.",Table!B200,", """,Table!A200,""", JavaOperandType.Inline",Table!D200,", JavaFlowControl.",Table!F200,", ",Table!E200,", JavaStackBehavior.",A199,", JavaStackBehavior.",B199,");")</f>
-        <v>Saload = new JavaInstruction(JavaOpCode.Saload, "saload", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B200," = new JavaOpCode(JavaOpCodeTag.",Table!B200,", """,Table!A200,""", JavaOperandType.Inline",Table!D200,", JavaFlowControl.",Table!F200,", ",Table!E200,", JavaStackBehavior.",A199,", JavaStackBehavior.",B199,");")</f>
+        <v>Saload = new JavaOpCode(JavaOpCodeTag.Saload, "saload", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
@@ -11476,8 +11473,8 @@
         <v>Push0</v>
       </c>
       <c r="C200" s="1" t="str">
-        <f>CONCATENATE(Table!B201," = new JavaInstruction(JavaOpCode.",Table!B201,", """,Table!A201,""", JavaOperandType.Inline",Table!D201,", JavaFlowControl.",Table!F201,", ",Table!E201,", JavaStackBehavior.",A200,", JavaStackBehavior.",B200,");")</f>
-        <v>Sastore = new JavaInstruction(JavaOpCode.Sastore, "sastore", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI_PopI, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B201," = new JavaOpCode(JavaOpCodeTag.",Table!B201,", """,Table!A201,""", JavaOperandType.Inline",Table!D201,", JavaFlowControl.",Table!F201,", ",Table!E201,", JavaStackBehavior.",A200,", JavaStackBehavior.",B200,");")</f>
+        <v>Sastore = new JavaOpCode(JavaOpCodeTag.Sastore, "sastore", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.PopRef_PopI_PopI, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
@@ -11490,8 +11487,8 @@
         <v>PushI</v>
       </c>
       <c r="C201" s="1" t="str">
-        <f>CONCATENATE(Table!B202," = new JavaInstruction(JavaOpCode.",Table!B202,", """,Table!A202,""", JavaOperandType.Inline",Table!D202,", JavaFlowControl.",Table!F202,", ",Table!E202,", JavaStackBehavior.",A201,", JavaStackBehavior.",B201,");")</f>
-        <v>Sipush = new JavaInstruction(JavaOpCode.Sipush, "sipush", JavaOperandType.InlineI2, JavaFlowControl.Next, 3, JavaStackBehavior.Pop0, JavaStackBehavior.PushI);</v>
+        <f>CONCATENATE(Table!B202," = new JavaOpCode(JavaOpCodeTag.",Table!B202,", """,Table!A202,""", JavaOperandType.Inline",Table!D202,", JavaFlowControl.",Table!F202,", ",Table!E202,", JavaStackBehavior.",A201,", JavaStackBehavior.",B201,");")</f>
+        <v>Sipush = new JavaOpCode(JavaOpCodeTag.Sipush, "sipush", JavaOperandType.InlineI2, JavaFlowControl.Next, 3, JavaStackBehavior.Pop0, JavaStackBehavior.PushI);</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
@@ -11504,8 +11501,8 @@
         <v>Push1</v>
       </c>
       <c r="C202" s="1" t="str">
-        <f>CONCATENATE(Table!B203," = new JavaInstruction(JavaOpCode.",Table!B203,", """,Table!A203,""", JavaOperandType.Inline",Table!D203,", JavaFlowControl.",Table!F203,", ",Table!E203,", JavaStackBehavior.",A202,", JavaStackBehavior.",B202,");")</f>
-        <v>Swap = new JavaInstruction(JavaOpCode.Swap, "swap", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop1_Pop1, JavaStackBehavior.Push1);</v>
+        <f>CONCATENATE(Table!B203," = new JavaOpCode(JavaOpCodeTag.",Table!B203,", """,Table!A203,""", JavaOperandType.Inline",Table!D203,", JavaFlowControl.",Table!F203,", ",Table!E203,", JavaStackBehavior.",A202,", JavaStackBehavior.",B202,");")</f>
+        <v>Swap = new JavaOpCode(JavaOpCodeTag.Swap, "swap", JavaOperandType.InlineNone, JavaFlowControl.Next, 1, JavaStackBehavior.Pop1_Pop1, JavaStackBehavior.Push1);</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
@@ -11518,8 +11515,8 @@
         <v>Push0</v>
       </c>
       <c r="C203" s="1" t="str">
-        <f>CONCATENATE(Table!B204," = new JavaInstruction(JavaOpCode.",Table!B204,", """,Table!A204,""", JavaOperandType.Inline",Table!D204,", JavaFlowControl.",Table!F204,", ",Table!E204,", JavaStackBehavior.",A203,", JavaStackBehavior.",B203,");")</f>
-        <v>Tableswitch = new JavaInstruction(JavaOpCode.Tableswitch, "tableswitch", JavaOperandType.InlineTableSwitch, JavaFlowControl.Next, 0, JavaStackBehavior.PopI, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B204," = new JavaOpCode(JavaOpCodeTag.",Table!B204,", """,Table!A204,""", JavaOperandType.Inline",Table!D204,", JavaFlowControl.",Table!F204,", ",Table!E204,", JavaStackBehavior.",A203,", JavaStackBehavior.",B203,");")</f>
+        <v>Tableswitch = new JavaOpCode(JavaOpCodeTag.Tableswitch, "tableswitch", JavaOperandType.InlineTableSwitch, JavaFlowControl.ConditionalBranch, 0, JavaStackBehavior.PopI, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
@@ -11532,8 +11529,8 @@
         <v>Push0</v>
       </c>
       <c r="C204" s="1" t="str">
-        <f>CONCATENATE(Table!B205," = new JavaInstruction(JavaOpCode.",Table!B205,", """,Table!A205,""", JavaOperandType.Inline",Table!D205,", JavaFlowControl.",Table!F205,", ",Table!E205,", JavaStackBehavior.",A204,", JavaStackBehavior.",B204,");")</f>
-        <v>Wide = new JavaInstruction(JavaOpCode.Wide, "wide", JavaOperandType.InlineNone, JavaFlowControl.Meta, 0, JavaStackBehavior.Pop0, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B205," = new JavaOpCode(JavaOpCodeTag.",Table!B205,", """,Table!A205,""", JavaOperandType.Inline",Table!D205,", JavaFlowControl.",Table!F205,", ",Table!E205,", JavaStackBehavior.",A204,", JavaStackBehavior.",B204,");")</f>
+        <v>Wide = new JavaOpCode(JavaOpCodeTag.Wide, "wide", JavaOperandType.InlineNone, JavaFlowControl.Meta, 0, JavaStackBehavior.Pop0, JavaStackBehavior.Push0);</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
@@ -11546,8 +11543,8 @@
         <v>Push0</v>
       </c>
       <c r="C205" s="1" t="str">
-        <f>CONCATENATE(Table!B206," = new JavaInstruction(JavaOpCode.",Table!B206,", """,Table!A206,""", JavaOperandType.Inline",Table!D206,", JavaFlowControl.",Table!F206,", ",Table!E206,", JavaStackBehavior.",A205,", JavaStackBehavior.",B205,");")</f>
-        <v>Xxxunusedxxx1 = new JavaInstruction(JavaOpCode.Xxxunusedxxx1, "xxxunusedxxx1", JavaOperandType.InlineNone, JavaFlowControl.Special, 1, JavaStackBehavior.Pop0, JavaStackBehavior.Push0);</v>
+        <f>CONCATENATE(Table!B206," = new JavaOpCode(JavaOpCodeTag.",Table!B206,", """,Table!A206,""", JavaOperandType.Inline",Table!D206,", JavaFlowControl.",Table!F206,", ",Table!E206,", JavaStackBehavior.",A205,", JavaStackBehavior.",B205,");")</f>
+        <v>Xxxunusedxxx1 = new JavaOpCode(JavaOpCodeTag.Xxxunusedxxx1, "xxxunusedxxx1", JavaOperandType.InlineNone, JavaFlowControl.Special, 1, JavaStackBehavior.Pop0, JavaStackBehavior.Push0);</v>
       </c>
     </row>
   </sheetData>
@@ -11559,11 +11556,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A205"/>
   <sheetViews>
-    <sheetView topLeftCell="A195" workbookViewId="0">
-      <selection sqref="A1:A205"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
@@ -12804,11 +12802,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A205"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A205"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">

</xml_diff>